<commit_message>
Recorded and added some music, actually added pygame display which is WIP
</commit_message>
<xml_diff>
--- a/Dev/EBTA Developent Roadmap.xlsx
+++ b/Dev/EBTA Developent Roadmap.xlsx
@@ -338,9 +338,6 @@
     <t>9 -</t>
   </si>
   <si>
-    <t>12 -</t>
-  </si>
-  <si>
     <t>13 -</t>
   </si>
   <si>
@@ -726,6 +723,9 @@
   </si>
   <si>
     <t>11 - 60 Added almost all features to list</t>
+  </si>
+  <si>
+    <t>12 - 45 Recorded Erik+Brian Music, added music to game, worked on pygame display while reading documentation.</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1101,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1176,7 @@
         <v>45</v>
       </c>
       <c r="J9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1184,91 +1184,91 @@
         <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C10" t="s">
+        <v>230</v>
+      </c>
+      <c r="D10" t="s">
         <v>231</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>102</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>103</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>104</v>
-      </c>
-      <c r="G10" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" t="s">
         <v>106</v>
       </c>
-      <c r="B11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>107</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>108</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>109</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>110</v>
-      </c>
-      <c r="G11" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" t="s">
         <v>112</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>113</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>114</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>115</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>116</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>117</v>
-      </c>
-      <c r="G12" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" t="s">
         <v>121</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>122</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>123</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>124</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>125</v>
-      </c>
-      <c r="G13" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2089,7 +2089,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -2142,7 +2142,7 @@
         <v>82</v>
       </c>
       <c r="F5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>87</v>
@@ -2186,7 +2186,7 @@
         <v>89</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H6" t="s">
         <v>90</v>
@@ -2218,25 +2218,25 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" t="s">
         <v>128</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I7" t="s">
         <v>130</v>
-      </c>
-      <c r="H7" t="s">
-        <v>132</v>
-      </c>
-      <c r="I7" t="s">
-        <v>131</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>13</v>
@@ -2265,19 +2265,19 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="F8" t="s">
-        <v>138</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="H8" t="s">
         <v>135</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>136</v>
-      </c>
-      <c r="I8" t="s">
-        <v>137</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>14</v>
@@ -2306,19 +2306,19 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" t="s">
         <v>139</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="H9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I9" t="s">
         <v>140</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>178</v>
-      </c>
-      <c r="H9" t="s">
-        <v>142</v>
-      </c>
-      <c r="I9" t="s">
-        <v>141</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>17</v>
@@ -2344,22 +2344,22 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F10" t="s">
         <v>143</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="H10" t="s">
         <v>144</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>145</v>
-      </c>
-      <c r="I10" t="s">
-        <v>146</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>15</v>
@@ -2385,25 +2385,25 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E11" t="s">
         <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I11" t="s">
         <v>151</v>
-      </c>
-      <c r="I11" t="s">
-        <v>152</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>11</v>
@@ -2417,25 +2417,25 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F12" t="s">
+        <v>166</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="H12" t="s">
+        <v>159</v>
+      </c>
+      <c r="I12" t="s">
         <v>167</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="H12" t="s">
-        <v>160</v>
-      </c>
-      <c r="I12" t="s">
-        <v>168</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>79</v>
@@ -2452,25 +2452,25 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
+        <v>162</v>
+      </c>
+      <c r="D13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E13" t="s">
+        <v>161</v>
+      </c>
+      <c r="F13" t="s">
+        <v>164</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="H13" t="s">
         <v>163</v>
       </c>
-      <c r="D13" t="s">
-        <v>156</v>
-      </c>
-      <c r="E13" t="s">
-        <v>162</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="I13" t="s">
         <v>165</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="H13" t="s">
-        <v>164</v>
-      </c>
-      <c r="I13" t="s">
-        <v>166</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>17</v>
@@ -2487,17 +2487,17 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" t="s">
+        <v>169</v>
+      </c>
+      <c r="I14" t="s">
         <v>170</v>
-      </c>
-      <c r="I14" t="s">
-        <v>171</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>14</v>
@@ -2511,22 +2511,22 @@
         <v>15</v>
       </c>
       <c r="D15" t="s">
+        <v>174</v>
+      </c>
+      <c r="E15" t="s">
+        <v>173</v>
+      </c>
+      <c r="F15" t="s">
         <v>175</v>
       </c>
-      <c r="E15" t="s">
-        <v>174</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="G15" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>177</v>
-      </c>
       <c r="H15" t="s">
+        <v>183</v>
+      </c>
+      <c r="I15" t="s">
         <v>184</v>
-      </c>
-      <c r="I15" t="s">
-        <v>185</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>15</v>
@@ -2540,22 +2540,22 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E16" t="s">
+        <v>178</v>
+      </c>
+      <c r="F16" t="s">
         <v>179</v>
       </c>
-      <c r="F16" t="s">
-        <v>180</v>
-      </c>
       <c r="G16" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2566,25 +2566,25 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F17" t="s">
+        <v>185</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="H17" t="s">
         <v>186</v>
       </c>
-      <c r="G17" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="H17" t="s">
-        <v>187</v>
-      </c>
       <c r="I17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2595,25 +2595,25 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D18">
         <v>10</v>
       </c>
       <c r="E18" t="s">
+        <v>188</v>
+      </c>
+      <c r="F18" t="s">
         <v>189</v>
       </c>
-      <c r="F18" t="s">
-        <v>190</v>
-      </c>
       <c r="G18" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2624,25 +2624,25 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D19">
         <v>6</v>
       </c>
       <c r="E19" t="s">
+        <v>192</v>
+      </c>
+      <c r="F19" t="s">
+        <v>194</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="H19" t="s">
         <v>193</v>
       </c>
-      <c r="F19" t="s">
-        <v>195</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="H19" t="s">
-        <v>194</v>
-      </c>
       <c r="I19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2656,19 +2656,19 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
+        <v>196</v>
+      </c>
+      <c r="F20" t="s">
         <v>197</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="H20" t="s">
         <v>198</v>
       </c>
-      <c r="G20" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>199</v>
-      </c>
-      <c r="I20" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2679,22 +2679,22 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E21" t="s">
+        <v>204</v>
+      </c>
+      <c r="F21" t="s">
         <v>205</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="H21" t="s">
         <v>207</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>208</v>
-      </c>
-      <c r="I21" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2708,19 +2708,19 @@
         <v>15</v>
       </c>
       <c r="E22" t="s">
+        <v>209</v>
+      </c>
+      <c r="F22" t="s">
         <v>210</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="H22" t="s">
         <v>211</v>
       </c>
-      <c r="G22" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>212</v>
-      </c>
-      <c r="I22" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2734,19 +2734,19 @@
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F23" t="s">
+        <v>215</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="H23" t="s">
         <v>216</v>
       </c>
-      <c r="G23" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>217</v>
-      </c>
-      <c r="I23" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2757,22 +2757,22 @@
         <v>15</v>
       </c>
       <c r="D24" t="s">
+        <v>221</v>
+      </c>
+      <c r="E24" t="s">
+        <v>218</v>
+      </c>
+      <c r="F24" t="s">
         <v>222</v>
       </c>
-      <c r="E24" t="s">
+      <c r="G24" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="H24" t="s">
+        <v>220</v>
+      </c>
+      <c r="I24" t="s">
         <v>219</v>
-      </c>
-      <c r="F24" t="s">
-        <v>223</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="H24" t="s">
-        <v>221</v>
-      </c>
-      <c r="I24" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2787,19 +2787,19 @@
         <v>4</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F25" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="H25" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="G25" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>227</v>
-      </c>
       <c r="I25" s="11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2813,19 +2813,19 @@
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F26" t="s">
+        <v>227</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="H26" t="s">
+        <v>229</v>
+      </c>
+      <c r="I26" t="s">
         <v>228</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="H26" t="s">
-        <v>230</v>
-      </c>
-      <c r="I26" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2953,7 +2953,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
going throug todo lists
</commit_message>
<xml_diff>
--- a/Dev/EBTA Developent Roadmap.xlsx
+++ b/Dev/EBTA Developent Roadmap.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="239">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -338,9 +338,6 @@
     <t>9 -</t>
   </si>
   <si>
-    <t>13 -</t>
-  </si>
-  <si>
     <t>14 -</t>
   </si>
   <si>
@@ -461,9 +458,6 @@
     <t>Experience Levels + Mobs</t>
   </si>
   <si>
-    <t>Adding an experience level to the game and mobs that respawn so you feel like you're progressing. Probably buffs stats and helps you beat higher level people/things.</t>
-  </si>
-  <si>
     <t>More RPG style and feel like you're progressing</t>
   </si>
   <si>
@@ -536,18 +530,12 @@
     <t>Mobile gamers, anynonwindows/don't want to download. Basically any loose gamer. Also compeditive side online</t>
   </si>
   <si>
-    <t>Fast Addressing</t>
-  </si>
-  <si>
     <t>Well thought out, easier to player and higher skill cap</t>
   </si>
   <si>
     <t>Speedrunners, first time players, etc</t>
   </si>
   <si>
-    <t>Make keywords shorter, have list of items to choose from quickly, maybe accept short names? Maybe take cardinal coords.</t>
-  </si>
-  <si>
     <t>Mins total worked on</t>
   </si>
   <si>
@@ -726,6 +714,39 @@
   </si>
   <si>
     <t>12 - 45 Recorded Erik+Brian Music, added music to game, worked on pygame display while reading documentation.</t>
+  </si>
+  <si>
+    <t>Item and Mechanic Balance</t>
+  </si>
+  <si>
+    <t>Combat Update</t>
+  </si>
+  <si>
+    <t>Attack and defense, speed doesn't do anything. Would need to be be after combat update. Possibly have star/some sort of indicator for bosses</t>
+  </si>
+  <si>
+    <t>Name Manipulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do more with name including character address you by name and work with names including name infulence. </t>
+  </si>
+  <si>
+    <t>Difficulties</t>
+  </si>
+  <si>
+    <t>Easy, Medium, Hard, Ironman verson where can't heal/carry more than you can.</t>
+  </si>
+  <si>
+    <t>Text Parsing/Input (fast Addressing)</t>
+  </si>
+  <si>
+    <t>Make keywords shorter, have list of items to choose from quickly, maybe accept short names? Maybe take cardinal coords. More things rather than equip.</t>
+  </si>
+  <si>
+    <t>Adding an experience level to the game and mobs that respawn so you feel like you're progressing. Probably buffs stats and helps you beat higher level people/things. Also the respawn with golden gauntlet thanos for Paul the buss driver.</t>
+  </si>
+  <si>
+    <t>13 - ✔ Started going through old TODO lists.</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1122,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,7 +1197,7 @@
         <v>45</v>
       </c>
       <c r="J9" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1184,91 +1205,91 @@
         <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C10" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D10" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F10" t="s">
         <v>102</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>103</v>
-      </c>
-      <c r="G10" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" t="s">
         <v>105</v>
       </c>
-      <c r="B11" t="s">
-        <v>119</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>106</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>107</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>108</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>109</v>
-      </c>
-      <c r="G11" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
         <v>111</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>112</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>113</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>114</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>115</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>116</v>
-      </c>
-      <c r="G12" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" t="s">
         <v>120</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>121</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>122</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>123</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>124</v>
-      </c>
-      <c r="G13" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2064,7 +2085,7 @@
   <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2089,7 +2110,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -2142,7 +2163,7 @@
         <v>82</v>
       </c>
       <c r="F5" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>87</v>
@@ -2186,7 +2207,7 @@
         <v>89</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H6" t="s">
         <v>90</v>
@@ -2218,25 +2239,25 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F7" t="s">
         <v>127</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" t="s">
+        <v>130</v>
+      </c>
+      <c r="I7" t="s">
         <v>129</v>
-      </c>
-      <c r="H7" t="s">
-        <v>131</v>
-      </c>
-      <c r="I7" t="s">
-        <v>130</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>13</v>
@@ -2265,19 +2286,19 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="F8" t="s">
-        <v>137</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="H8" t="s">
         <v>134</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>135</v>
-      </c>
-      <c r="I8" t="s">
-        <v>136</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>14</v>
@@ -2306,19 +2327,19 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" t="s">
         <v>138</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="H9" t="s">
+        <v>140</v>
+      </c>
+      <c r="I9" t="s">
         <v>139</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="H9" t="s">
-        <v>141</v>
-      </c>
-      <c r="I9" t="s">
-        <v>140</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>17</v>
@@ -2344,22 +2365,22 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" t="s">
+        <v>237</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="H10" t="s">
         <v>142</v>
       </c>
-      <c r="F10" t="s">
+      <c r="I10" t="s">
         <v>143</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="H10" t="s">
-        <v>144</v>
-      </c>
-      <c r="I10" t="s">
-        <v>145</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>15</v>
@@ -2385,25 +2406,25 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E11" t="s">
         <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>11</v>
@@ -2417,25 +2438,25 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" t="s">
+        <v>152</v>
+      </c>
+      <c r="F12" t="s">
+        <v>164</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="D12" t="s">
-        <v>155</v>
-      </c>
-      <c r="E12" t="s">
-        <v>154</v>
-      </c>
-      <c r="F12" t="s">
-        <v>166</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>158</v>
-      </c>
       <c r="H12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>79</v>
@@ -2452,25 +2473,25 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" t="s">
+        <v>159</v>
+      </c>
+      <c r="F13" t="s">
         <v>162</v>
       </c>
-      <c r="D13" t="s">
-        <v>155</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="G13" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="H13" t="s">
         <v>161</v>
       </c>
-      <c r="F13" t="s">
-        <v>164</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>163</v>
-      </c>
-      <c r="I13" t="s">
-        <v>165</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>17</v>
@@ -2487,17 +2508,17 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>168</v>
+        <v>235</v>
       </c>
       <c r="F14" t="s">
-        <v>171</v>
+        <v>236</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="I14" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>14</v>
@@ -2511,22 +2532,22 @@
         <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E15" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F15" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H15" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="I15" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>15</v>
@@ -2540,22 +2561,22 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E16" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H16" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="I16" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2566,25 +2587,25 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" t="s">
+        <v>177</v>
+      </c>
+      <c r="F17" t="s">
         <v>181</v>
       </c>
-      <c r="F17" t="s">
-        <v>185</v>
-      </c>
       <c r="G17" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H17" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="I17" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2595,25 +2616,25 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D18">
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F18" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H18" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I18" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2624,25 +2645,25 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D19">
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F19" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H19" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="I19" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2656,19 +2677,19 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F20" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H20" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="I20" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2679,22 +2700,22 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E21" t="s">
+        <v>200</v>
+      </c>
+      <c r="F21" t="s">
+        <v>201</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="H21" t="s">
+        <v>203</v>
+      </c>
+      <c r="I21" t="s">
         <v>204</v>
-      </c>
-      <c r="F21" t="s">
-        <v>205</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>206</v>
-      </c>
-      <c r="H21" t="s">
-        <v>207</v>
-      </c>
-      <c r="I21" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2708,19 +2729,19 @@
         <v>15</v>
       </c>
       <c r="E22" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F22" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H22" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="I22" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2734,19 +2755,19 @@
         <v>8</v>
       </c>
       <c r="E23" t="s">
+        <v>209</v>
+      </c>
+      <c r="F23" t="s">
+        <v>211</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="H23" t="s">
+        <v>212</v>
+      </c>
+      <c r="I23" t="s">
         <v>213</v>
-      </c>
-      <c r="F23" t="s">
-        <v>215</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="H23" t="s">
-        <v>216</v>
-      </c>
-      <c r="I23" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2757,22 +2778,22 @@
         <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E24" t="s">
+        <v>214</v>
+      </c>
+      <c r="F24" t="s">
         <v>218</v>
       </c>
-      <c r="F24" t="s">
-        <v>222</v>
-      </c>
       <c r="G24" s="10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H24" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="I24" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2787,19 +2808,19 @@
         <v>4</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2813,19 +2834,19 @@
         <v>4</v>
       </c>
       <c r="E26" t="s">
+        <v>220</v>
+      </c>
+      <c r="F26" t="s">
+        <v>223</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="H26" t="s">
+        <v>225</v>
+      </c>
+      <c r="I26" t="s">
         <v>224</v>
-      </c>
-      <c r="F26" t="s">
-        <v>227</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="H26" t="s">
-        <v>229</v>
-      </c>
-      <c r="I26" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2880,6 +2901,15 @@
       <c r="B32" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C32" t="s">
+        <v>229</v>
+      </c>
+      <c r="E32" t="s">
+        <v>228</v>
+      </c>
+      <c r="F32" t="s">
+        <v>230</v>
+      </c>
       <c r="G32" s="10"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2889,6 +2919,12 @@
       <c r="B33" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E33" t="s">
+        <v>231</v>
+      </c>
+      <c r="F33" t="s">
+        <v>232</v>
+      </c>
       <c r="G33" s="10"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2897,6 +2933,12 @@
       </c>
       <c r="B34" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>233</v>
+      </c>
+      <c r="F34" t="s">
+        <v>234</v>
       </c>
       <c r="G34" s="10"/>
     </row>
@@ -2953,7 +2995,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D47" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed sound effects added last feature list ideas
</commit_message>
<xml_diff>
--- a/Dev/EBTA Developent Roadmap.xlsx
+++ b/Dev/EBTA Developent Roadmap.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="298">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -299,9 +299,6 @@
     <t>All Future, Online, Getting Devs, Multiplayer</t>
   </si>
   <si>
-    <t>Make PAP unlock when you get to end of game</t>
-  </si>
-  <si>
     <t>Lots of content, adds reward for finding everything</t>
   </si>
   <si>
@@ -338,12 +335,6 @@
     <t>9 -</t>
   </si>
   <si>
-    <t>14 -</t>
-  </si>
-  <si>
-    <t>15 -</t>
-  </si>
-  <si>
     <t>16 -</t>
   </si>
   <si>
@@ -413,9 +404,6 @@
     <t>Interriors Implement</t>
   </si>
   <si>
-    <t>Make a basic interrior of bsb and fully test</t>
-  </si>
-  <si>
     <t>0.30</t>
   </si>
   <si>
@@ -440,15 +428,9 @@
     <t>Our friends lol</t>
   </si>
   <si>
-    <t>Adding your dad, Alex Jones, Arnold, Jesse Ventura, auto turrets etc</t>
-  </si>
-  <si>
     <t>Bio Cards</t>
   </si>
   <si>
-    <t>Adding explinations to all jokes and inside things to keep game relavent. Not sure if this would take away from game OR if you would only play the year you have it. Idk</t>
-  </si>
-  <si>
     <t>Future Eng Phys people</t>
   </si>
   <si>
@@ -464,9 +446,6 @@
     <t>RPGs, grindy people etc</t>
   </si>
   <si>
-    <t>Adding map and all suplementary info to the GUI (maybe whole game?) so we can customize content. IDK. I like idea of two window system with map, player icon, pictures, etc on side.</t>
-  </si>
-  <si>
     <t>BD, 10?</t>
   </si>
   <si>
@@ -545,9 +524,6 @@
     <t xml:space="preserve">BD, 25? </t>
   </si>
   <si>
-    <t>Make combat more turn based with actions, reactions, preps, combos, etc. Maybe some skill involved?</t>
-  </si>
-  <si>
     <t>0.32?</t>
   </si>
   <si>
@@ -557,9 +533,6 @@
     <t>2019 Kipling Update</t>
   </si>
   <si>
-    <t>Year selector, tutorial, intro, Map/characters, storyline/quests. This is a substantial piece of work</t>
-  </si>
-  <si>
     <t>BD, 4+10+8+15+20?</t>
   </si>
   <si>
@@ -587,9 +560,6 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Adding time to game. Maybe watch system, time based events, time based characters/moving, etc</t>
-  </si>
-  <si>
     <t>2019 Storyline, weather, night mode</t>
   </si>
   <si>
@@ -611,9 +581,6 @@
     <t>Auto Descriptions</t>
   </si>
   <si>
-    <t>Making so surroundings of obveous areas print out</t>
-  </si>
-  <si>
     <t>Less bugs, more consistency</t>
   </si>
   <si>
@@ -635,9 +602,6 @@
     <t>Creative mode</t>
   </si>
   <si>
-    <t>Can add content to game and make their own quests/stories</t>
-  </si>
-  <si>
     <t>0.34?</t>
   </si>
   <si>
@@ -650,9 +614,6 @@
     <t>Better Map/Quest Navigation</t>
   </si>
   <si>
-    <t>Map display better, quest tracker, can give hints on where to go/where things are</t>
-  </si>
-  <si>
     <t>Beginer friendly game</t>
   </si>
   <si>
@@ -662,12 +623,6 @@
     <t>Minigames</t>
   </si>
   <si>
-    <t>Classes, object methods, how map works, commenting code. Updating to python 3. Interactables class.</t>
-  </si>
-  <si>
-    <t>Mini-gamers around area. Not made by me but implemented.</t>
-  </si>
-  <si>
     <t>Immersive and fun</t>
   </si>
   <si>
@@ -722,9 +677,6 @@
     <t>Combat Update</t>
   </si>
   <si>
-    <t>Attack and defense, speed doesn't do anything. Would need to be be after combat update. Possibly have star/some sort of indicator for bosses</t>
-  </si>
-  <si>
     <t>Name Manipulation</t>
   </si>
   <si>
@@ -734,26 +686,315 @@
     <t>Difficulties</t>
   </si>
   <si>
-    <t>Easy, Medium, Hard, Ironman verson where can't heal/carry more than you can.</t>
-  </si>
-  <si>
-    <t>Text Parsing/Input (fast Addressing)</t>
-  </si>
-  <si>
-    <t>Make keywords shorter, have list of items to choose from quickly, maybe accept short names? Maybe take cardinal coords. More things rather than equip.</t>
-  </si>
-  <si>
-    <t>Adding an experience level to the game and mobs that respawn so you feel like you're progressing. Probably buffs stats and helps you beat higher level people/things. Also the respawn with golden gauntlet thanos for Paul the buss driver.</t>
-  </si>
-  <si>
     <t>13 - ✔ Started going through old TODO lists.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flying, Electricity, </t>
+  </si>
+  <si>
+    <t>Rebalance mechanics so that Speed plays more of an effect.</t>
+  </si>
+  <si>
+    <t>Right now defense is v important but with healing items added this should fix it</t>
+  </si>
+  <si>
+    <t>Better head items plz</t>
+  </si>
+  <si>
+    <t>Need to know that Jana has the textbook, maybe the story should say that somewhere</t>
+  </si>
+  <si>
+    <t>Not obveous that equip means to pick up</t>
+  </si>
+  <si>
+    <t>When you inspect the car it says 'Ya thought these were the keys"</t>
+  </si>
+  <si>
+    <t>When you searching when nothings there "You double take and there's still nothing there"</t>
+  </si>
+  <si>
+    <t>If you search 20 times you die</t>
+  </si>
+  <si>
+    <t>After giving dirty needle to sharp exchange a random encounter with a person that says "You're the greatest semaritan in the world" and gives you and Uzi</t>
+  </si>
+  <si>
+    <t>Phil says that need to be pushed more toward the Phenoix</t>
+  </si>
+  <si>
+    <t>Notes option (a list of all lore you've gone through)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding map and all suplementary info to the GUI (maybe whole game?) so we can customize content. IDK. I like idea of two window system with map, player icon, pictures, etc on side. </t>
+  </si>
+  <si>
+    <t>Input (fast Addressing)</t>
+  </si>
+  <si>
+    <t>Make keywords shorter, have list of items to choose from quickly, maybe accept short names? Maybe take cardinal coords. More things rather than equip. Also possibly controller support?</t>
+  </si>
+  <si>
+    <t>Adding time to game. Maybe watch system, time based events, time based characters/moving, etc. Either BOTW 2 min for 1 hr with longest day, or minecraft. I don't think ever step 5 minutes. Starting day is 12pm, day of Kipling (for 2017-2018 version).</t>
+  </si>
+  <si>
+    <t>Collectables and Trophies</t>
+  </si>
+  <si>
+    <t>Make a basic interrior of bsb and fully test.</t>
+  </si>
+  <si>
+    <t>NPCs</t>
+  </si>
+  <si>
+    <t>They move around, have  a companion, can equip items to yourself to store for later games so they act as a companion.</t>
+  </si>
+  <si>
+    <t>Making so surroundings of obveous areas print out. Have lore print first and then title+search around you.</t>
+  </si>
+  <si>
+    <t>Teliporter</t>
+  </si>
+  <si>
+    <t>Sling ring, teliport anywhere you know. Portal gun, teliport anywhere you can see. Instant transmission (anything). Zombies teliporter (where another one is but also in time). Star Trek teliport (anywhere but only to/from consol).</t>
+  </si>
+  <si>
+    <t>Desctruction</t>
+  </si>
+  <si>
+    <t>Building and all things are breakable/fightable/destroyable.</t>
+  </si>
+  <si>
+    <t>GTA Police</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Star level where police come after you, eventually SWAT, eventually have to escape on rocket in smoke stack to go meet Elon musk on the moon. </t>
+  </si>
+  <si>
+    <t>Can add content to game and make their own quests/stories. 
+Maybe unlocks when you beat the game.</t>
+  </si>
+  <si>
+    <t>Attack and defense, speed doesn't do anything. Would need to be be after combat update. Possibly have star/some sort of indicator for bosses.
+More direct reward for exploration with something that ties back into game.</t>
+  </si>
+  <si>
+    <t>Text Display</t>
+  </si>
+  <si>
+    <t>GUI text printer, change colour, font, style of words to highlight.</t>
+  </si>
+  <si>
+    <t>Move map to right side.
+Map display better, quest tracker, can give hints on where to go/where things are
+Ingame journal or notes function.</t>
+  </si>
+  <si>
+    <t>Keep track of all items/things collected</t>
+  </si>
+  <si>
+    <t>(more use of storyline, music, definition to people to give realism to the world)</t>
+  </si>
+  <si>
+    <t>Some sort of skill component to fighting</t>
+  </si>
+  <si>
+    <t>Scater Erik Update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">. You see a campus police guard pull up to talk to someone on the skateboard.
+"Erik the Sk8r: Hey Bill"
+"Bill the Mac Cop: Hey Erik, you know you can't be here right?"
+"Bill: Comomon man we do this every day"
+"Erik: Okay then, see you tomorrow!"
+He scates off quickly up 
+"Bill the Mac Cop: You can't skate on campus prop... aww whatever."
+Involves lore from the skate video
+</t>
+  </si>
+  <si>
+    <t>Belzabad plays when you fight kleiman</t>
+  </si>
+  <si>
+    <t>Undead/Errie Update</t>
+  </si>
+  <si>
+    <t>Expand on the Story and the high council so they can piece everything together</t>
+  </si>
+  <si>
+    <t>Put item descriptions to have items help tell the story</t>
+  </si>
+  <si>
+    <t>Fix all text problems or make more auto text mechanics to improve playability</t>
+  </si>
+  <si>
+    <t>Hollywood Expansion</t>
+  </si>
+  <si>
+    <t>Hollywood Murder Mystery</t>
+  </si>
+  <si>
+    <t>Philpocalpyse storyline</t>
+  </si>
+  <si>
+    <t>The Areana</t>
+  </si>
+  <si>
+    <t>Green Lake</t>
+  </si>
+  <si>
+    <t>Tyler wants it to be Sandbox mode, no linear stuff, events unfold from there</t>
+  </si>
+  <si>
+    <t>Adding an experience level to the game and mobs that respawn so you feel like you're progressing. Probably buffs stats and helps you beat higher level people/things. Also the respawn with golden gauntlet thanos for Paul the buss driver.
+In general, have more crazy/dangerous things happen as you progress in quests/storyline (sand worms pop up, idk, crazyness)
+Could have random drop loot</t>
+  </si>
+  <si>
+    <t>Including Iron man suit with Energy, craftables and consumables with energy. Secret weird flying place/base. Secret places you can only get to by flying into upper buildings
+You can fly up too far and fly out of the game</t>
+  </si>
+  <si>
+    <t>Easy, Medium, Hard, Ironman verson where can't heal/carry more than you can. Maybe all with different endings.
+Easy-medium-Hardcore modes where you have 1. map w. quest outline (maybe a box?) - exploitable map/looking - no map  2. Enemy difficulty 3. Item outlines? 4. No eating 5. Full inventory vs expandable vs just you?</t>
+  </si>
+  <si>
+    <t>Have Brendan Fallon character with eclipse mug, rocketry t-shirt, Strainer on head?SafetyGlasses?, and iron ring</t>
+  </si>
+  <si>
+    <t>Social Media and Website</t>
+  </si>
+  <si>
+    <t>1st year Storyline and Arts/quad Expansion</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Need story arc for body armour</t>
+  </si>
+  <si>
+    <t>AR version of the game -Ekamada</t>
+  </si>
+  <si>
+    <t>Mini-gamers around area. Not made by me but implemented. Including pong, chess (Mitch), tetris (Zac), Zork, and watching Ascii new hope, Classic riddles/storries (goat, chicken, fox)
+Liars Dice
+ Tyler and Angus in full pirate gear, Hani is part of the wall (part of the ship part of the crew (the Die is cast and Davy Jones is there as well )</t>
+  </si>
+  <si>
+    <t>People drop money/you can make money
+Petter is a seller and you can buy Marvin the Martian thing
+Can drop a little bit from cops but not too much to farm</t>
+  </si>
+  <si>
+    <t>Easier way to access game, not just goo.gl/iK8dL9 (Website)</t>
+  </si>
+  <si>
+    <t>Tutorial</t>
+  </si>
+  <si>
+    <t>Start player in secluded area/small island to get a sense but still have tutorial
+First 5 minutes set tone of the game, set expectations and colour whole experience. 3ways to draw in (best have at least 2 of these and multiple intros)
+1. Sell you with the narrative 2. Wow you with the mechanics 3. Draw you in with the spectacle
+Mystery is a great tool for hooking someone. Can also sell the world  (put what is compelling in there and don't hold back)
+Deliver why player would want to play the game and deliver in 1st 5 minute (don't even have to take away powers). Shouldn't front load tutorial either. They simplified it
+Start with spectacular or novel. Can throw into a story already in progress (in medius res)</t>
+  </si>
+  <si>
+    <t>14 - 45 going through lists, still need to go through written work then clean up the actual list before priority and breaking down big ones.</t>
+  </si>
+  <si>
+    <t>Update Launcher</t>
+  </si>
+  <si>
+    <t>Weather</t>
+  </si>
+  <si>
+    <t>Ingame Settings</t>
+  </si>
+  <si>
+    <t>In GUI window</t>
+  </si>
+  <si>
+    <t>Adding your dad, Alex Jones, Arnold, Jesse Ventura, auto turrets etc, harry potter ring that can talk to the dead
+-Even more secret place under okons storage place. Leads to underground base.
+Mike the liar random event. Running across campus saying stuff. Comments on 4th wall things about the game ex) "They need an autocomplete"
+Stackable Visor Glasses
+Brendan's jacket holds things in the game
+scuba Steve (and it's Haugen)</t>
+  </si>
+  <si>
+    <t>Ritual gone wrong that spawns dumb undead things at night. 
+Ritual involves turning Casion calculator into the other.
+If you go to edge and press side 1000(50) times you go around to the other edge
+Pressing down 420 times in a certain place sents you to hell and you fight satan, and Bezabad plays.
+You can also sumon Satan to get the joint of destiny
+Teachers come back to life and you can kill zombie versions of them</t>
+  </si>
+  <si>
+    <t>Nazi Zombies</t>
+  </si>
+  <si>
+    <t>Just bassically Nazi Zombies mode
+ Wunderwaffe DG-2  1000, 100, -10
+      Chain lightning! 115 not included</t>
+  </si>
+  <si>
+    <t>Farming</t>
+  </si>
+  <si>
+    <t>Real life farming times for best weapons
+    Every 1/20 pumpkin gives mutated Wunder pumpkin which is best headgear
+     Because it's better reactor it's mutated
+     If creating long term things need to have good, stable, encrypted save files that can be updated with version
+     Create element 420 in the reactor to make wonder weapons</t>
+  </si>
+  <si>
+    <t>See 13 Hollywood Productions March 7th large section of ideas.
+Make combat more turn based with actions, reactions, preps, combos, etc. Maybe some skill involved? Mashing a key to beat someone. At least for now someone comes back for round two.
+Every Person has their own weakness.
+Use Darksouls style damage system
+Bullet time</t>
+  </si>
+  <si>
+    <t>Classes, object methods, how map works, commenting code. Updating to python 3. Interactables class. Buildings as an entity.
+PP8 style using PyCharm
+Get rid of global variables and restructure code
+Make an entity class (name, description, location, stats, health, item need, item give, inventory, deathtext, etc) and then all subclasses  using inheritance
+Entity
+     Person(each has same attributes and stuff, even schedule would be the same)
+          Boss?
+     Place
+          Interroor
+     Item
+          Interactable
+          Interactable can go, just add a moveable flag to items with new entity structute that allows give/take</t>
+  </si>
+  <si>
+    <t>Make PAP unlock when you get to end of game
+Unlocked by finishing all of the game
+Sound of lightening
+ followed by the sounds of cowboys
+Looks like you need to give something to get something in return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding explinations to all jokes and inside things to keep game relavent. Not sure if this would take away from game OR if you would only play the year you have it. Idk.
+When characters die they drop bio cheet and what their interests are (credits like a great help for devloping game)
+Add better biosheet, description of items to explain jokes, a tutorial, and more help to have players finish the game and enjoy it
+</t>
+  </si>
+  <si>
+    <t>Year selector, tutorial, intro, Map/characters, storyline/quests. This is a substantial piece of work
+See Google Keep notes</t>
+  </si>
+  <si>
+    <t>15 - 120 Attempted to make game playable by changing sound effects, realized will be unplayble until inbetween build, layed game without secrets to look for feedback and balance (file called Doug for Alpha0.29, made file in balance folder, Added last things from google keep notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -791,6 +1032,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF202124"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -812,7 +1059,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -839,6 +1086,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1122,7 +1374,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,7 +1409,7 @@
         <v>14</v>
       </c>
       <c r="J7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1168,128 +1420,131 @@
         <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" t="s">
         <v>92</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>93</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>94</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>95</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>96</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>97</v>
-      </c>
-      <c r="G9" t="s">
-        <v>98</v>
       </c>
       <c r="I9" s="9">
         <v>45</v>
       </c>
       <c r="J9" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C10" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="D10" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="E10" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="F10" t="s">
-        <v>102</v>
+        <v>281</v>
       </c>
       <c r="G10" t="s">
-        <v>103</v>
+        <v>297</v>
+      </c>
+      <c r="H10">
+        <v>330</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" t="s">
         <v>104</v>
       </c>
-      <c r="B11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="F11" t="s">
         <v>105</v>
       </c>
-      <c r="D11" t="s">
+      <c r="G11" t="s">
         <v>106</v>
-      </c>
-      <c r="E11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F11" t="s">
-        <v>108</v>
-      </c>
-      <c r="G11" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" t="s">
         <v>110</v>
       </c>
-      <c r="B12" t="s">
+      <c r="E12" t="s">
         <v>111</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F12" t="s">
         <v>112</v>
       </c>
-      <c r="D12" t="s">
+      <c r="G12" t="s">
         <v>113</v>
-      </c>
-      <c r="E12" t="s">
-        <v>114</v>
-      </c>
-      <c r="F12" t="s">
-        <v>115</v>
-      </c>
-      <c r="G12" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" t="s">
         <v>117</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" t="s">
         <v>119</v>
       </c>
-      <c r="C13" t="s">
+      <c r="F13" t="s">
         <v>120</v>
       </c>
-      <c r="D13" t="s">
+      <c r="G13" t="s">
         <v>121</v>
-      </c>
-      <c r="E13" t="s">
-        <v>122</v>
-      </c>
-      <c r="F13" t="s">
-        <v>123</v>
-      </c>
-      <c r="G13" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1299,10 +1554,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" activeCellId="1" sqref="J4 J6"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1936,7 +2191,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>23</v>
       </c>
@@ -1953,7 +2208,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>25</v>
       </c>
@@ -1967,7 +2222,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>26</v>
       </c>
@@ -1987,7 +2242,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>27</v>
       </c>
@@ -2004,7 +2259,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>29</v>
       </c>
@@ -2024,47 +2279,136 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>30</v>
+      </c>
       <c r="B38" s="1"/>
       <c r="F38" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+      <c r="F39" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+      <c r="F40" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+      <c r="F41" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+      <c r="F42" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+      <c r="F43" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
+      <c r="F44" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="1"/>
+      <c r="G45" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="1"/>
+      <c r="F46" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="1"/>
+      <c r="F47" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="1"/>
+      <c r="F48" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="1"/>
+      <c r="F49" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="1"/>
+      <c r="F50" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F53" s="15" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="15" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F55" s="15" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F56" s="15" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="15" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F58" s="16" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F59" s="15" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F62" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:F50">
@@ -2082,10 +2426,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P47"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2110,7 +2454,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -2162,8 +2506,8 @@
       <c r="E5" t="s">
         <v>82</v>
       </c>
-      <c r="F5" t="s">
-        <v>210</v>
+      <c r="F5" s="14" t="s">
+        <v>293</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>87</v>
@@ -2203,17 +2547,17 @@
       <c r="E6" t="s">
         <v>84</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="H6" t="s">
         <v>89</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>90</v>
-      </c>
-      <c r="I6" t="s">
-        <v>91</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>16</v>
@@ -2239,25 +2583,25 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" t="s">
+        <v>236</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="H7" t="s">
         <v>126</v>
       </c>
-      <c r="F7" t="s">
-        <v>127</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="H7" t="s">
-        <v>130</v>
-      </c>
       <c r="I7" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>13</v>
@@ -2286,19 +2630,19 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>132</v>
-      </c>
-      <c r="F8" t="s">
-        <v>136</v>
+        <v>128</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>286</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>14</v>
@@ -2327,19 +2671,19 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>137</v>
-      </c>
-      <c r="F9" t="s">
-        <v>138</v>
+        <v>132</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>295</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H9" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="I9" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>17</v>
@@ -2365,22 +2709,22 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E10" t="s">
-        <v>141</v>
-      </c>
-      <c r="F10" t="s">
-        <v>237</v>
+        <v>135</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>267</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H10" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="I10" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>15</v>
@@ -2406,25 +2750,25 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D11" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E11" t="s">
         <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>144</v>
+        <v>231</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H11" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="I11" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>11</v>
@@ -2438,25 +2782,25 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D12" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="E12" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="F12" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="H12" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="I12" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>79</v>
@@ -2473,25 +2817,25 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D13" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="E13" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="F13" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H13" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="I13" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>17</v>
@@ -2508,17 +2852,17 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="F14" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="I14" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>14</v>
@@ -2532,22 +2876,22 @@
         <v>15</v>
       </c>
       <c r="D15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E15" t="s">
+        <v>162</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="H15" t="s">
         <v>170</v>
       </c>
-      <c r="E15" t="s">
-        <v>169</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="I15" t="s">
         <v>171</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="H15" t="s">
-        <v>179</v>
-      </c>
-      <c r="I15" t="s">
-        <v>180</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>15</v>
@@ -2561,22 +2905,22 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="E16" t="s">
+        <v>166</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="H16" t="s">
         <v>174</v>
       </c>
-      <c r="F16" t="s">
-        <v>175</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="H16" t="s">
-        <v>183</v>
-      </c>
       <c r="I16" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2587,25 +2931,25 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F17" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H17" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="I17" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2616,25 +2960,25 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="D18">
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="F18" t="s">
-        <v>185</v>
+        <v>234</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H18" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="I18" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2645,25 +2989,25 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="D19">
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="F19" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="H19" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="I19" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2677,19 +3021,19 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="F20" t="s">
-        <v>193</v>
+        <v>239</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H20" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="I20" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2700,22 +3044,22 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E21" t="s">
-        <v>200</v>
-      </c>
-      <c r="F21" t="s">
-        <v>201</v>
+        <v>189</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>246</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="H21" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="I21" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2729,19 +3073,19 @@
         <v>15</v>
       </c>
       <c r="E22" t="s">
-        <v>205</v>
-      </c>
-      <c r="F22" t="s">
-        <v>206</v>
+        <v>193</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>250</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H22" t="s">
-        <v>207</v>
+        <v>194</v>
       </c>
       <c r="I22" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2755,19 +3099,19 @@
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>209</v>
-      </c>
-      <c r="F23" t="s">
-        <v>211</v>
+        <v>196</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>276</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H23" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="I23" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2778,22 +3122,22 @@
         <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="E24" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="F24" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="H24" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="I24" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2808,19 +3152,19 @@
         <v>4</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2834,19 +3178,19 @@
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="F26" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H26" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="I26" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2856,6 +3200,9 @@
       <c r="B27" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E27" t="s">
+        <v>282</v>
+      </c>
       <c r="G27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2865,6 +3212,9 @@
       <c r="B28" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E28" t="s">
+        <v>283</v>
+      </c>
       <c r="G28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2874,6 +3224,12 @@
       <c r="B29" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E29" t="s">
+        <v>284</v>
+      </c>
+      <c r="F29" t="s">
+        <v>285</v>
+      </c>
       <c r="G29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2883,6 +3239,12 @@
       <c r="B30" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E30" t="s">
+        <v>279</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>280</v>
+      </c>
       <c r="G30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2892,6 +3254,12 @@
       <c r="B31" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E31" t="s">
+        <v>273</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>277</v>
+      </c>
       <c r="G31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2902,13 +3270,13 @@
         <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="E32" t="s">
-        <v>228</v>
-      </c>
-      <c r="F32" t="s">
-        <v>230</v>
+        <v>213</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>247</v>
       </c>
       <c r="G32" s="10"/>
     </row>
@@ -2920,10 +3288,10 @@
         <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="F33" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="G33" s="10"/>
     </row>
@@ -2935,10 +3303,10 @@
         <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>233</v>
-      </c>
-      <c r="F34" t="s">
-        <v>234</v>
+        <v>217</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>269</v>
       </c>
       <c r="G34" s="10"/>
     </row>
@@ -2949,6 +3317,12 @@
       <c r="B35" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E35" t="s">
+        <v>219</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>268</v>
+      </c>
       <c r="G35" s="10"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2958,6 +3332,12 @@
       <c r="B36" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E36" t="s">
+        <v>235</v>
+      </c>
+      <c r="F36" t="s">
+        <v>251</v>
+      </c>
       <c r="G36" s="10"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2967,6 +3347,12 @@
       <c r="B37" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E37" t="s">
+        <v>257</v>
+      </c>
+      <c r="F37" s="14" t="s">
+        <v>287</v>
+      </c>
       <c r="G37" s="10"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2976,6 +3362,12 @@
       <c r="B38" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E38" t="s">
+        <v>237</v>
+      </c>
+      <c r="F38" t="s">
+        <v>238</v>
+      </c>
       <c r="G38" s="10"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2985,24 +3377,111 @@
       <c r="B39" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E39" t="s">
+        <v>240</v>
+      </c>
+      <c r="F39" t="s">
+        <v>241</v>
+      </c>
       <c r="G39" s="10"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="E40" t="s">
+        <v>242</v>
+      </c>
+      <c r="F40" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>244</v>
+      </c>
+      <c r="F41" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>248</v>
+      </c>
+      <c r="F42" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>254</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>261</v>
+      </c>
+      <c r="F44" s="14" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="50" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>288</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>290</v>
+      </c>
+      <c r="F51" s="14" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="53" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="54" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D47" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="O5:O10">
     <sortCondition descending="1" ref="O5"/>
   </sortState>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B39">
       <formula1>$K$5:$K$10</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Finished features list overview. Needs refinement
</commit_message>
<xml_diff>
--- a/Dev/EBTA Developent Roadmap.xlsx
+++ b/Dev/EBTA Developent Roadmap.xlsx
@@ -18,6 +18,7 @@
     <sheet name="Habit Diagram" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alpha 0.30 Feature Lock'!$A$4:$I$54</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Feedback!$A$1:$F$50</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="398">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -335,9 +336,6 @@
     <t>9 -</t>
   </si>
   <si>
-    <t>16 -</t>
-  </si>
-  <si>
     <t>18 -</t>
   </si>
   <si>
@@ -377,9 +375,6 @@
     <t>30 -</t>
   </si>
   <si>
-    <t>17 -</t>
-  </si>
-  <si>
     <t>1 -</t>
   </si>
   <si>
@@ -740,9 +735,6 @@
     <t>Collectables and Trophies</t>
   </si>
   <si>
-    <t>Make a basic interrior of bsb and fully test.</t>
-  </si>
-  <si>
     <t>NPCs</t>
   </si>
   <si>
@@ -759,9 +751,6 @@
   </si>
   <si>
     <t>Desctruction</t>
-  </si>
-  <si>
-    <t>Building and all things are breakable/fightable/destroyable.</t>
   </si>
   <si>
     <t>GTA Police</t>
@@ -801,17 +790,6 @@
     <t>Scater Erik Update</t>
   </si>
   <si>
-    <t xml:space="preserve">. You see a campus police guard pull up to talk to someone on the skateboard.
-"Erik the Sk8r: Hey Bill"
-"Bill the Mac Cop: Hey Erik, you know you can't be here right?"
-"Bill: Comomon man we do this every day"
-"Erik: Okay then, see you tomorrow!"
-He scates off quickly up 
-"Bill the Mac Cop: You can't skate on campus prop... aww whatever."
-Involves lore from the skate video
-</t>
-  </si>
-  <si>
     <t>Belzabad plays when you fight kleiman</t>
   </si>
   <si>
@@ -828,9 +806,6 @@
   </si>
   <si>
     <t>Hollywood Expansion</t>
-  </si>
-  <si>
-    <t>Hollywood Murder Mystery</t>
   </si>
   <si>
     <t>Philpocalpyse storyline</t>
@@ -854,10 +829,6 @@
 You can fly up too far and fly out of the game</t>
   </si>
   <si>
-    <t>Easy, Medium, Hard, Ironman verson where can't heal/carry more than you can. Maybe all with different endings.
-Easy-medium-Hardcore modes where you have 1. map w. quest outline (maybe a box?) - exploitable map/looking - no map  2. Enemy difficulty 3. Item outlines? 4. No eating 5. Full inventory vs expandable vs just you?</t>
-  </si>
-  <si>
     <t>Have Brendan Fallon character with eclipse mug, rocketry t-shirt, Strainer on head?SafetyGlasses?, and iron ring</t>
   </si>
   <si>
@@ -879,11 +850,6 @@
     <t>Mini-gamers around area. Not made by me but implemented. Including pong, chess (Mitch), tetris (Zac), Zork, and watching Ascii new hope, Classic riddles/storries (goat, chicken, fox)
 Liars Dice
  Tyler and Angus in full pirate gear, Hani is part of the wall (part of the ship part of the crew (the Die is cast and Davy Jones is there as well )</t>
-  </si>
-  <si>
-    <t>People drop money/you can make money
-Petter is a seller and you can buy Marvin the Martian thing
-Can drop a little bit from cops but not too much to farm</t>
   </si>
   <si>
     <t>Easier way to access game, not just goo.gl/iK8dL9 (Website)</t>
@@ -912,9 +878,6 @@
     <t>Ingame Settings</t>
   </si>
   <si>
-    <t>In GUI window</t>
-  </si>
-  <si>
     <t>Adding your dad, Alex Jones, Arnold, Jesse Ventura, auto turrets etc, harry potter ring that can talk to the dead
 -Even more secret place under okons storage place. Leads to underground base.
 Mike the liar random event. Running across campus saying stuff. Comments on 4th wall things about the game ex) "They need an autocomplete"
@@ -923,14 +886,6 @@
 scuba Steve (and it's Haugen)</t>
   </si>
   <si>
-    <t>Ritual gone wrong that spawns dumb undead things at night. 
-Ritual involves turning Casion calculator into the other.
-If you go to edge and press side 1000(50) times you go around to the other edge
-Pressing down 420 times in a certain place sents you to hell and you fight satan, and Bezabad plays.
-You can also sumon Satan to get the joint of destiny
-Teachers come back to life and you can kill zombie versions of them</t>
-  </si>
-  <si>
     <t>Nazi Zombies</t>
   </si>
   <si>
@@ -956,9 +911,30 @@
 Bullet time</t>
   </si>
   <si>
+    <t>Make PAP unlock when you get to end of game
+Unlocked by finishing all of the game
+Sound of lightening
+ followed by the sounds of cowboys
+Looks like you need to give something to get something in return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding explinations to all jokes and inside things to keep game relavent. Not sure if this would take away from game OR if you would only play the year you have it. Idk.
+When characters die they drop bio cheet and what their interests are (credits like a great help for devloping game)
+Add better biosheet, description of items to explain jokes, a tutorial, and more help to have players finish the game and enjoy it
+</t>
+  </si>
+  <si>
+    <t>Year selector, tutorial, intro, Map/characters, storyline/quests. This is a substantial piece of work
+See Google Keep notes</t>
+  </si>
+  <si>
+    <t>15 - 120 Attempted to make game playable by changing sound effects, realized will be unplayble until inbetween build, layed game without secrets to look for feedback and balance (file called Doug for Alpha0.29, made file in balance folder, Added last things from google keep notes</t>
+  </si>
+  <si>
     <t>Classes, object methods, how map works, commenting code. Updating to python 3. Interactables class. Buildings as an entity.
 PP8 style using PyCharm
 Get rid of global variables and restructure code
+Using and understanding effecient python code chunks (See Liam F. and his book)
 Make an entity class (name, description, location, stats, health, item need, item give, inventory, deathtext, etc) and then all subclasses  using inheritance
 Entity
      Person(each has same attributes and stuff, even schedule would be the same)
@@ -970,31 +946,366 @@
           Interactable can go, just add a moveable flag to items with new entity structute that allows give/take</t>
   </si>
   <si>
-    <t>Make PAP unlock when you get to end of game
-Unlocked by finishing all of the game
-Sound of lightening
- followed by the sounds of cowboys
-Looks like you need to give something to get something in return</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adding explinations to all jokes and inside things to keep game relavent. Not sure if this would take away from game OR if you would only play the year you have it. Idk.
-When characters die they drop bio cheet and what their interests are (credits like a great help for devloping game)
-Add better biosheet, description of items to explain jokes, a tutorial, and more help to have players finish the game and enjoy it
+    <t>A way to make game update automatically is with an update launcher. Only if not going online</t>
+  </si>
+  <si>
+    <t>People who like being involved w. development and feedback, like to play updates</t>
+  </si>
+  <si>
+    <t>Early acess, easy to follow along, easy to update and keep save files</t>
+  </si>
+  <si>
+    <t>15 ?</t>
+  </si>
+  <si>
+    <t>Adding different weather changes, debufs, and envoirnment to keep up emersion</t>
+  </si>
+  <si>
+    <t>0.36</t>
+  </si>
+  <si>
+    <t>Immersive Dynamic world</t>
+  </si>
+  <si>
+    <t>RPGers, readers</t>
+  </si>
+  <si>
+    <t>Full fleshed, easy to change for settings</t>
+  </si>
+  <si>
+    <t>In GUI window have options to save/load game, pause, volume settings, window size, text size, colour settings maybe?
+These settings are saved locally to the game file</t>
+  </si>
+  <si>
+    <t>Anyone who wants to setup perfect</t>
+  </si>
+  <si>
+    <t>BD, 12?</t>
+  </si>
+  <si>
+    <t>Easy for new players old alike</t>
+  </si>
+  <si>
+    <t>A new or old player</t>
+  </si>
+  <si>
+    <t>Immersed Economy</t>
+  </si>
+  <si>
+    <t>RPGers, economists</t>
+  </si>
+  <si>
+    <t>People drop money/you can make money
+Petter is a seller and you can buy Marvin the Martian thing
+Can drop a little bit from cops but not too much to farm
+Investing in stocks
+Grand exchange for items</t>
+  </si>
+  <si>
+    <t>Boss balance</t>
+  </si>
+  <si>
+    <t>Making sure all bosses are beatable without secrets so at least not frustrating for new players</t>
+  </si>
+  <si>
+    <t>Challenging but not punishing</t>
+  </si>
+  <si>
+    <t>People who don't mind a challenge</t>
+  </si>
+  <si>
+    <t>Balanced and nice to play in many parallel ways</t>
+  </si>
+  <si>
+    <t>Immersive</t>
+  </si>
+  <si>
+    <t>0.33?</t>
+  </si>
+  <si>
+    <t>Boss Balance</t>
+  </si>
+  <si>
+    <t>Easy, Medium, Hard, Ironman verson where can't heal/carry more than you can. Maybe all with different endings.
+Easy-medium-Hardcore modes where you have 1. map w. quest outline (maybe a box?) - exploitable map/looking - no map  2. Enemy difficulty 3. Item outlines? 4. No eating 5. Full inventory vs expandable vs just you?
+Try not to do just simple health/attack scaling. Maybe add new mechanics</t>
+  </si>
+  <si>
+    <t>Game for all people, returning or new</t>
+  </si>
+  <si>
+    <t>People who like a challenge</t>
+  </si>
+  <si>
+    <t>0.36?</t>
+  </si>
+  <si>
+    <t>Lots of endgame content</t>
+  </si>
+  <si>
+    <t>Collectors/maxers</t>
+  </si>
+  <si>
+    <t>Completionists</t>
+  </si>
+  <si>
+    <t>0.37 ?</t>
+  </si>
+  <si>
+    <t>Rewarding for going along progress, collectable</t>
+  </si>
+  <si>
+    <t>0.38</t>
+  </si>
+  <si>
+    <t>Spooky</t>
+  </si>
+  <si>
+    <t>Immersive, like people</t>
+  </si>
+  <si>
+    <t>Creative Mode</t>
+  </si>
+  <si>
+    <t>0.37?</t>
+  </si>
+  <si>
+    <t>Fix Description List</t>
+  </si>
+  <si>
+    <t>Breakdown big ones</t>
+  </si>
+  <si>
+    <t>Compile big list</t>
+  </si>
+  <si>
+    <t>Put priorties/finish list</t>
+  </si>
+  <si>
+    <t>Integrate bug/must have from feedback</t>
+  </si>
+  <si>
+    <t>Endgame Content</t>
+  </si>
+  <si>
+    <t>Crazy, references</t>
+  </si>
+  <si>
+    <t>0.38?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Building and all things are breakable/fightable/destroyable.
+When things break the items/characters get put on main floor but dead, interrior destroyed, </t>
+  </si>
+  <si>
+    <t>Make a basic interrior of bsb and fully test. Then make all multilevel buildings an interrior</t>
+  </si>
+  <si>
+    <t>Crazy, creative</t>
+  </si>
+  <si>
+    <t>Anarchists</t>
+  </si>
+  <si>
+    <t>0.35 ?</t>
+  </si>
+  <si>
+    <t>Consequences/acountability for killing</t>
+  </si>
+  <si>
+    <t>Survivalists</t>
+  </si>
+  <si>
+    <t>GUI, Text display</t>
+  </si>
+  <si>
+    <t>Beautiful, bright, contrast</t>
+  </si>
+  <si>
+    <t>People who like seeing things</t>
+  </si>
+  <si>
+    <t>0.39?</t>
+  </si>
+  <si>
+    <t>0.40?</t>
+  </si>
+  <si>
+    <t>0.42?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Involves lore from the skate video
+. You see a campus police guard pull up to talk to someone on the skateboard.
+"Erik the Sk8r: Hey Bill"
+"Bill the Mac Cop: Hey Erik, you know you can't be here right?"
+"Bill: Comomon man we do this every day"
+"Erik: Okay then, see you tomorrow!"
+He scates off quickly up 
+"Bill the Mac Cop: You can't skate on campus prop... aww whatever."
 </t>
   </si>
   <si>
-    <t>Year selector, tutorial, intro, Map/characters, storyline/quests. This is a substantial piece of work
-See Google Keep notes</t>
-  </si>
-  <si>
-    <t>15 - 120 Attempted to make game playable by changing sound effects, realized will be unplayble until inbetween build, layed game without secrets to look for feedback and balance (file called Doug for Alpha0.29, made file in balance folder, Added last things from google keep notes</t>
+    <t>Hollywood House</t>
+  </si>
+  <si>
+    <t>Lots of inside references</t>
+  </si>
+  <si>
+    <t>30?</t>
+  </si>
+  <si>
+    <t>Scater Update</t>
+  </si>
+  <si>
+    <t>Hollywood Murder Mystery. All aspects and functions of hollywood</t>
+  </si>
+  <si>
+    <t>Integrate into other things</t>
+  </si>
+  <si>
+    <t>Matlab, HFF 2020, any other game I make</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Someone who likes text adventures</t>
+  </si>
+  <si>
+    <t>My pride work shown everywhere</t>
+  </si>
+  <si>
+    <t>Immersive world with lots of areas</t>
+  </si>
+  <si>
+    <t>Eng Phys, survalists</t>
+  </si>
+  <si>
+    <t>Phil clones himself to make it more efficient but gets out of control
+Have to fight off all ranges of Phils
+Only way to kill them is to poisen cafine supply into the school. So only drunk Phil remains</t>
+  </si>
+  <si>
+    <t>20?</t>
+  </si>
+  <si>
+    <t>GTA police</t>
+  </si>
+  <si>
+    <t>Crazy, lots of content</t>
+  </si>
+  <si>
+    <t>Fight combatants against eachother (including different Phils).
+Can also fight in it yourself</t>
+  </si>
+  <si>
+    <t>15?</t>
+  </si>
+  <si>
+    <t>Minigame/fighting challenge</t>
+  </si>
+  <si>
+    <t>Fighters</t>
+  </si>
+  <si>
+    <t>Me</t>
+  </si>
+  <si>
+    <t>You teliport to green lake, explore all the mysteries of Brendan Fallon's past and life</t>
+  </si>
+  <si>
+    <t>For Myself</t>
+  </si>
+  <si>
+    <t>Looking to grow</t>
+  </si>
+  <si>
+    <t>People who want community/involvement</t>
+  </si>
+  <si>
+    <t>Artwork/title screens</t>
+  </si>
+  <si>
+    <t>Having a ascii art converter and font typing creator, making a cover picture, having all the pictures of stuff in game</t>
+  </si>
+  <si>
+    <t>30 ?</t>
+  </si>
+  <si>
+    <t>Make facebook, twitter, website, instagram outreach and update to keep players/community involved and invite new players</t>
+  </si>
+  <si>
+    <t>Open to all People</t>
+  </si>
+  <si>
+    <t>Mac Eng Students</t>
+  </si>
+  <si>
+    <t>Expand Map to whole school, make a storyline containing first year eng experience</t>
+  </si>
+  <si>
+    <t>Google Maps Import</t>
+  </si>
+  <si>
+    <t>10 ?</t>
+  </si>
+  <si>
+    <t>Zombie Lovers</t>
+  </si>
+  <si>
+    <t>Games/projects need synthergy to be more than the sum of their parts</t>
+  </si>
+  <si>
+    <t>Layout roadmap/plan document</t>
+  </si>
+  <si>
+    <t>Darkness lovers</t>
+  </si>
+  <si>
+    <t>Ritual gone wrong that spawns dumb undead things at night. 
+Ritual involves turning Casion calculator into the other.
+If you go to edge and press side 1000(50) times you go around to the other edge
+Pressing down 420 times in a certain place sents you to hell and you fight satan, and Bezabad plays.
+You can also sumon Satan to get the joint of destiny
+Teachers come back to life and you can kill zombie versions of them
+Maybe involve kathulu</t>
+  </si>
+  <si>
+    <t>Minigames, crazyness</t>
+  </si>
+  <si>
+    <t>Megan Goodland, Farmers</t>
+  </si>
+  <si>
+    <t>Endgame/many ways to play</t>
+  </si>
+  <si>
+    <t>20 ?</t>
+  </si>
+  <si>
+    <t>16 - X</t>
+  </si>
+  <si>
+    <t>17 - 45 finished feature lock list, needs descr. Cleanup, feedback, and review</t>
+  </si>
+  <si>
+    <t>Would like to finish feature lock at least and get into breakdown</t>
+  </si>
+  <si>
+    <t>Breakdown</t>
+  </si>
+  <si>
+    <t>Feature lock release Oct 1?</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1038,6 +1349,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1059,7 +1378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1091,6 +1410,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1374,7 +1694,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,11 +1765,14 @@
       <c r="G9" t="s">
         <v>97</v>
       </c>
+      <c r="H9" t="s">
+        <v>397</v>
+      </c>
       <c r="I9" s="9">
         <v>45</v>
       </c>
       <c r="J9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1457,22 +1780,22 @@
         <v>100</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D10" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F10" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="G10" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="H10">
         <v>330</v>
@@ -1480,71 +1803,80 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>392</v>
+      </c>
+      <c r="B11" t="s">
+        <v>393</v>
+      </c>
+      <c r="C11" t="s">
         <v>101</v>
       </c>
-      <c r="B11" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>102</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>103</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>104</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>105</v>
       </c>
-      <c r="G11" t="s">
-        <v>106</v>
+      <c r="I11" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" t="s">
         <v>107</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>108</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>109</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>110</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>111</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>112</v>
       </c>
-      <c r="G12" t="s">
-        <v>113</v>
+      <c r="I12" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>113</v>
+      </c>
+      <c r="B13" t="s">
         <v>114</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" t="s">
         <v>116</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>117</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
         <v>118</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>119</v>
       </c>
-      <c r="F13" t="s">
-        <v>120</v>
-      </c>
-      <c r="G13" t="s">
-        <v>121</v>
+      <c r="I13" t="s">
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -1556,8 +1888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1567,28 +1899,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="17" t="s">
         <v>70</v>
       </c>
       <c r="J1" t="s">
@@ -2285,124 +2617,124 @@
       </c>
       <c r="B38" s="1"/>
       <c r="F38" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
       <c r="F39" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="F40" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B41" s="1"/>
       <c r="F41" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="F42" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
       <c r="F43" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="F44" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B45" s="1"/>
       <c r="G45" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" s="1"/>
       <c r="F46" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="F47" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B48" s="1"/>
       <c r="F48" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
       <c r="F49" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
       <c r="F50" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F51" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F52" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F53" s="15" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F54" s="15" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F55" s="15" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F56" s="15" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F57" s="15" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
     </row>
     <row r="58" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F58" s="16" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F59" s="15" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
@@ -2426,10 +2758,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P54"/>
+  <dimension ref="A1:P63"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2450,31 +2782,31 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="B4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="17" t="s">
         <v>81</v>
       </c>
       <c r="K4" t="s">
@@ -2507,7 +2839,7 @@
         <v>82</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>87</v>
@@ -2548,10 +2880,10 @@
         <v>84</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H6" t="s">
         <v>89</v>
@@ -2583,25 +2915,25 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" t="s">
+        <v>336</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" t="s">
+        <v>124</v>
+      </c>
+      <c r="I7" t="s">
         <v>123</v>
-      </c>
-      <c r="F7" t="s">
-        <v>236</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="H7" t="s">
-        <v>126</v>
-      </c>
-      <c r="I7" t="s">
-        <v>125</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>13</v>
@@ -2630,19 +2962,19 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="H8" t="s">
         <v>128</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>286</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="I8" t="s">
         <v>129</v>
-      </c>
-      <c r="H8" t="s">
-        <v>130</v>
-      </c>
-      <c r="I8" t="s">
-        <v>131</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>14</v>
@@ -2671,19 +3003,19 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="H9" t="s">
         <v>132</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>295</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>165</v>
-      </c>
-      <c r="H9" t="s">
-        <v>134</v>
-      </c>
       <c r="I9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>17</v>
@@ -2709,22 +3041,22 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E10" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" t="s">
+        <v>134</v>
+      </c>
+      <c r="I10" t="s">
         <v>135</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>267</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="H10" t="s">
-        <v>136</v>
-      </c>
-      <c r="I10" t="s">
-        <v>137</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>15</v>
@@ -2750,25 +3082,25 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E11" t="s">
         <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>11</v>
@@ -2782,25 +3114,25 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" t="s">
+        <v>144</v>
+      </c>
+      <c r="E12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" t="s">
+        <v>155</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D12" t="s">
-        <v>146</v>
-      </c>
-      <c r="E12" t="s">
-        <v>145</v>
-      </c>
-      <c r="F12" t="s">
-        <v>157</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>149</v>
-      </c>
       <c r="H12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>79</v>
@@ -2817,25 +3149,25 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" t="s">
         <v>153</v>
       </c>
-      <c r="D13" t="s">
-        <v>146</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="G13" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="H13" t="s">
         <v>152</v>
       </c>
-      <c r="F13" t="s">
-        <v>155</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>154</v>
-      </c>
-      <c r="I13" t="s">
-        <v>156</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>17</v>
@@ -2852,17 +3184,17 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F14" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>14</v>
@@ -2876,22 +3208,22 @@
         <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E15" t="s">
+        <v>160</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>292</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>164</v>
-      </c>
       <c r="H15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>15</v>
@@ -2905,22 +3237,22 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="I16" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2931,25 +3263,25 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I17" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2960,25 +3292,25 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D18">
         <v>10</v>
       </c>
       <c r="E18" t="s">
+        <v>173</v>
+      </c>
+      <c r="F18" t="s">
+        <v>232</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H18" t="s">
         <v>175</v>
       </c>
-      <c r="F18" t="s">
-        <v>234</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="H18" t="s">
-        <v>177</v>
-      </c>
       <c r="I18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2989,25 +3321,25 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D19">
         <v>6</v>
       </c>
       <c r="E19" t="s">
+        <v>176</v>
+      </c>
+      <c r="F19" t="s">
         <v>178</v>
       </c>
-      <c r="F19" t="s">
-        <v>180</v>
-      </c>
       <c r="G19" s="10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -3021,19 +3353,19 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
+        <v>180</v>
+      </c>
+      <c r="F20" t="s">
+        <v>236</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H20" t="s">
+        <v>181</v>
+      </c>
+      <c r="I20" t="s">
         <v>182</v>
-      </c>
-      <c r="F20" t="s">
-        <v>239</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="H20" t="s">
-        <v>183</v>
-      </c>
-      <c r="I20" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -3044,22 +3376,22 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E21" t="s">
+        <v>187</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="H21" t="s">
         <v>189</v>
       </c>
-      <c r="F21" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="G21" s="10" t="s">
+      <c r="I21" t="s">
         <v>190</v>
-      </c>
-      <c r="H21" t="s">
-        <v>191</v>
-      </c>
-      <c r="I21" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -3073,19 +3405,19 @@
         <v>15</v>
       </c>
       <c r="E22" t="s">
+        <v>191</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>246</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="H22" t="s">
+        <v>192</v>
+      </c>
+      <c r="I22" t="s">
         <v>193</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="H22" t="s">
-        <v>194</v>
-      </c>
-      <c r="I22" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -3099,19 +3431,19 @@
         <v>8</v>
       </c>
       <c r="E23" t="s">
+        <v>194</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="H23" t="s">
+        <v>195</v>
+      </c>
+      <c r="I23" t="s">
         <v>196</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="H23" t="s">
-        <v>197</v>
-      </c>
-      <c r="I23" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3122,22 +3454,22 @@
         <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E24" t="s">
+        <v>197</v>
+      </c>
+      <c r="F24" t="s">
+        <v>201</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="H24" t="s">
         <v>199</v>
       </c>
-      <c r="F24" t="s">
-        <v>203</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="H24" t="s">
-        <v>201</v>
-      </c>
       <c r="I24" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -3152,19 +3484,19 @@
         <v>4</v>
       </c>
       <c r="E25" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="F25" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="F25" s="11" t="s">
-        <v>206</v>
-      </c>
       <c r="G25" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -3178,19 +3510,19 @@
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F26" t="s">
+        <v>206</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H26" t="s">
         <v>208</v>
       </c>
-      <c r="G26" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="H26" t="s">
-        <v>210</v>
-      </c>
       <c r="I26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -3198,291 +3530,809 @@
         <v>23</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>291</v>
       </c>
       <c r="E27" t="s">
-        <v>282</v>
-      </c>
-      <c r="G27" s="10"/>
+        <v>274</v>
+      </c>
+      <c r="F27" t="s">
+        <v>288</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="H27" t="s">
+        <v>290</v>
+      </c>
+      <c r="I27" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>24</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>173</v>
+      </c>
+      <c r="D28">
+        <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>283</v>
-      </c>
-      <c r="G28" s="10"/>
+        <v>275</v>
+      </c>
+      <c r="F28" t="s">
+        <v>292</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="H28" t="s">
+        <v>294</v>
+      </c>
+      <c r="I28" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="C29" t="s">
+        <v>342</v>
+      </c>
+      <c r="D29" t="s">
+        <v>291</v>
       </c>
       <c r="E29" t="s">
-        <v>284</v>
-      </c>
-      <c r="F29" t="s">
-        <v>285</v>
-      </c>
-      <c r="G29" s="10"/>
+        <v>276</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H29" t="s">
+        <v>296</v>
+      </c>
+      <c r="I29" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="C30" t="s">
+        <v>164</v>
+      </c>
+      <c r="D30" t="s">
+        <v>299</v>
       </c>
       <c r="E30" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>280</v>
-      </c>
-      <c r="G30" s="10"/>
+        <v>272</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="I30" s="14" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="D31">
+        <v>8</v>
       </c>
       <c r="E31" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="G31" s="10"/>
+        <v>304</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="I31" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>214</v>
+        <v>212</v>
+      </c>
+      <c r="D32">
+        <v>12</v>
       </c>
       <c r="E32" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="G32" s="10"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="I32" s="14" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>29</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="D33">
+        <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F33" t="s">
-        <v>216</v>
-      </c>
-      <c r="G33" s="10"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>310</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>30</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="C34" t="s">
+        <v>312</v>
+      </c>
+      <c r="D34">
+        <v>16</v>
       </c>
       <c r="E34" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="G34" s="10"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>31</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="D35">
+        <v>20</v>
       </c>
       <c r="E35" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="G35" s="10"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="H35" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="I35" s="14" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>32</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="D36">
+        <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F36" t="s">
-        <v>251</v>
-      </c>
-      <c r="G36" s="10"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
+      </c>
+      <c r="D37">
+        <v>20</v>
       </c>
       <c r="E37" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="G37" s="10"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>387</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="H37" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="I37" s="14" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>34</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="C38" t="s">
+        <v>173</v>
+      </c>
+      <c r="D38">
+        <v>6</v>
       </c>
       <c r="E38" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F38" t="s">
-        <v>238</v>
-      </c>
-      <c r="G38" s="10"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H38" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="I38" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>35</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" t="s">
+        <v>325</v>
+      </c>
+      <c r="D39">
+        <v>12</v>
+      </c>
+      <c r="E39" t="s">
+        <v>237</v>
+      </c>
+      <c r="F39" t="s">
+        <v>238</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="H39" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="I39" s="14" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>36</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" t="s">
+        <v>325</v>
+      </c>
+      <c r="D40">
+        <v>20</v>
+      </c>
+      <c r="E40" t="s">
+        <v>239</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>335</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="I40" s="14" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>37</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s">
+        <v>240</v>
+      </c>
+      <c r="F41" t="s">
+        <v>241</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="H41" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="I41" s="14" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>38</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42">
         <v>7</v>
       </c>
-      <c r="E39" t="s">
-        <v>240</v>
-      </c>
-      <c r="F39" t="s">
-        <v>241</v>
-      </c>
-      <c r="G39" s="10"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
-      <c r="E40" t="s">
-        <v>242</v>
-      </c>
-      <c r="F40" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E41" t="s">
+      <c r="E42" t="s">
         <v>244</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F42" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E42" t="s">
-        <v>248</v>
-      </c>
-      <c r="F42" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G42" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H42" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="I42" s="14" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>39</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43">
+        <v>10</v>
+      </c>
       <c r="E43" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="H43" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="I43" s="14" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>40</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C44" t="s">
+        <v>352</v>
+      </c>
+      <c r="D44" t="s">
+        <v>351</v>
+      </c>
       <c r="E44" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="H44" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="I44" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>41</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" t="s">
+        <v>363</v>
+      </c>
+      <c r="D45" t="s">
+        <v>362</v>
+      </c>
       <c r="E45" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="H45" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="I45" s="14" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>42</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" t="s">
+        <v>366</v>
+      </c>
       <c r="E46" t="s">
+        <v>258</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="H46" s="14" t="s">
+        <v>367</v>
+      </c>
+      <c r="I46" s="14" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>43</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" t="s">
+        <v>362</v>
+      </c>
+      <c r="E47" t="s">
+        <v>259</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="I47" s="14" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>44</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" t="s">
+        <v>366</v>
+      </c>
+      <c r="E48" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E47" t="s">
+      <c r="F48" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="H48" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="I48" s="14" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>45</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" t="s">
+        <v>381</v>
+      </c>
+      <c r="D49" t="s">
+        <v>376</v>
+      </c>
+      <c r="E49" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E48" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E49" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="50" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="H49" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="I49" s="14" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>46</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" t="s">
+        <v>382</v>
+      </c>
       <c r="E50" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="H50" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="I50" s="14" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>47</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" t="s">
+        <v>391</v>
+      </c>
       <c r="E51" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="53" spans="5:6" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="H51" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="I51" s="14" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>48</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D52">
+        <v>8</v>
+      </c>
+      <c r="E52" t="s">
+        <v>305</v>
+      </c>
+      <c r="F52" t="s">
+        <v>306</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H52" t="s">
+        <v>307</v>
+      </c>
+      <c r="I52" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>49</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" t="s">
+        <v>356</v>
+      </c>
       <c r="E53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="54" spans="5:6" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+      <c r="F53" t="s">
+        <v>355</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="H53" t="s">
+        <v>358</v>
+      </c>
+      <c r="I53" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>50</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" t="s">
+        <v>164</v>
+      </c>
+      <c r="D54" t="s">
+        <v>136</v>
+      </c>
       <c r="E54" t="s">
+        <v>374</v>
+      </c>
+      <c r="F54" t="s">
+        <v>375</v>
+      </c>
+      <c r="G54" s="10"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
         <v>67</v>
       </c>
     </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D57" s="11" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
+        <v>384</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A4:I54"/>
   <sortState ref="O5:O10">
     <sortCondition descending="1" ref="O5"/>
   </sortState>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B39">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B54">
       <formula1>$K$5:$K$10</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
finished cleaning features and working on integrating feedback
</commit_message>
<xml_diff>
--- a/Dev/EBTA Developent Roadmap.xlsx
+++ b/Dev/EBTA Developent Roadmap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Outline" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="402">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -198,12 +198,6 @@
     <t>put DOD in game</t>
   </si>
   <si>
-    <t>Angus, Beef, Barber</t>
-  </si>
-  <si>
-    <t>"Call me a liar"</t>
-  </si>
-  <si>
     <t>"B is back" (Zac)</t>
   </si>
   <si>
@@ -213,9 +207,6 @@
     <t>Priorities</t>
   </si>
   <si>
-    <t>*Short word for verbs,  for inv, s for stats</t>
-  </si>
-  <si>
     <t>GUI</t>
   </si>
   <si>
@@ -336,9 +327,6 @@
     <t>9 -</t>
   </si>
   <si>
-    <t>18 -</t>
-  </si>
-  <si>
     <t>19 -</t>
   </si>
   <si>
@@ -492,15 +480,9 @@
     <t>MMORPG</t>
   </si>
   <si>
-    <t>Make other players be able to interact</t>
-  </si>
-  <si>
     <t>People who play MMOs, grindy people, compeditive, etc</t>
   </si>
   <si>
-    <t>Make game run in javascript/whatever online so you can play game online. Also has QT scoreboard so more compeditive</t>
-  </si>
-  <si>
     <t>Mobile gamers, anynonwindows/don't want to download. Basically any loose gamer. Also compeditive side online</t>
   </si>
   <si>
@@ -528,9 +510,6 @@
     <t>2019 Kipling Update</t>
   </si>
   <si>
-    <t>BD, 4+10+8+15+20?</t>
-  </si>
-  <si>
     <t>Music + Compile</t>
   </si>
   <si>
@@ -543,9 +522,6 @@
     <t>People who like grinding, more professional gamers, etc</t>
   </si>
   <si>
-    <t>Refine music so can transitions and have different music for different settings</t>
-  </si>
-  <si>
     <t>Enjoyable to play, adds more moods</t>
   </si>
   <si>
@@ -567,9 +543,6 @@
     <t>Makes game safter to play and give info to. Also less easy to hack.</t>
   </si>
   <si>
-    <t>Making so save/load and all personal game data is kept easy. Also encrypted transfer is better.</t>
-  </si>
-  <si>
     <t>Online</t>
   </si>
   <si>
@@ -636,9 +609,6 @@
     <t>25 ?</t>
   </si>
   <si>
-    <t>Use google maps data to design exteriors/interriors for things</t>
-  </si>
-  <si>
     <t>Pygame Build</t>
   </si>
   <si>
@@ -651,9 +621,6 @@
     <t>More features of eveyrthing</t>
   </si>
   <si>
-    <t>Make so it takes files automatically, gives icon automatically, does code checks, and installer gives desktop icon. Overwriting old instal to update would be nice.</t>
-  </si>
-  <si>
     <t>Beginniers and developers</t>
   </si>
   <si>
@@ -675,115 +642,39 @@
     <t>Name Manipulation</t>
   </si>
   <si>
-    <t xml:space="preserve">Do more with name including character address you by name and work with names including name infulence. </t>
-  </si>
-  <si>
     <t>Difficulties</t>
   </si>
   <si>
     <t>13 - ✔ Started going through old TODO lists.</t>
   </si>
   <si>
-    <t xml:space="preserve">Flying, Electricity, </t>
-  </si>
-  <si>
-    <t>Rebalance mechanics so that Speed plays more of an effect.</t>
-  </si>
-  <si>
-    <t>Right now defense is v important but with healing items added this should fix it</t>
-  </si>
-  <si>
-    <t>Better head items plz</t>
-  </si>
-  <si>
-    <t>Need to know that Jana has the textbook, maybe the story should say that somewhere</t>
-  </si>
-  <si>
-    <t>Not obveous that equip means to pick up</t>
-  </si>
-  <si>
-    <t>When you inspect the car it says 'Ya thought these were the keys"</t>
-  </si>
-  <si>
-    <t>When you searching when nothings there "You double take and there's still nothing there"</t>
-  </si>
-  <si>
-    <t>If you search 20 times you die</t>
-  </si>
-  <si>
     <t>After giving dirty needle to sharp exchange a random encounter with a person that says "You're the greatest semaritan in the world" and gives you and Uzi</t>
   </si>
   <si>
-    <t>Phil says that need to be pushed more toward the Phenoix</t>
-  </si>
-  <si>
     <t>Notes option (a list of all lore you've gone through)</t>
   </si>
   <si>
-    <t xml:space="preserve">Adding map and all suplementary info to the GUI (maybe whole game?) so we can customize content. IDK. I like idea of two window system with map, player icon, pictures, etc on side. </t>
-  </si>
-  <si>
     <t>Input (fast Addressing)</t>
   </si>
   <si>
-    <t>Make keywords shorter, have list of items to choose from quickly, maybe accept short names? Maybe take cardinal coords. More things rather than equip. Also possibly controller support?</t>
-  </si>
-  <si>
-    <t>Adding time to game. Maybe watch system, time based events, time based characters/moving, etc. Either BOTW 2 min for 1 hr with longest day, or minecraft. I don't think ever step 5 minutes. Starting day is 12pm, day of Kipling (for 2017-2018 version).</t>
-  </si>
-  <si>
     <t>Collectables and Trophies</t>
   </si>
   <si>
     <t>NPCs</t>
   </si>
   <si>
-    <t>They move around, have  a companion, can equip items to yourself to store for later games so they act as a companion.</t>
-  </si>
-  <si>
-    <t>Making so surroundings of obveous areas print out. Have lore print first and then title+search around you.</t>
-  </si>
-  <si>
     <t>Teliporter</t>
   </si>
   <si>
-    <t>Sling ring, teliport anywhere you know. Portal gun, teliport anywhere you can see. Instant transmission (anything). Zombies teliporter (where another one is but also in time). Star Trek teliport (anywhere but only to/from consol).</t>
-  </si>
-  <si>
     <t>Desctruction</t>
   </si>
   <si>
     <t>GTA Police</t>
   </si>
   <si>
-    <t xml:space="preserve">Star level where police come after you, eventually SWAT, eventually have to escape on rocket in smoke stack to go meet Elon musk on the moon. </t>
-  </si>
-  <si>
-    <t>Can add content to game and make their own quests/stories. 
-Maybe unlocks when you beat the game.</t>
-  </si>
-  <si>
-    <t>Attack and defense, speed doesn't do anything. Would need to be be after combat update. Possibly have star/some sort of indicator for bosses.
-More direct reward for exploration with something that ties back into game.</t>
-  </si>
-  <si>
     <t>Text Display</t>
   </si>
   <si>
-    <t>GUI text printer, change colour, font, style of words to highlight.</t>
-  </si>
-  <si>
-    <t>Move map to right side.
-Map display better, quest tracker, can give hints on where to go/where things are
-Ingame journal or notes function.</t>
-  </si>
-  <si>
-    <t>Keep track of all items/things collected</t>
-  </si>
-  <si>
-    <t>(more use of storyline, music, definition to people to give realism to the world)</t>
-  </si>
-  <si>
     <t>Some sort of skill component to fighting</t>
   </si>
   <si>
@@ -820,18 +711,6 @@
     <t>Tyler wants it to be Sandbox mode, no linear stuff, events unfold from there</t>
   </si>
   <si>
-    <t>Adding an experience level to the game and mobs that respawn so you feel like you're progressing. Probably buffs stats and helps you beat higher level people/things. Also the respawn with golden gauntlet thanos for Paul the buss driver.
-In general, have more crazy/dangerous things happen as you progress in quests/storyline (sand worms pop up, idk, crazyness)
-Could have random drop loot</t>
-  </si>
-  <si>
-    <t>Including Iron man suit with Energy, craftables and consumables with energy. Secret weird flying place/base. Secret places you can only get to by flying into upper buildings
-You can fly up too far and fly out of the game</t>
-  </si>
-  <si>
-    <t>Have Brendan Fallon character with eclipse mug, rocketry t-shirt, Strainer on head?SafetyGlasses?, and iron ring</t>
-  </si>
-  <si>
     <t>Social Media and Website</t>
   </si>
   <si>
@@ -841,31 +720,12 @@
     <t>Currency</t>
   </si>
   <si>
-    <t>Need story arc for body armour</t>
-  </si>
-  <si>
     <t>AR version of the game -Ekamada</t>
   </si>
   <si>
-    <t>Mini-gamers around area. Not made by me but implemented. Including pong, chess (Mitch), tetris (Zac), Zork, and watching Ascii new hope, Classic riddles/storries (goat, chicken, fox)
-Liars Dice
- Tyler and Angus in full pirate gear, Hani is part of the wall (part of the ship part of the crew (the Die is cast and Davy Jones is there as well )</t>
-  </si>
-  <si>
-    <t>Easier way to access game, not just goo.gl/iK8dL9 (Website)</t>
-  </si>
-  <si>
     <t>Tutorial</t>
   </si>
   <si>
-    <t>Start player in secluded area/small island to get a sense but still have tutorial
-First 5 minutes set tone of the game, set expectations and colour whole experience. 3ways to draw in (best have at least 2 of these and multiple intros)
-1. Sell you with the narrative 2. Wow you with the mechanics 3. Draw you in with the spectacle
-Mystery is a great tool for hooking someone. Can also sell the world  (put what is compelling in there and don't hold back)
-Deliver why player would want to play the game and deliver in 1st 5 minute (don't even have to take away powers). Shouldn't front load tutorial either. They simplified it
-Start with spectacular or novel. Can throw into a story already in progress (in medius res)</t>
-  </si>
-  <si>
     <t>14 - 45 going through lists, still need to go through written work then clean up the actual list before priority and breaking down big ones.</t>
   </si>
   <si>
@@ -878,65 +738,303 @@
     <t>Ingame Settings</t>
   </si>
   <si>
-    <t>Adding your dad, Alex Jones, Arnold, Jesse Ventura, auto turrets etc, harry potter ring that can talk to the dead
--Even more secret place under okons storage place. Leads to underground base.
-Mike the liar random event. Running across campus saying stuff. Comments on 4th wall things about the game ex) "They need an autocomplete"
-Stackable Visor Glasses
-Brendan's jacket holds things in the game
-scuba Steve (and it's Haugen)</t>
-  </si>
-  <si>
     <t>Nazi Zombies</t>
   </si>
   <si>
-    <t>Just bassically Nazi Zombies mode
- Wunderwaffe DG-2  1000, 100, -10
-      Chain lightning! 115 not included</t>
-  </si>
-  <si>
     <t>Farming</t>
   </si>
   <si>
-    <t>Real life farming times for best weapons
-    Every 1/20 pumpkin gives mutated Wunder pumpkin which is best headgear
-     Because it's better reactor it's mutated
-     If creating long term things need to have good, stable, encrypted save files that can be updated with version
-     Create element 420 in the reactor to make wonder weapons</t>
-  </si>
-  <si>
-    <t>See 13 Hollywood Productions March 7th large section of ideas.
-Make combat more turn based with actions, reactions, preps, combos, etc. Maybe some skill involved? Mashing a key to beat someone. At least for now someone comes back for round two.
-Every Person has their own weakness.
-Use Darksouls style damage system
-Bullet time</t>
-  </si>
-  <si>
-    <t>Make PAP unlock when you get to end of game
-Unlocked by finishing all of the game
-Sound of lightening
- followed by the sounds of cowboys
-Looks like you need to give something to get something in return</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adding explinations to all jokes and inside things to keep game relavent. Not sure if this would take away from game OR if you would only play the year you have it. Idk.
-When characters die they drop bio cheet and what their interests are (credits like a great help for devloping game)
-Add better biosheet, description of items to explain jokes, a tutorial, and more help to have players finish the game and enjoy it
-</t>
-  </si>
-  <si>
-    <t>Year selector, tutorial, intro, Map/characters, storyline/quests. This is a substantial piece of work
-See Google Keep notes</t>
-  </si>
-  <si>
     <t>15 - 120 Attempted to make game playable by changing sound effects, realized will be unplayble until inbetween build, layed game without secrets to look for feedback and balance (file called Doug for Alpha0.29, made file in balance folder, Added last things from google keep notes</t>
   </si>
   <si>
-    <t>Classes, object methods, how map works, commenting code. Updating to python 3. Interactables class. Buildings as an entity.
-PP8 style using PyCharm
-Get rid of global variables and restructure code
-Using and understanding effecient python code chunks (See Liam F. and his book)
-Make an entity class (name, description, location, stats, health, item need, item give, inventory, deathtext, etc) and then all subclasses  using inheritance
-Entity
+    <t>People who like being involved w. development and feedback, like to play updates</t>
+  </si>
+  <si>
+    <t>Early acess, easy to follow along, easy to update and keep save files</t>
+  </si>
+  <si>
+    <t>15 ?</t>
+  </si>
+  <si>
+    <t>0.36</t>
+  </si>
+  <si>
+    <t>Immersive Dynamic world</t>
+  </si>
+  <si>
+    <t>RPGers, readers</t>
+  </si>
+  <si>
+    <t>Full fleshed, easy to change for settings</t>
+  </si>
+  <si>
+    <t>Anyone who wants to setup perfect</t>
+  </si>
+  <si>
+    <t>BD, 12?</t>
+  </si>
+  <si>
+    <t>Easy for new players old alike</t>
+  </si>
+  <si>
+    <t>A new or old player</t>
+  </si>
+  <si>
+    <t>Immersed Economy</t>
+  </si>
+  <si>
+    <t>RPGers, economists</t>
+  </si>
+  <si>
+    <t>Boss balance</t>
+  </si>
+  <si>
+    <t>Challenging but not punishing</t>
+  </si>
+  <si>
+    <t>People who don't mind a challenge</t>
+  </si>
+  <si>
+    <t>Balanced and nice to play in many parallel ways</t>
+  </si>
+  <si>
+    <t>Immersive</t>
+  </si>
+  <si>
+    <t>0.33?</t>
+  </si>
+  <si>
+    <t>Boss Balance</t>
+  </si>
+  <si>
+    <t>Game for all people, returning or new</t>
+  </si>
+  <si>
+    <t>People who like a challenge</t>
+  </si>
+  <si>
+    <t>0.36?</t>
+  </si>
+  <si>
+    <t>Lots of endgame content</t>
+  </si>
+  <si>
+    <t>Collectors/maxers</t>
+  </si>
+  <si>
+    <t>Completionists</t>
+  </si>
+  <si>
+    <t>0.37 ?</t>
+  </si>
+  <si>
+    <t>Rewarding for going along progress, collectable</t>
+  </si>
+  <si>
+    <t>0.38</t>
+  </si>
+  <si>
+    <t>Spooky</t>
+  </si>
+  <si>
+    <t>Immersive, like people</t>
+  </si>
+  <si>
+    <t>Creative Mode</t>
+  </si>
+  <si>
+    <t>0.37?</t>
+  </si>
+  <si>
+    <t>Fix Description List</t>
+  </si>
+  <si>
+    <t>Breakdown big ones</t>
+  </si>
+  <si>
+    <t>Compile big list</t>
+  </si>
+  <si>
+    <t>Put priorties/finish list</t>
+  </si>
+  <si>
+    <t>Integrate bug/must have from feedback</t>
+  </si>
+  <si>
+    <t>Endgame Content</t>
+  </si>
+  <si>
+    <t>Crazy, references</t>
+  </si>
+  <si>
+    <t>0.38?</t>
+  </si>
+  <si>
+    <t>Crazy, creative</t>
+  </si>
+  <si>
+    <t>Anarchists</t>
+  </si>
+  <si>
+    <t>0.35 ?</t>
+  </si>
+  <si>
+    <t>Consequences/acountability for killing</t>
+  </si>
+  <si>
+    <t>Survivalists</t>
+  </si>
+  <si>
+    <t>GUI, Text display</t>
+  </si>
+  <si>
+    <t>Beautiful, bright, contrast</t>
+  </si>
+  <si>
+    <t>People who like seeing things</t>
+  </si>
+  <si>
+    <t>0.39?</t>
+  </si>
+  <si>
+    <t>0.40?</t>
+  </si>
+  <si>
+    <t>0.42?</t>
+  </si>
+  <si>
+    <t>Hollywood House</t>
+  </si>
+  <si>
+    <t>Lots of inside references</t>
+  </si>
+  <si>
+    <t>30?</t>
+  </si>
+  <si>
+    <t>Scater Update</t>
+  </si>
+  <si>
+    <t>Integrate into other things</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Someone who likes text adventures</t>
+  </si>
+  <si>
+    <t>My pride work shown everywhere</t>
+  </si>
+  <si>
+    <t>Immersive world with lots of areas</t>
+  </si>
+  <si>
+    <t>Eng Phys, survalists</t>
+  </si>
+  <si>
+    <t>20?</t>
+  </si>
+  <si>
+    <t>GTA police</t>
+  </si>
+  <si>
+    <t>Crazy, lots of content</t>
+  </si>
+  <si>
+    <t>15?</t>
+  </si>
+  <si>
+    <t>Minigame/fighting challenge</t>
+  </si>
+  <si>
+    <t>Fighters</t>
+  </si>
+  <si>
+    <t>Me</t>
+  </si>
+  <si>
+    <t>For Myself</t>
+  </si>
+  <si>
+    <t>Looking to grow</t>
+  </si>
+  <si>
+    <t>People who want community/involvement</t>
+  </si>
+  <si>
+    <t>Artwork/title screens</t>
+  </si>
+  <si>
+    <t>30 ?</t>
+  </si>
+  <si>
+    <t>Open to all People</t>
+  </si>
+  <si>
+    <t>Mac Eng Students</t>
+  </si>
+  <si>
+    <t>Google Maps Import</t>
+  </si>
+  <si>
+    <t>10 ?</t>
+  </si>
+  <si>
+    <t>Zombie Lovers</t>
+  </si>
+  <si>
+    <t>Games/projects need synthergy to be more than the sum of their parts</t>
+  </si>
+  <si>
+    <t>Layout roadmap/plan document</t>
+  </si>
+  <si>
+    <t>Darkness lovers</t>
+  </si>
+  <si>
+    <t>Minigames, crazyness</t>
+  </si>
+  <si>
+    <t>Megan Goodland, Farmers</t>
+  </si>
+  <si>
+    <t>Endgame/many ways to play</t>
+  </si>
+  <si>
+    <t>20 ?</t>
+  </si>
+  <si>
+    <t>16 - X</t>
+  </si>
+  <si>
+    <t>17 - 45 finished feature lock list, needs descr. Cleanup, feedback, and review</t>
+  </si>
+  <si>
+    <t>Would like to finish feature lock at least and get into breakdown</t>
+  </si>
+  <si>
+    <t>Breakdown</t>
+  </si>
+  <si>
+    <t>Feature lock release Oct 1?</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Maybe consider doing half release with all mechanics then rest of 2019 Kipling in the (maybe 0.30.0 and 0.30.5 or just 0.30 and 0.31)</t>
+  </si>
+  <si>
+    <t>Item/Player Attributes</t>
+  </si>
+  <si>
+    <t>* Classes, object methods, how map works (numbered adjacency lists), commenting code. Updating to python 3. Interactables class. Buildings as an entity.
+* PP8 style using PyCharm
+* Get rid of global variables and restructure code
+* Using and understanding effecient python code chunks (See Liam F. and his book)
+* Make an entity class (name, description, location, stats, health, item need, item give, inventory, deathtext, etc) and then all subclasses  using inheritance
+* Entity
      Person(each has same attributes and stuff, even schedule would be the same)
           Boss?
      Place
@@ -946,359 +1044,375 @@
           Interactable can go, just add a moveable flag to items with new entity structute that allows give/take</t>
   </si>
   <si>
-    <t>A way to make game update automatically is with an update launcher. Only if not going online</t>
-  </si>
-  <si>
-    <t>People who like being involved w. development and feedback, like to play updates</t>
-  </si>
-  <si>
-    <t>Early acess, easy to follow along, easy to update and keep save files</t>
-  </si>
-  <si>
-    <t>15 ?</t>
-  </si>
-  <si>
-    <t>Adding different weather changes, debufs, and envoirnment to keep up emersion</t>
-  </si>
-  <si>
-    <t>0.36</t>
-  </si>
-  <si>
-    <t>Immersive Dynamic world</t>
-  </si>
-  <si>
-    <t>RPGers, readers</t>
-  </si>
-  <si>
-    <t>Full fleshed, easy to change for settings</t>
-  </si>
-  <si>
-    <t>In GUI window have options to save/load game, pause, volume settings, window size, text size, colour settings maybe?
-These settings are saved locally to the game file</t>
-  </si>
-  <si>
-    <t>Anyone who wants to setup perfect</t>
-  </si>
-  <si>
-    <t>BD, 12?</t>
-  </si>
-  <si>
-    <t>Easy for new players old alike</t>
-  </si>
-  <si>
-    <t>A new or old player</t>
-  </si>
-  <si>
-    <t>Immersed Economy</t>
-  </si>
-  <si>
-    <t>RPGers, economists</t>
-  </si>
-  <si>
-    <t>People drop money/you can make money
-Petter is a seller and you can buy Marvin the Martian thing
-Can drop a little bit from cops but not too much to farm
-Investing in stocks
-Grand exchange for items</t>
-  </si>
-  <si>
-    <t>Boss balance</t>
-  </si>
-  <si>
-    <t>Making sure all bosses are beatable without secrets so at least not frustrating for new players</t>
-  </si>
-  <si>
-    <t>Challenging but not punishing</t>
-  </si>
-  <si>
-    <t>People who don't mind a challenge</t>
-  </si>
-  <si>
-    <t>Balanced and nice to play in many parallel ways</t>
-  </si>
-  <si>
-    <t>Immersive</t>
-  </si>
-  <si>
-    <t>0.33?</t>
-  </si>
-  <si>
-    <t>Boss Balance</t>
-  </si>
-  <si>
-    <t>Easy, Medium, Hard, Ironman verson where can't heal/carry more than you can. Maybe all with different endings.
-Easy-medium-Hardcore modes where you have 1. map w. quest outline (maybe a box?) - exploitable map/looking - no map  2. Enemy difficulty 3. Item outlines? 4. No eating 5. Full inventory vs expandable vs just you?
-Try not to do just simple health/attack scaling. Maybe add new mechanics</t>
-  </si>
-  <si>
-    <t>Game for all people, returning or new</t>
-  </si>
-  <si>
-    <t>People who like a challenge</t>
-  </si>
-  <si>
-    <t>0.36?</t>
-  </si>
-  <si>
-    <t>Lots of endgame content</t>
-  </si>
-  <si>
-    <t>Collectors/maxers</t>
-  </si>
-  <si>
-    <t>Completionists</t>
-  </si>
-  <si>
-    <t>0.37 ?</t>
-  </si>
-  <si>
-    <t>Rewarding for going along progress, collectable</t>
-  </si>
-  <si>
-    <t>0.38</t>
-  </si>
-  <si>
-    <t>Spooky</t>
-  </si>
-  <si>
-    <t>Immersive, like people</t>
-  </si>
-  <si>
-    <t>Creative Mode</t>
-  </si>
-  <si>
-    <t>0.37?</t>
-  </si>
-  <si>
-    <t>Fix Description List</t>
-  </si>
-  <si>
-    <t>Breakdown big ones</t>
-  </si>
-  <si>
-    <t>Compile big list</t>
-  </si>
-  <si>
-    <t>Put priorties/finish list</t>
-  </si>
-  <si>
-    <t>Integrate bug/must have from feedback</t>
-  </si>
-  <si>
-    <t>Endgame Content</t>
-  </si>
-  <si>
-    <t>Crazy, references</t>
-  </si>
-  <si>
-    <t>0.38?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Building and all things are breakable/fightable/destroyable.
-When things break the items/characters get put on main floor but dead, interrior destroyed, </t>
-  </si>
-  <si>
-    <t>Make a basic interrior of bsb and fully test. Then make all multilevel buildings an interrior</t>
-  </si>
-  <si>
-    <t>Crazy, creative</t>
-  </si>
-  <si>
-    <t>Anarchists</t>
-  </si>
-  <si>
-    <t>0.35 ?</t>
-  </si>
-  <si>
-    <t>Consequences/acountability for killing</t>
-  </si>
-  <si>
-    <t>Survivalists</t>
-  </si>
-  <si>
-    <t>GUI, Text display</t>
-  </si>
-  <si>
-    <t>Beautiful, bright, contrast</t>
-  </si>
-  <si>
-    <t>People who like seeing things</t>
-  </si>
-  <si>
-    <t>0.39?</t>
-  </si>
-  <si>
-    <t>0.40?</t>
-  </si>
-  <si>
-    <t>0.42?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Involves lore from the skate video
+    <t>* Make PAP unlock when you get to end of game
+* Unlocked by finishing all of the game
+* Sound of lightening
+ * followed by the sounds of cowboys
+* Looks like you need to give something to get something in return
+* PAP EXP level</t>
+  </si>
+  <si>
+    <t>* Make a basic interrior of bsb and fully test. 
+* Then make all multilevel buildings an interrior</t>
+  </si>
+  <si>
+    <t>* Adding your dad, Alex Jones, Arnold, Jesse Ventura, auto turrets etc, harry potter ring that can talk to the dead
+* Even more secret place under okons storage place. Leads to underground base.
+* Mike the liar random event. Running across campus saying stuff. Comments on 4th wall things about the game ex) "They need an autocomplete"
+* Stackable Visor Glasses
+* Brendan's jacket holds things in the game
+scuba Steve (and it's Haugen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Adding explinations to all jokes and inside things to keep game relavent. Not sure if this would take away from game OR if you would only play the year you have it. Idk.
+* When characters die they drop bio cheet and what their interests are (credits like a great help for devloping game)
+* Add better biosheet, description of items to explain jokes, a tutorial, and more help to have players finish the game and enjoy it
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Adding an experience level to the game and mobs that respawn so you feel like you're progressing. Probably buffs stats and helps you beat higher level people/things. Also the respawn with golden gauntlet thanos for Paul the buss driver.
+* In general, have more crazy/dangerous things happen as you progress in quests/storyline (sand worms pop up, idk, crazyness)
+* Could have random drop loot
+* Having fire with cooking be able to cook multiple types of foods (Eggs, meat, bread, ) with BOTW sound
+* Having more combinations of cooking food
+* Having more Runescape cooking, experience levels to unlock/burn less, burn levels, etc
+</t>
+  </si>
+  <si>
+    <t>* Make game run in javascript/whatever online so you can play game online. 
+* Also has QT scoreboard so more compeditive</t>
+  </si>
+  <si>
+    <t>* Make other players be able to interact, fight, talk to eachother</t>
+  </si>
+  <si>
+    <t>* See 13 Hollywood Productions March 7th large section of ideas.
+* Make combat more turn based with actions, reactions, preps, combos, etc.  
+* Maybe some skill involved? 
+* Mashing a key to beat someone.
+*  At least for now someone comes back for round two.
+* Every Person has their own weakness/strengths.
+* Use Darksouls style damage system
+* Bullet time</t>
+  </si>
+  <si>
+    <t>* Adding time to game. 
+* Either BOTW 2 min for 1 hr with longest day, or minecraft. I don't think ever step 5 minutes. 
+* Maybe watch system
+* time based events, 
+* time based characters/moving, etc. 
+* Starting day is 12pm, day after Kipling (for 2017-2018 version).
+* For 2019 version make so have at least a week before kipling</t>
+  </si>
+  <si>
+    <t>BD, 15+10+8+15+20?</t>
+  </si>
+  <si>
+    <t>* Making so save/load and all personal game data is kept safe and unhackable 
+* Also probably encrypted is better for online pins, etc</t>
+  </si>
+  <si>
+    <t>* Making so surroundings of obveous areas print out. 
+* Have lore print first and then title+search around you.</t>
+  </si>
+  <si>
+    <t>* Can add content to game and make their own quests/stories. 
+* Maybe unlocks when you beat the game.
+* Save files need to be able to recompile after adding items
+* Able to add items, quests, people, change descriptions, etc
+* Almost like scripting tools within the game
+* Maybe make a set of mod tools with the game? Maybe those are Excel Sheets?</t>
+  </si>
+  <si>
+    <t>* Move map to right side GUI.
+* Map display better
+* quest tracker, can give hints on where to go/where things are
+* Ingame journal or notes function.</t>
+  </si>
+  <si>
+    <t>* Mini-gamers around area. Not made by me but implemented.
+* pong 
+* chess (Mitch is always there) 
+* tetris (Zac introduces you)
+* Zork
+* watching Ascii new hope
+* Classic riddles/storries (goat, chicken, fox)
+* Liars Dice (SP or MP) Tyler and Angus in full pirate gear, Hani is part of the wall (part of the ship part of the crew (the Die is cast and Davy Jones is there as well )</t>
+  </si>
+  <si>
+    <t>* Use google maps data to design exteriors/interriors for things</t>
+  </si>
+  <si>
+    <t>* Make so it takes files automatically
+* gives icon automatically 
+* does code checks out 
+* installer gives desktop icon
+* Overwriting old instal to update would be nice.</t>
+  </si>
+  <si>
+    <t>* In GUI window have options to save/load game, pause, volume settings, window size, text size, colour settings maybe?
+* These settings are saved locally to the game file</t>
+  </si>
+  <si>
+    <t>* Start player in secluded area/small island to get a sense but still have tutorial
+* First 5 minutes set tone of the game, set expectations and colour whole experience. 
+* 3ways to draw in (best have at least 2 of these and multiple intros)
+* 1. Sell you with the narrative 2. Wow you with the mechanics 3. Draw you in with the spectacle
+* Mystery is a great tool for hooking someone. Can also sell the world  (put what is compelling in there and don't hold back)
+* Deliver why player would want to play the game and deliver in 1st 5 minute (don't even have to take away powers). 
+* Shouldn't front load tutorial either. They simplified it
+* Start with spectacular or novel. Can throw into a story already in progress (in medius res)</t>
+  </si>
+  <si>
+    <t>* People drop money/you can make money
+* Petter is a seller and you can buy Marvin the Martian thing
+* Can drop a little bit from cops but not too much to farm
+* Investing in stocks that are real and pulled from an API
+* Grand exchange for items</t>
+  </si>
+  <si>
+    <t>*Adding different weather changes
+* debufs
+* envoirnment to keep up emersion
+* Pulling realworld weather and weather predictions from an API</t>
+  </si>
+  <si>
+    <t>* Attack and defense, speed doesn't do anything. 
+* Would need to be be after combat update. 
+* Possibly have star/some sort of indicator for bosses OR have the indicator just be how hard they can hit you/how big they are
+* More direct reward for exploration with something that ties back into game (like BOTW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Do more with name including character address you by name and work with names including name infulence. </t>
+  </si>
+  <si>
+    <t>* Easy, Medium, Hard, Ironman verson where can't heal/carry more than you can
+* Maybe all with different endings
+* Easy-medium-Hardcore modes where you have 
+1. map w. quest outline (maybe a box?) - exploitable map/looking - no map  
+2. Enemy difficulty 
+3. Item outlines? 
+4. No eating 
+5. Full inventory vs expandable vs just you?
+* Try not to do just simple health/attack scaling. Maybe add new mechanics</t>
+  </si>
+  <si>
+    <t>* Items can give Flying, Electricity, crafting, survival, weight, volume stored
+* Water, food, and stanima for player
+* Being able to carry more things or have Backbacks
+* Including Iron man suit with Energy, craftables and consumables with energy. 
+* Secret weird flying place/base. Secret places you can only get to by flying into upper buildings
+* You can fly up too far and fly out of the game</t>
+  </si>
+  <si>
+    <t>* Keep track of all items/things collected
+* Steam/platinum trophies</t>
+  </si>
+  <si>
+    <t>* Make facebook, twitter, website, instagram outreach and update to keep players/community involved and invite new players
+* Put game on steam</t>
+  </si>
+  <si>
+    <t>* Ritual gone wrong that spawns dumb undead things at night. Ritual involves turning Casion calculator into the other.
+* If you go to edge and press side 1000(50) times you go around to the other edge
+* Pressing down 420 times in a certain place sents you to hell and you fight satan, and Bezabad plays.
+* You can also sumon Satan to get the joint of destiny
+* Teachers come back to life and you can kill zombie versions of them
+* Maybe involve kathulu</t>
+  </si>
+  <si>
+    <t>* They move around
+* Have  a companion
+* Can equip items to yourself to store for later games so they act as a companion.</t>
+  </si>
+  <si>
+    <t>* Sling ring, teliport anywhere you know
+* Portal gun
+* Teliport anywhere you can see
+* Instant transmission (anything)
+* Zombies teliporter (where another one is but also in time)
+* Star Trek teliport (anywhere but only to/from consol).</t>
+  </si>
+  <si>
+    <t>* Building and all things are breakable/fightable/destroyable.
+* When things break the items/characters get put on main floor but dead, interrior destroyed
+* Blowing up building calls to police</t>
+  </si>
+  <si>
+    <t>* Star level where police come after you, eventually SWAT
+* eventually have to escape on rocket in smoke stack to go meet Elon musk on the moon</t>
+  </si>
+  <si>
+    <t>* GUI text printer, change colour, font, style of words to highlight.</t>
+  </si>
+  <si>
+    <t>* Involves lore from the skate video
 . You see a campus police guard pull up to talk to someone on the skateboard.
 "Erik the Sk8r: Hey Bill"
 "Bill the Mac Cop: Hey Erik, you know you can't be here right?"
 "Bill: Comomon man we do this every day"
 "Erik: Okay then, see you tomorrow!"
 He scates off quickly up 
-"Bill the Mac Cop: You can't skate on campus prop... aww whatever."
+"Bill the Mac Cop: You can't skate on campus prop... aww whatever."</t>
+  </si>
+  <si>
+    <t>* Hollywood Murder Mystery. All aspects and functions of hollywood
+* Have to fight the racoons</t>
+  </si>
+  <si>
+    <t>* Phil clones himself to make it more efficient but gets out of control
+* Have to fight off all ranges of Phils
+* Only way to kill them is to poisen cafine supply into the school
+* So only drunk Phil remains</t>
+  </si>
+  <si>
+    <t>* Fight combatants against eachother (including different Phils).
+* Can also fight in it yourself to go up ranks</t>
+  </si>
+  <si>
+    <t>* You teliport to green lake, explore all the mysteries of Brendan Fallon's past and life
+* See update notes</t>
+  </si>
+  <si>
+    <t>* Expand Map to whole school
+* make a storyline containing first year eng experience and classes</t>
+  </si>
+  <si>
+    <t>* Just bassically Nazi Zombies mode
+* Wunderwaffe DG-2  1000, 100, -10
+*  Chain lightning! 115 not included</t>
+  </si>
+  <si>
+    <t>* Real life farming times for best weapons
+* Every 1/20 pumpkin gives mutated Wunder pumpkin which is best headgear
+* Because it's better reactor it's mutated
+* If creating long term things need to have good, stable, encrypted save files that can be updated with version
+* Create element 420 in the reactor to make wonder weapons</t>
+  </si>
+  <si>
+    <t>* Matlab 
+* HFF 2020
+* any other game I make</t>
+  </si>
+  <si>
+    <t>* Having a ascii art converter and font typing creator
+* making a cover picture
+* having all the pictures of stuff in game</t>
+  </si>
+  <si>
+    <t>Text/Grammar/Naming</t>
+  </si>
+  <si>
+    <t>Short word for verbs,  for inv, s for stats</t>
+  </si>
+  <si>
+    <t>* Make keywords shorter, have list of items to choose from quickly [1-2], maybe accept short names? 
+* Maybe take cardinal coords. 
+* More things rather than equip. 
+* Also possibly controller support?
+* Short word for verbs,  for inv, s for stats</t>
+  </si>
+  <si>
+    <t>Angus, Beef, Barber ("Call me a liar")</t>
+  </si>
+  <si>
+    <t>Map/Items/People</t>
+  </si>
+  <si>
+    <t>I kinda disagree with this one for now. Don't think it should autosave</t>
+  </si>
+  <si>
+    <t>* A way to make game update automatically is with an update launcher
+* Only if not going online
+* Auto save every once and a while</t>
+  </si>
+  <si>
+    <t>* Making sure all bosses are beatable without secrets so at least not frustrating for new players
+* See balance metrics from balance sheet
+* Maybe only have saving and autosaving as a developer.</t>
+  </si>
+  <si>
+    <t>* Adding map and all suplementary info to the GUI (maybe whole game?) so we can customize content. 
+* IDK. I like idea of two window system with map, player icon, pictures, etc on side. 
+* Size of window (ascii art print)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Spelling and grammar check before release (maybe needs a text output function)
+* Don't except empty name
+* "B is back" (Zac)
+* "Dell, Intel Inside"
+* search keyword for search
 </t>
   </si>
   <si>
-    <t>Hollywood House</t>
-  </si>
-  <si>
-    <t>Lots of inside references</t>
-  </si>
-  <si>
-    <t>30?</t>
-  </si>
-  <si>
-    <t>Scater Update</t>
-  </si>
-  <si>
-    <t>Hollywood Murder Mystery. All aspects and functions of hollywood</t>
-  </si>
-  <si>
-    <t>Integrate into other things</t>
-  </si>
-  <si>
-    <t>Matlab, HFF 2020, any other game I make</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Someone who likes text adventures</t>
-  </si>
-  <si>
-    <t>My pride work shown everywhere</t>
-  </si>
-  <si>
-    <t>Immersive world with lots of areas</t>
-  </si>
-  <si>
-    <t>Eng Phys, survalists</t>
-  </si>
-  <si>
-    <t>Phil clones himself to make it more efficient but gets out of control
-Have to fight off all ranges of Phils
-Only way to kill them is to poisen cafine supply into the school. So only drunk Phil remains</t>
-  </si>
-  <si>
-    <t>20?</t>
-  </si>
-  <si>
-    <t>GTA police</t>
-  </si>
-  <si>
-    <t>Crazy, lots of content</t>
-  </si>
-  <si>
-    <t>Fight combatants against eachother (including different Phils).
-Can also fight in it yourself</t>
-  </si>
-  <si>
-    <t>15?</t>
-  </si>
-  <si>
-    <t>Minigame/fighting challenge</t>
-  </si>
-  <si>
-    <t>Fighters</t>
-  </si>
-  <si>
-    <t>Me</t>
-  </si>
-  <si>
-    <t>You teliport to green lake, explore all the mysteries of Brendan Fallon's past and life</t>
-  </si>
-  <si>
-    <t>For Myself</t>
-  </si>
-  <si>
-    <t>Looking to grow</t>
-  </si>
-  <si>
-    <t>People who want community/involvement</t>
-  </si>
-  <si>
-    <t>Artwork/title screens</t>
-  </si>
-  <si>
-    <t>Having a ascii art converter and font typing creator, making a cover picture, having all the pictures of stuff in game</t>
-  </si>
-  <si>
-    <t>30 ?</t>
-  </si>
-  <si>
-    <t>Make facebook, twitter, website, instagram outreach and update to keep players/community involved and invite new players</t>
-  </si>
-  <si>
-    <t>Open to all People</t>
-  </si>
-  <si>
-    <t>Mac Eng Students</t>
-  </si>
-  <si>
-    <t>Expand Map to whole school, make a storyline containing first year eng experience</t>
-  </si>
-  <si>
-    <t>Google Maps Import</t>
-  </si>
-  <si>
-    <t>10 ?</t>
-  </si>
-  <si>
-    <t>Zombie Lovers</t>
-  </si>
-  <si>
-    <t>Games/projects need synthergy to be more than the sum of their parts</t>
-  </si>
-  <si>
-    <t>Layout roadmap/plan document</t>
-  </si>
-  <si>
-    <t>Darkness lovers</t>
-  </si>
-  <si>
-    <t>Ritual gone wrong that spawns dumb undead things at night. 
-Ritual involves turning Casion calculator into the other.
-If you go to edge and press side 1000(50) times you go around to the other edge
-Pressing down 420 times in a certain place sents you to hell and you fight satan, and Bezabad plays.
-You can also sumon Satan to get the joint of destiny
-Teachers come back to life and you can kill zombie versions of them
-Maybe involve kathulu</t>
-  </si>
-  <si>
-    <t>Minigames, crazyness</t>
-  </si>
-  <si>
-    <t>Megan Goodland, Farmers</t>
-  </si>
-  <si>
-    <t>Endgame/many ways to play</t>
-  </si>
-  <si>
-    <t>20 ?</t>
-  </si>
-  <si>
-    <t>16 - X</t>
-  </si>
-  <si>
-    <t>17 - 45 finished feature lock list, needs descr. Cleanup, feedback, and review</t>
-  </si>
-  <si>
-    <t>Would like to finish feature lock at least and get into breakdown</t>
-  </si>
-  <si>
-    <t>Breakdown</t>
-  </si>
-  <si>
-    <t>Feature lock release Oct 1?</t>
-  </si>
-  <si>
-    <t>Total</t>
+    <t>*Year selector
+* tutorial
+* intro
+* Map/characters ( Measure Alice or Bob &amp; they collapse, also DOD)
+* BSB Dungeon
+* storyline/quests. This is a substantial piece of work
+* See Google Keep notes on the story</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Queues</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>* When you inspect the car it says 'Ya thought these were the keys"
+* When you searching when nothings there "You double take and there's still nothing there" (If you search 20 times you die)</t>
+  </si>
+  <si>
+    <t>SharpExchange</t>
+  </si>
+  <si>
+    <t>* Right now defense is v important but with healing items added this should fix it
+* Better head items plz
+* Need story arc for body armour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Need to know that Jana has the textbook, maybe the story should say that somewhere
+* Not obveous that equip means to pick up
+* Phil says that need to be pushed more toward the Phenoix (more people you talk to, or items, tell story about the Phoneix)
+</t>
+  </si>
+  <si>
+    <t>More use of storyline, music, definition to people to give realism to the world</t>
+  </si>
+  <si>
+    <t>Put into feature lock</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Have Brendan Fallon character with eclipse mug, rocketry t-shirt, Strainer on head?SafetyGlasses?, and iron ring (more characters)</t>
+  </si>
+  <si>
+    <t>Easier way to access game, not just goo.gl/iK8dL9 (Website maybe)</t>
+  </si>
+  <si>
+    <t>* Allow Sounds to play
+* transitions and have 
+* different music for different settings
+* Belzabad plays when you fight kleiman
+* Channel Orange by Frank Ocean</t>
+  </si>
+  <si>
+    <t>* Error checking to see if place exists before moving
+* Wear earphones on head
+* 3W text in QT
+* Add Nicole to EP office
+* Wacky items are good
+* 3BB PID with MSP430
+* Have Brendan Fallon character with eclipse mug, rocketry t-shirt, Strainer on head?SafetyGlasses?, and iron ring (more characters)</t>
+  </si>
+  <si>
+    <t>18 - 90 Cleaned up features list, started going through and combining with feedback</t>
   </si>
 </sst>
 </file>
@@ -1378,7 +1492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1411,11 +1525,79 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1426,6 +1608,44 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H51" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:H51"/>
+  <sortState ref="A2:H51">
+    <sortCondition ref="B1:B51"/>
+  </sortState>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Feedback" dataDxfId="6"/>
+    <tableColumn id="2" name="Priority" dataDxfId="5"/>
+    <tableColumn id="3" name="Links"/>
+    <tableColumn id="4" name="When Reported (update)"/>
+    <tableColumn id="5" name="Est Implement Time (hrs)"/>
+    <tableColumn id="6" name="Description (64 char max)"/>
+    <tableColumn id="7" name="Details"/>
+    <tableColumn id="8" name="What kind of game it makes (who)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:I56" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A4:I56"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Feature"/>
+    <tableColumn id="2" name="0.30 Priority" dataDxfId="3"/>
+    <tableColumn id="3" name="Links"/>
+    <tableColumn id="4" name="Est Implement Time (hrs)"/>
+    <tableColumn id="5" name="Description (64 char max)"/>
+    <tableColumn id="6" name="Details" dataDxfId="2"/>
+    <tableColumn id="7" name="When to implement(update)" dataDxfId="1"/>
+    <tableColumn id="8" name="What kind of game it makes "/>
+    <tableColumn id="9" name="Who would play this game"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1693,8 +1913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1729,7 +1949,7 @@
         <v>14</v>
       </c>
       <c r="J7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1740,62 +1960,62 @@
         <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" t="s">
         <v>91</v>
       </c>
-      <c r="B9" t="s">
+      <c r="E9" t="s">
         <v>92</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
         <v>93</v>
       </c>
-      <c r="D9" t="s">
+      <c r="G9" t="s">
         <v>94</v>
       </c>
-      <c r="E9" t="s">
-        <v>95</v>
-      </c>
-      <c r="F9" t="s">
-        <v>96</v>
-      </c>
-      <c r="G9" t="s">
-        <v>97</v>
-      </c>
       <c r="H9" t="s">
-        <v>397</v>
+        <v>329</v>
       </c>
       <c r="I9" s="9">
         <v>45</v>
       </c>
       <c r="J9" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C10" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D10" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="E10" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="F10" t="s">
-        <v>273</v>
+        <v>231</v>
       </c>
       <c r="G10" t="s">
-        <v>286</v>
+        <v>237</v>
       </c>
       <c r="H10">
         <v>330</v>
@@ -1803,80 +2023,80 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>392</v>
+        <v>324</v>
       </c>
       <c r="B11" t="s">
-        <v>393</v>
+        <v>325</v>
       </c>
       <c r="C11" t="s">
+        <v>401</v>
+      </c>
+      <c r="D11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" t="s">
         <v>101</v>
       </c>
-      <c r="D11" t="s">
-        <v>102</v>
-      </c>
-      <c r="E11" t="s">
-        <v>103</v>
-      </c>
-      <c r="F11" t="s">
-        <v>104</v>
-      </c>
-      <c r="G11" t="s">
-        <v>105</v>
-      </c>
       <c r="I11" t="s">
-        <v>394</v>
+        <v>326</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E12" t="s">
         <v>106</v>
       </c>
-      <c r="B12" t="s">
+      <c r="F12" t="s">
         <v>107</v>
       </c>
-      <c r="C12" t="s">
+      <c r="G12" t="s">
         <v>108</v>
       </c>
-      <c r="D12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E12" t="s">
-        <v>110</v>
-      </c>
-      <c r="F12" t="s">
-        <v>111</v>
-      </c>
-      <c r="G12" t="s">
-        <v>112</v>
-      </c>
       <c r="I12" t="s">
-        <v>395</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E13" t="s">
         <v>113</v>
       </c>
-      <c r="B13" t="s">
+      <c r="F13" t="s">
         <v>114</v>
       </c>
-      <c r="C13" t="s">
+      <c r="G13" t="s">
         <v>115</v>
       </c>
-      <c r="D13" t="s">
-        <v>116</v>
-      </c>
-      <c r="E13" t="s">
-        <v>117</v>
-      </c>
-      <c r="F13" t="s">
-        <v>118</v>
-      </c>
-      <c r="G13" t="s">
-        <v>119</v>
-      </c>
       <c r="I13" t="s">
-        <v>396</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -1886,16 +2106,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N62"/>
+  <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="7.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="4" max="5" width="25.42578125" customWidth="1"/>
     <col min="6" max="6" width="32.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" customWidth="1"/>
+    <col min="8" max="8" width="33.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1909,29 +2133,29 @@
         <v>22</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="11">
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1947,17 +2171,17 @@
         <v>32</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>33</v>
+        <v>7</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="11">
         <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1973,17 +2197,17 @@
         <v>34</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
+        <v>33</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -1998,18 +2222,18 @@
       <c r="F4" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" t="s">
-        <v>21</v>
+      <c r="J4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2024,18 +2248,18 @@
       <c r="F5" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>18</v>
+      <c r="J5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="11">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2051,17 +2275,17 @@
         <v>27</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2074,14 +2298,20 @@
         <v>0.25</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="11">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -2094,14 +2324,14 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="11">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -2121,7 +2351,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="11">
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -2134,14 +2364,14 @@
         <v>0.75</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>377</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="11">
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2161,7 +2391,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="11">
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2178,7 +2408,7 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="11">
         <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -2195,7 +2425,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="11">
         <v>35</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2208,63 +2438,66 @@
         <v>0.25</v>
       </c>
       <c r="F14" t="s">
-        <v>55</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>36</v>
+      <c r="A15" s="11">
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C15" t="s">
+        <v>396</v>
+      </c>
       <c r="D15">
         <v>0.28000000000000003</v>
       </c>
       <c r="E15">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2</v>
+      <c r="A16" s="11">
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D16">
         <v>0.28000000000000003</v>
       </c>
       <c r="E16">
-        <v>4</v>
-      </c>
-      <c r="F16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>12</v>
+        <v>1.5</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>48</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D17">
-        <v>0.28000000000000003</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E17">
         <v>0.5</v>
       </c>
-      <c r="F17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>15</v>
+      <c r="F17" s="15" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
@@ -2273,35 +2506,32 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
         <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C19" t="s">
-        <v>61</v>
-      </c>
       <c r="D19">
         <v>0.28000000000000003</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="F19" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>30</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
+        <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>17</v>
@@ -2313,32 +2543,35 @@
         <v>2</v>
       </c>
       <c r="F20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>31</v>
+        <v>35</v>
+      </c>
+      <c r="G20" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D21">
         <v>0.28000000000000003</v>
       </c>
       <c r="E21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>32</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>30</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>17</v>
@@ -2347,32 +2580,35 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E22">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>33</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <v>31</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
       <c r="D23">
         <v>0.28000000000000003</v>
       </c>
       <c r="E23">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>34</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
+        <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>17</v>
@@ -2384,89 +2620,92 @@
         <v>0.5</v>
       </c>
       <c r="F24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>16</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" t="s">
-        <v>61</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>33</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D25">
         <v>0.28000000000000003</v>
       </c>
       <c r="E25">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="F25" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
+        <v>34</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="D26">
         <v>0.28000000000000003</v>
       </c>
       <c r="E26">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F26" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>4</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>14</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="19">
+        <v>36</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>387</v>
       </c>
       <c r="D27">
-        <v>0.28000000000000003</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E27">
-        <v>1.5</v>
+        <v>6</v>
       </c>
       <c r="F27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>28</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" t="s">
-        <v>64</v>
+        <v>387</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="19">
+        <v>38</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D28">
         <v>0.28000000000000003</v>
       </c>
       <c r="E28">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="F28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>1</v>
+        <v>389</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="19">
+        <v>40</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D29">
         <v>0.28000000000000003</v>
@@ -2475,94 +2714,103 @@
         <v>5</v>
       </c>
       <c r="F29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>9</v>
+        <v>394</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="19">
+        <v>42</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D30">
-        <v>0.28000000000000003</v>
+        <v>0.27</v>
       </c>
       <c r="E30">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="F30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>20</v>
+        <v>391</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="19">
+        <v>44</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D31">
         <v>0.28000000000000003</v>
       </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
       <c r="F31" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>22</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="19">
+        <v>45</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D32">
         <v>0.28000000000000003</v>
       </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
       <c r="F32" t="s">
-        <v>42</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>23</v>
+      <c r="A33" s="19">
+        <v>50</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D33">
-        <v>0.28000000000000003</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E33">
-        <v>3</v>
-      </c>
-      <c r="F33" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>25</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D34">
         <v>0.28000000000000003</v>
       </c>
+      <c r="E34">
+        <v>1.5</v>
+      </c>
       <c r="F34" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>26</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D35">
         <v>0.28000000000000003</v>
@@ -2571,255 +2819,391 @@
         <v>4</v>
       </c>
       <c r="F35" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>27</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C36" t="s">
-        <v>63</v>
+        <v>17</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D36">
         <v>0.28000000000000003</v>
       </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
       <c r="F36" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>29</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>15</v>
+        <v>28</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D37">
         <v>0.28000000000000003</v>
       </c>
       <c r="E37">
+        <v>2.5</v>
+      </c>
+      <c r="F37" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="19">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>388</v>
+      </c>
+      <c r="G38" s="14" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="19">
+        <v>47</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E39" t="s">
+        <v>295</v>
+      </c>
+      <c r="F39" s="15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>9</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+      <c r="F41" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>20</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>22</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F43" t="s">
+        <v>42</v>
+      </c>
+      <c r="G43" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>23</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="F44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>25</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>26</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E46">
         <v>4</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>27</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C47" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="F47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>29</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C48" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+      <c r="F48" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>30</v>
-      </c>
-      <c r="B38" s="1"/>
-      <c r="F38" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="1"/>
-      <c r="F39" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
-      <c r="F40" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
-      <c r="F41" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="1"/>
-      <c r="F42" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="1"/>
-      <c r="F43" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="1"/>
-      <c r="F44" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
-      <c r="G45" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="1"/>
-      <c r="F46" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="1"/>
-      <c r="F47" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
-      <c r="F48" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="1"/>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="19">
+        <v>39</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
       <c r="F49" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="1"/>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="19">
+        <v>41</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E50">
+        <v>5</v>
+      </c>
       <c r="F50" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F51" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F52" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F53" s="15" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F54" s="15" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F55" s="15" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F56" s="15" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F57" s="15" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F58" s="16" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F59" s="15" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F62" t="s">
-        <v>67</v>
-      </c>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="19">
+        <v>49</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="E51" t="s">
+        <v>295</v>
+      </c>
+      <c r="F51" s="16" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F53" s="15"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="11" t="s">
+        <v>395</v>
+      </c>
+      <c r="F54" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F57" s="15"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F50">
-    <sortState ref="A2:E50">
-      <sortCondition ref="B1:B50"/>
-    </sortState>
-  </autoFilter>
   <sortState ref="J2:J6">
     <sortCondition ref="J1"/>
   </sortState>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B37">
+      <formula1>$J$2:$J$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B38:B51">
+      <formula1>$J$2:$J$7</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P63"/>
+  <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" customWidth="1"/>
     <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G4" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O4" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="K4" t="s">
-        <v>59</v>
-      </c>
-      <c r="N4" t="s">
-        <v>77</v>
-      </c>
-      <c r="O4" t="s">
-        <v>76</v>
-      </c>
       <c r="P4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -2830,31 +3214,31 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" t="s">
         <v>83</v>
       </c>
-      <c r="E5" t="s">
+      <c r="I5" t="s">
         <v>82</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="H5" t="s">
-        <v>86</v>
-      </c>
-      <c r="I5" t="s">
-        <v>85</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>7</v>
@@ -2877,19 +3261,19 @@
         <v>1.5</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>283</v>
+        <v>333</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>16</v>
@@ -2915,25 +3299,25 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>121</v>
-      </c>
-      <c r="F7" t="s">
-        <v>336</v>
+        <v>117</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>334</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>13</v>
@@ -2962,19 +3346,19 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>277</v>
+        <v>335</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H8" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="I8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>14</v>
@@ -3003,19 +3387,19 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>284</v>
+        <v>336</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H9" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="I9" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>17</v>
@@ -3041,22 +3425,22 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E10" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>261</v>
+        <v>337</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H10" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I10" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>15</v>
@@ -3082,25 +3466,25 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D11" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" t="s">
-        <v>229</v>
+        <v>58</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>384</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="I11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>11</v>
@@ -3114,28 +3498,28 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E12" t="s">
+        <v>139</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" t="s">
         <v>144</v>
       </c>
-      <c r="E12" t="s">
-        <v>143</v>
-      </c>
-      <c r="F12" t="s">
-        <v>155</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="H12" t="s">
-        <v>148</v>
-      </c>
       <c r="I12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>13</v>
@@ -3149,25 +3533,25 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D13" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E13" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F13" t="s">
-        <v>153</v>
+        <v>339</v>
       </c>
       <c r="G13" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" t="s">
+        <v>148</v>
+      </c>
+      <c r="I13" t="s">
         <v>149</v>
-      </c>
-      <c r="H13" t="s">
-        <v>152</v>
-      </c>
-      <c r="I13" t="s">
-        <v>154</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>17</v>
@@ -3184,17 +3568,17 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>230</v>
-      </c>
-      <c r="F14" t="s">
-        <v>231</v>
+        <v>207</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>378</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="I14" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>14</v>
@@ -3208,22 +3592,22 @@
         <v>15</v>
       </c>
       <c r="D15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" t="s">
+        <v>154</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="H15" t="s">
         <v>161</v>
       </c>
-      <c r="E15" t="s">
-        <v>160</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="G15" s="10" t="s">
+      <c r="I15" t="s">
         <v>162</v>
-      </c>
-      <c r="H15" t="s">
-        <v>168</v>
-      </c>
-      <c r="I15" t="s">
-        <v>169</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>15</v>
@@ -3237,22 +3621,22 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>165</v>
+        <v>342</v>
       </c>
       <c r="E16" t="s">
+        <v>158</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="H16" t="s">
         <v>164</v>
       </c>
-      <c r="F16" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="H16" t="s">
-        <v>172</v>
-      </c>
       <c r="I16" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -3263,25 +3647,25 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>166</v>
-      </c>
-      <c r="F17" t="s">
-        <v>170</v>
+        <v>159</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>399</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H17" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="I17" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -3292,25 +3676,25 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D18">
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>173</v>
-      </c>
-      <c r="F18" t="s">
-        <v>232</v>
+        <v>165</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>341</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H18" t="s">
+        <v>167</v>
+      </c>
+      <c r="I18" t="s">
         <v>175</v>
-      </c>
-      <c r="I18" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -3321,25 +3705,25 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="D19">
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>176</v>
-      </c>
-      <c r="F19" t="s">
-        <v>178</v>
+        <v>168</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>343</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H19" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="I19" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -3353,19 +3737,19 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>180</v>
-      </c>
-      <c r="F20" t="s">
-        <v>236</v>
+        <v>171</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>344</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H20" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="I20" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -3376,22 +3760,22 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E21" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>242</v>
+        <v>345</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="H21" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="I21" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -3401,23 +3785,26 @@
       <c r="B22" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C22" t="s">
+        <v>284</v>
+      </c>
       <c r="D22">
         <v>15</v>
       </c>
       <c r="E22" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>246</v>
+        <v>346</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H22" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="I22" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -3431,19 +3818,19 @@
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>269</v>
+        <v>347</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H23" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="I23" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3454,22 +3841,22 @@
         <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E24" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="F24" t="s">
-        <v>201</v>
+        <v>348</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H24" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="I24" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -3484,19 +3871,19 @@
         <v>4</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -3510,19 +3897,19 @@
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>203</v>
-      </c>
-      <c r="F26" t="s">
-        <v>206</v>
+        <v>193</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>349</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H26" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="I26" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -3532,23 +3919,26 @@
       <c r="B27" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C27" t="s">
+        <v>269</v>
+      </c>
       <c r="D27" t="s">
-        <v>291</v>
+        <v>240</v>
       </c>
       <c r="E27" t="s">
-        <v>274</v>
-      </c>
-      <c r="F27" t="s">
-        <v>288</v>
+        <v>232</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>382</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H27" t="s">
-        <v>290</v>
+        <v>239</v>
       </c>
       <c r="I27" t="s">
-        <v>289</v>
+        <v>238</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -3559,25 +3949,25 @@
         <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D28">
         <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>275</v>
-      </c>
-      <c r="F28" t="s">
-        <v>292</v>
+        <v>233</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>353</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>293</v>
+        <v>241</v>
       </c>
       <c r="H28" t="s">
-        <v>294</v>
+        <v>242</v>
       </c>
       <c r="I28" t="s">
-        <v>295</v>
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -3588,25 +3978,25 @@
         <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>342</v>
+        <v>284</v>
       </c>
       <c r="D29" t="s">
-        <v>291</v>
+        <v>240</v>
       </c>
       <c r="E29" t="s">
-        <v>276</v>
+        <v>234</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>297</v>
+        <v>350</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H29" t="s">
-        <v>296</v>
+        <v>244</v>
       </c>
       <c r="I29" t="s">
-        <v>298</v>
+        <v>245</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -3617,25 +4007,25 @@
         <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D30" t="s">
-        <v>299</v>
+        <v>246</v>
       </c>
       <c r="E30" t="s">
-        <v>271</v>
+        <v>230</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>272</v>
+        <v>351</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>300</v>
+        <v>247</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>301</v>
+        <v>248</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -3649,19 +4039,19 @@
         <v>8</v>
       </c>
       <c r="E31" t="s">
-        <v>266</v>
+        <v>228</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>304</v>
+        <v>352</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>293</v>
+        <v>241</v>
       </c>
       <c r="H31" s="14" t="s">
-        <v>302</v>
+        <v>249</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>303</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -3672,25 +4062,25 @@
         <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="D32">
         <v>12</v>
       </c>
       <c r="E32" t="s">
-        <v>211</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>243</v>
+        <v>200</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>354</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>309</v>
+        <v>254</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3704,19 +4094,19 @@
         <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="F33" t="s">
-        <v>214</v>
+        <v>355</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="H33" s="14" t="s">
-        <v>310</v>
+        <v>255</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3727,25 +4117,25 @@
         <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>312</v>
+        <v>257</v>
       </c>
       <c r="D34">
         <v>16</v>
       </c>
       <c r="E34" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>313</v>
+        <v>356</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>311</v>
+        <v>256</v>
       </c>
       <c r="H34" s="14" t="s">
-        <v>314</v>
+        <v>258</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>315</v>
+        <v>259</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -3759,19 +4149,19 @@
         <v>20</v>
       </c>
       <c r="E35" t="s">
-        <v>217</v>
+        <v>331</v>
       </c>
       <c r="F35" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="H35" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="I35" s="14" t="s">
         <v>262</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="H35" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="I35" s="14" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -3785,19 +4175,19 @@
         <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>233</v>
-      </c>
-      <c r="F36" t="s">
-        <v>247</v>
+        <v>208</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>358</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>320</v>
+        <v>264</v>
       </c>
       <c r="H36" s="14" t="s">
-        <v>321</v>
+        <v>265</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>319</v>
+        <v>263</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -3811,19 +4201,19 @@
         <v>20</v>
       </c>
       <c r="E37" t="s">
-        <v>252</v>
+        <v>217</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>387</v>
+        <v>360</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>322</v>
+        <v>266</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>323</v>
+        <v>267</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>386</v>
+        <v>319</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -3834,25 +4224,25 @@
         <v>17</v>
       </c>
       <c r="C38" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="D38">
         <v>6</v>
       </c>
       <c r="E38" t="s">
-        <v>234</v>
-      </c>
-      <c r="F38" t="s">
-        <v>235</v>
+        <v>209</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>361</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>324</v>
+        <v>268</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -3863,25 +4253,25 @@
         <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>325</v>
+        <v>269</v>
       </c>
       <c r="D39">
         <v>12</v>
       </c>
       <c r="E39" t="s">
-        <v>237</v>
-      </c>
-      <c r="F39" t="s">
-        <v>238</v>
+        <v>210</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>362</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>326</v>
+        <v>270</v>
       </c>
       <c r="H39" s="14" t="s">
-        <v>333</v>
+        <v>277</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>332</v>
+        <v>276</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -3892,25 +4282,25 @@
         <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>325</v>
+        <v>269</v>
       </c>
       <c r="D40">
         <v>20</v>
       </c>
       <c r="E40" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>335</v>
+        <v>363</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>334</v>
+        <v>278</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>337</v>
+        <v>279</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>338</v>
+        <v>280</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -3924,19 +4314,19 @@
         <v>10</v>
       </c>
       <c r="E41" t="s">
-        <v>240</v>
-      </c>
-      <c r="F41" t="s">
-        <v>241</v>
+        <v>212</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>364</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>339</v>
+        <v>281</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>340</v>
+        <v>282</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>341</v>
+        <v>283</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -3950,19 +4340,19 @@
         <v>7</v>
       </c>
       <c r="E42" t="s">
-        <v>244</v>
+        <v>213</v>
       </c>
       <c r="F42" t="s">
-        <v>245</v>
+        <v>365</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H42" s="14" t="s">
-        <v>343</v>
+        <v>285</v>
       </c>
       <c r="I42" s="14" t="s">
-        <v>344</v>
+        <v>286</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3976,19 +4366,19 @@
         <v>10</v>
       </c>
       <c r="E43" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>348</v>
+        <v>366</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>334</v>
+        <v>278</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>350</v>
+        <v>291</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>349</v>
+        <v>290</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3999,25 +4389,25 @@
         <v>15</v>
       </c>
       <c r="C44" t="s">
-        <v>352</v>
+        <v>293</v>
       </c>
       <c r="D44" t="s">
-        <v>351</v>
+        <v>292</v>
       </c>
       <c r="E44" t="s">
-        <v>256</v>
+        <v>221</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>353</v>
+        <v>367</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>334</v>
+        <v>278</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>359</v>
+        <v>298</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -4028,25 +4418,25 @@
         <v>15</v>
       </c>
       <c r="C45" t="s">
-        <v>363</v>
+        <v>301</v>
       </c>
       <c r="D45" t="s">
-        <v>362</v>
+        <v>300</v>
       </c>
       <c r="E45" t="s">
-        <v>257</v>
+        <v>222</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>345</v>
+        <v>287</v>
       </c>
       <c r="H45" s="14" t="s">
-        <v>364</v>
+        <v>302</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>360</v>
+        <v>299</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -4057,22 +4447,22 @@
         <v>15</v>
       </c>
       <c r="D46" t="s">
-        <v>366</v>
+        <v>303</v>
       </c>
       <c r="E46" t="s">
-        <v>258</v>
+        <v>223</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>345</v>
+        <v>287</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>367</v>
+        <v>304</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>368</v>
+        <v>305</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -4083,22 +4473,22 @@
         <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>362</v>
+        <v>300</v>
       </c>
       <c r="E47" t="s">
-        <v>259</v>
+        <v>224</v>
       </c>
       <c r="F47" s="14" t="s">
         <v>370</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>346</v>
+        <v>288</v>
       </c>
       <c r="H47" s="14" t="s">
-        <v>371</v>
+        <v>307</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>369</v>
+        <v>306</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -4109,22 +4499,22 @@
         <v>15</v>
       </c>
       <c r="D48" t="s">
-        <v>366</v>
+        <v>303</v>
       </c>
       <c r="E48" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>377</v>
+        <v>359</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H48" s="14" t="s">
-        <v>372</v>
+        <v>308</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>373</v>
+        <v>309</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -4135,25 +4525,25 @@
         <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>381</v>
+        <v>314</v>
       </c>
       <c r="D49" t="s">
-        <v>376</v>
+        <v>311</v>
       </c>
       <c r="E49" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>316</v>
+        <v>260</v>
       </c>
       <c r="H49" s="14" t="s">
-        <v>378</v>
+        <v>312</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>379</v>
+        <v>313</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -4164,22 +4554,22 @@
         <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>382</v>
+        <v>315</v>
       </c>
       <c r="E50" t="s">
-        <v>278</v>
+        <v>235</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>279</v>
+        <v>372</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>346</v>
+        <v>288</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>388</v>
+        <v>320</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>383</v>
+        <v>316</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -4190,22 +4580,22 @@
         <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>391</v>
+        <v>323</v>
       </c>
       <c r="E51" t="s">
-        <v>280</v>
+        <v>236</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>281</v>
+        <v>373</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>347</v>
+        <v>289</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>390</v>
+        <v>322</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>389</v>
+        <v>321</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -4219,19 +4609,19 @@
         <v>8</v>
       </c>
       <c r="E52" t="s">
-        <v>305</v>
-      </c>
-      <c r="F52" t="s">
-        <v>306</v>
+        <v>251</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>383</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="H52" t="s">
-        <v>307</v>
+        <v>252</v>
       </c>
       <c r="I52" t="s">
-        <v>308</v>
+        <v>253</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -4242,22 +4632,22 @@
         <v>15</v>
       </c>
       <c r="D53" t="s">
-        <v>356</v>
+        <v>295</v>
       </c>
       <c r="E53" t="s">
-        <v>354</v>
-      </c>
-      <c r="F53" t="s">
-        <v>355</v>
+        <v>294</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>374</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>356</v>
+        <v>295</v>
       </c>
       <c r="H53" t="s">
-        <v>358</v>
+        <v>297</v>
       </c>
       <c r="I53" t="s">
-        <v>357</v>
+        <v>296</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -4268,76 +4658,105 @@
         <v>17</v>
       </c>
       <c r="C54" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D54" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E54" t="s">
-        <v>374</v>
-      </c>
-      <c r="F54" t="s">
+        <v>310</v>
+      </c>
+      <c r="F54" s="14" t="s">
         <v>375</v>
       </c>
       <c r="G54" s="10"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>50</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E55" t="s">
-        <v>142</v>
+        <v>380</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D57" s="11" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D62" t="s">
+        <v>376</v>
+      </c>
+      <c r="F56" s="14" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
-        <v>384</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D65" s="11" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D66" s="11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="68" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="69" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="70" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D70" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="71" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="72" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>330</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:I54"/>
   <sortState ref="O5:O10">
     <sortCondition descending="1" ref="O5"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B55">
       <formula1>$K$5:$K$10</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Integrated all feedback to roadmap and now working through TODO list
</commit_message>
<xml_diff>
--- a/Dev/EBTA Developent Roadmap.xlsx
+++ b/Dev/EBTA Developent Roadmap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Outline" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="406">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -327,9 +327,6 @@
     <t>9 -</t>
   </si>
   <si>
-    <t>19 -</t>
-  </si>
-  <si>
     <t>20 -</t>
   </si>
   <si>
@@ -1027,6 +1024,382 @@
   </si>
   <si>
     <t>Item/Player Attributes</t>
+  </si>
+  <si>
+    <t>* Make PAP unlock when you get to end of game
+* Unlocked by finishing all of the game
+* Sound of lightening
+ * followed by the sounds of cowboys
+* Looks like you need to give something to get something in return
+* PAP EXP level</t>
+  </si>
+  <si>
+    <t>* Adding your dad, Alex Jones, Arnold, Jesse Ventura, auto turrets etc, harry potter ring that can talk to the dead
+* Even more secret place under okons storage place. Leads to underground base.
+* Mike the liar random event. Running across campus saying stuff. Comments on 4th wall things about the game ex) "They need an autocomplete"
+* Stackable Visor Glasses
+* Brendan's jacket holds things in the game
+scuba Steve (and it's Haugen)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Adding explinations to all jokes and inside things to keep game relavent. Not sure if this would take away from game OR if you would only play the year you have it. Idk.
+* When characters die they drop bio cheet and what their interests are (credits like a great help for devloping game)
+* Add better biosheet, description of items to explain jokes, a tutorial, and more help to have players finish the game and enjoy it
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Adding an experience level to the game and mobs that respawn so you feel like you're progressing. Probably buffs stats and helps you beat higher level people/things. Also the respawn with golden gauntlet thanos for Paul the buss driver.
+* In general, have more crazy/dangerous things happen as you progress in quests/storyline (sand worms pop up, idk, crazyness)
+* Could have random drop loot
+* Having fire with cooking be able to cook multiple types of foods (Eggs, meat, bread, ) with BOTW sound
+* Having more combinations of cooking food
+* Having more Runescape cooking, experience levels to unlock/burn less, burn levels, etc
+</t>
+  </si>
+  <si>
+    <t>* Make game run in javascript/whatever online so you can play game online. 
+* Also has QT scoreboard so more compeditive</t>
+  </si>
+  <si>
+    <t>* Make other players be able to interact, fight, talk to eachother</t>
+  </si>
+  <si>
+    <t>* Adding time to game. 
+* Either BOTW 2 min for 1 hr with longest day, or minecraft. I don't think ever step 5 minutes. 
+* Maybe watch system
+* time based events, 
+* time based characters/moving, etc. 
+* Starting day is 12pm, day after Kipling (for 2017-2018 version).
+* For 2019 version make so have at least a week before kipling</t>
+  </si>
+  <si>
+    <t>BD, 15+10+8+15+20?</t>
+  </si>
+  <si>
+    <t>* Making so surroundings of obveous areas print out. 
+* Have lore print first and then title+search around you.</t>
+  </si>
+  <si>
+    <t>* Can add content to game and make their own quests/stories. 
+* Maybe unlocks when you beat the game.
+* Save files need to be able to recompile after adding items
+* Able to add items, quests, people, change descriptions, etc
+* Almost like scripting tools within the game
+* Maybe make a set of mod tools with the game? Maybe those are Excel Sheets?</t>
+  </si>
+  <si>
+    <t>* Mini-gamers around area. Not made by me but implemented.
+* pong 
+* chess (Mitch is always there) 
+* tetris (Zac introduces you)
+* Zork
+* watching Ascii new hope
+* Classic riddles/storries (goat, chicken, fox)
+* Liars Dice (SP or MP) Tyler and Angus in full pirate gear, Hani is part of the wall (part of the ship part of the crew (the Die is cast and Davy Jones is there as well )</t>
+  </si>
+  <si>
+    <t>* Use google maps data to design exteriors/interriors for things</t>
+  </si>
+  <si>
+    <t>* Make so it takes files automatically
+* gives icon automatically 
+* does code checks out 
+* installer gives desktop icon
+* Overwriting old instal to update would be nice.</t>
+  </si>
+  <si>
+    <t>* In GUI window have options to save/load game, pause, volume settings, window size, text size, colour settings maybe?
+* These settings are saved locally to the game file</t>
+  </si>
+  <si>
+    <t>* Start player in secluded area/small island to get a sense but still have tutorial
+* First 5 minutes set tone of the game, set expectations and colour whole experience. 
+* 3ways to draw in (best have at least 2 of these and multiple intros)
+* 1. Sell you with the narrative 2. Wow you with the mechanics 3. Draw you in with the spectacle
+* Mystery is a great tool for hooking someone. Can also sell the world  (put what is compelling in there and don't hold back)
+* Deliver why player would want to play the game and deliver in 1st 5 minute (don't even have to take away powers). 
+* Shouldn't front load tutorial either. They simplified it
+* Start with spectacular or novel. Can throw into a story already in progress (in medius res)</t>
+  </si>
+  <si>
+    <t>* People drop money/you can make money
+* Petter is a seller and you can buy Marvin the Martian thing
+* Can drop a little bit from cops but not too much to farm
+* Investing in stocks that are real and pulled from an API
+* Grand exchange for items</t>
+  </si>
+  <si>
+    <t>*Adding different weather changes
+* debufs
+* envoirnment to keep up emersion
+* Pulling realworld weather and weather predictions from an API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Do more with name including character address you by name and work with names including name infulence. </t>
+  </si>
+  <si>
+    <t>* Easy, Medium, Hard, Ironman verson where can't heal/carry more than you can
+* Maybe all with different endings
+* Easy-medium-Hardcore modes where you have 
+1. map w. quest outline (maybe a box?) - exploitable map/looking - no map  
+2. Enemy difficulty 
+3. Item outlines? 
+4. No eating 
+5. Full inventory vs expandable vs just you?
+* Try not to do just simple health/attack scaling. Maybe add new mechanics</t>
+  </si>
+  <si>
+    <t>* Items can give Flying, Electricity, crafting, survival, weight, volume stored
+* Water, food, and stanima for player
+* Being able to carry more things or have Backbacks
+* Including Iron man suit with Energy, craftables and consumables with energy. 
+* Secret weird flying place/base. Secret places you can only get to by flying into upper buildings
+* You can fly up too far and fly out of the game</t>
+  </si>
+  <si>
+    <t>* Keep track of all items/things collected
+* Steam/platinum trophies</t>
+  </si>
+  <si>
+    <t>* Make facebook, twitter, website, instagram outreach and update to keep players/community involved and invite new players
+* Put game on steam</t>
+  </si>
+  <si>
+    <t>* They move around
+* Have  a companion
+* Can equip items to yourself to store for later games so they act as a companion.</t>
+  </si>
+  <si>
+    <t>* Sling ring, teliport anywhere you know
+* Portal gun
+* Teliport anywhere you can see
+* Instant transmission (anything)
+* Zombies teliporter (where another one is but also in time)
+* Star Trek teliport (anywhere but only to/from consol).</t>
+  </si>
+  <si>
+    <t>* Star level where police come after you, eventually SWAT
+* eventually have to escape on rocket in smoke stack to go meet Elon musk on the moon</t>
+  </si>
+  <si>
+    <t>* GUI text printer, change colour, font, style of words to highlight.</t>
+  </si>
+  <si>
+    <t>* Involves lore from the skate video
+. You see a campus police guard pull up to talk to someone on the skateboard.
+"Erik the Sk8r: Hey Bill"
+"Bill the Mac Cop: Hey Erik, you know you can't be here right?"
+"Bill: Comomon man we do this every day"
+"Erik: Okay then, see you tomorrow!"
+He scates off quickly up 
+"Bill the Mac Cop: You can't skate on campus prop... aww whatever."</t>
+  </si>
+  <si>
+    <t>* Hollywood Murder Mystery. All aspects and functions of hollywood
+* Have to fight the racoons</t>
+  </si>
+  <si>
+    <t>* Phil clones himself to make it more efficient but gets out of control
+* Have to fight off all ranges of Phils
+* Only way to kill them is to poisen cafine supply into the school
+* So only drunk Phil remains</t>
+  </si>
+  <si>
+    <t>* Fight combatants against eachother (including different Phils).
+* Can also fight in it yourself to go up ranks</t>
+  </si>
+  <si>
+    <t>* You teliport to green lake, explore all the mysteries of Brendan Fallon's past and life
+* See update notes</t>
+  </si>
+  <si>
+    <t>* Expand Map to whole school
+* make a storyline containing first year eng experience and classes</t>
+  </si>
+  <si>
+    <t>* Just bassically Nazi Zombies mode
+* Wunderwaffe DG-2  1000, 100, -10
+*  Chain lightning! 115 not included</t>
+  </si>
+  <si>
+    <t>* Real life farming times for best weapons
+* Every 1/20 pumpkin gives mutated Wunder pumpkin which is best headgear
+* Because it's better reactor it's mutated
+* If creating long term things need to have good, stable, encrypted save files that can be updated with version
+* Create element 420 in the reactor to make wonder weapons</t>
+  </si>
+  <si>
+    <t>* Matlab 
+* HFF 2020
+* any other game I make</t>
+  </si>
+  <si>
+    <t>* Having a ascii art converter and font typing creator
+* making a cover picture
+* having all the pictures of stuff in game</t>
+  </si>
+  <si>
+    <t>Text/Grammar/Naming</t>
+  </si>
+  <si>
+    <t>Short word for verbs,  for inv, s for stats</t>
+  </si>
+  <si>
+    <t>Angus, Beef, Barber ("Call me a liar")</t>
+  </si>
+  <si>
+    <t>I kinda disagree with this one for now. Don't think it should autosave</t>
+  </si>
+  <si>
+    <t>* A way to make game update automatically is with an update launcher
+* Only if not going online
+* Auto save every once and a while</t>
+  </si>
+  <si>
+    <t>* Making sure all bosses are beatable without secrets so at least not frustrating for new players
+* See balance metrics from balance sheet
+* Maybe only have saving and autosaving as a developer.</t>
+  </si>
+  <si>
+    <t>* Adding map and all suplementary info to the GUI (maybe whole game?) so we can customize content. 
+* IDK. I like idea of two window system with map, player icon, pictures, etc on side. 
+* Size of window (ascii art print)</t>
+  </si>
+  <si>
+    <t>*Year selector
+* tutorial
+* intro
+* Map/characters ( Measure Alice or Bob &amp; they collapse, also DOD)
+* BSB Dungeon
+* storyline/quests. This is a substantial piece of work
+* See Google Keep notes on the story</t>
+  </si>
+  <si>
+    <t>Balance</t>
+  </si>
+  <si>
+    <t>Queues</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>SharpExchange</t>
+  </si>
+  <si>
+    <t>* Right now defense is v important but with healing items added this should fix it
+* Better head items plz
+* Need story arc for body armour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Need to know that Jana has the textbook, maybe the story should say that somewhere
+* Not obveous that equip means to pick up
+* Phil says that need to be pushed more toward the Phenoix (more people you talk to, or items, tell story about the Phoneix)
+</t>
+  </si>
+  <si>
+    <t>More use of storyline, music, definition to people to give realism to the world</t>
+  </si>
+  <si>
+    <t>Put into feature lock</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>Have Brendan Fallon character with eclipse mug, rocketry t-shirt, Strainer on head?SafetyGlasses?, and iron ring (more characters)</t>
+  </si>
+  <si>
+    <t>Easier way to access game, not just goo.gl/iK8dL9 (Website maybe)</t>
+  </si>
+  <si>
+    <t>* Allow Sounds to play
+* transitions and have 
+* different music for different settings
+* Belzabad plays when you fight kleiman
+* Channel Orange by Frank Ocean</t>
+  </si>
+  <si>
+    <t>18 - 90 Cleaned up features list, started going through and combining with feedback</t>
+  </si>
+  <si>
+    <t>Procedural Generation</t>
+  </si>
+  <si>
+    <t>Having Map/dungeons, maybe charaters, proceduraly generated</t>
+  </si>
+  <si>
+    <t>* Attack and defense, speed doesn't do anything. 
+* Would need to be be after combat update. 
+* Possibly have star/some sort of indicator for bosses OR have the indicator just be how hard they can hit you/how big they are
+* More direct reward for exploration with something that ties back into game (like BOTW)
+* Having body armour Quantum relic</t>
+  </si>
+  <si>
+    <t>* When you inspect the car it says 'Ya thought these were the keys'
+* When you searching when nothings there "You double take and there's still nothing there" (If you search 20 times you die)</t>
+  </si>
+  <si>
+    <t>* Ritual gone wrong that spawns dumb undead things at night. Ritual involves turning Casion calculator into the other.
+* If you go to edge and press side 1000(50) times you go around to the other edge
+* Pressing down 420 times in a certain place sents you to hell and you fight satan, and Bezabad plays.
+* You can also sumon Satan to get the joint of destiny
+* Teachers come back to life and you can kill zombie versions of them
+* Can eat people after you kill them(Arther), depending on who you eat you die
+* Maybe involve kathulu</t>
+  </si>
+  <si>
+    <t>* Make keywords shorter, have list of items to choose from quickly [1-2], maybe accept short names? 
+* Maybe take cardinal coords. 
+* More things rather than equip. 
+* Also possibly controller support?
+* Short word for verbs,  for inv, s for stats
+* Try having WASD and other key accepts (maybe arrow keys) on the GUI acceptable</t>
+  </si>
+  <si>
+    <t>* Building and all things are breakable/fightable/destroyable.
+* When things break the items/characters get put on main floor but dead, interrior destroyed
+* Blowing up building calls to police
+* attack/eat rules sign/interactactables</t>
+  </si>
+  <si>
+    <t>* Move map to right side GUI.
+* Map display better
+* quest progress tracker, can give hints on where to go/where things are
+* Ingame journal or notes function.</t>
+  </si>
+  <si>
+    <t>Map/Items/People/Quests</t>
+  </si>
+  <si>
+    <t>Finished Feature lock so all future features go marked as not in this update</t>
+  </si>
+  <si>
+    <t>* Spelling and grammar check before release (maybe needs a text output function)
+* Don't except empty name
+* "B is back" (Zac)
+* "Dell, Intel Inside"
+* search keyword for search
+* When you inspect the car it says 'Ya thought these were the keys'
+* When you searching when nothings there "You double take and there's still nothing there" (If you search 20 times you die)
+* See TODO list for all remaining bugs</t>
+  </si>
+  <si>
+    <t>* Error checking to see if place exists before moving
+* Wear earphones on head
+* 3W text in QT
+* Add Nicole to EP office
+* Wacky items are good
+* 3BB PID with MSP430
+* Have Brendan Fallon character with eclipse mug, rocketry t-shirt, Strainer on head?SafetyGlasses?, and iron ring (more characters)
+* Giving context about 3W text and also have more things tell you about phoneix and also items (More use of storyline, music, definition to people to give realism to the world)
+* After giving dirty needle to sharp exchange a random encounter with a person that says "You're the greatest semaritan in the world" and gives you and Uzi
+* Need to know that Jana has the textbook, maybe the story should say that somewhere
+* Not obveous that equip means to pick up
+* Phil says that need to be pushed more toward the Phenoix (more people you talk to, or items, tell story about the Phoneix)
+** Tyler wants it to be Sandbox mode, no linear stuff, events unfold from there
+* Expand on the Story and the high council so they can piece everything together
+* See TODO list for all remaining bugs</t>
   </si>
   <si>
     <t>* Classes, object methods, how map works (numbered adjacency lists), commenting code. Updating to python 3. Interactables class. Buildings as an entity.
@@ -1041,49 +1414,8 @@
           Interroor
      Item
           Interactable
-          Interactable can go, just add a moveable flag to items with new entity structute that allows give/take</t>
-  </si>
-  <si>
-    <t>* Make PAP unlock when you get to end of game
-* Unlocked by finishing all of the game
-* Sound of lightening
- * followed by the sounds of cowboys
-* Looks like you need to give something to get something in return
-* PAP EXP level</t>
-  </si>
-  <si>
-    <t>* Make a basic interrior of bsb and fully test. 
-* Then make all multilevel buildings an interrior</t>
-  </si>
-  <si>
-    <t>* Adding your dad, Alex Jones, Arnold, Jesse Ventura, auto turrets etc, harry potter ring that can talk to the dead
-* Even more secret place under okons storage place. Leads to underground base.
-* Mike the liar random event. Running across campus saying stuff. Comments on 4th wall things about the game ex) "They need an autocomplete"
-* Stackable Visor Glasses
-* Brendan's jacket holds things in the game
-scuba Steve (and it's Haugen)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Adding explinations to all jokes and inside things to keep game relavent. Not sure if this would take away from game OR if you would only play the year you have it. Idk.
-* When characters die they drop bio cheet and what their interests are (credits like a great help for devloping game)
-* Add better biosheet, description of items to explain jokes, a tutorial, and more help to have players finish the game and enjoy it
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Adding an experience level to the game and mobs that respawn so you feel like you're progressing. Probably buffs stats and helps you beat higher level people/things. Also the respawn with golden gauntlet thanos for Paul the buss driver.
-* In general, have more crazy/dangerous things happen as you progress in quests/storyline (sand worms pop up, idk, crazyness)
-* Could have random drop loot
-* Having fire with cooking be able to cook multiple types of foods (Eggs, meat, bread, ) with BOTW sound
-* Having more combinations of cooking food
-* Having more Runescape cooking, experience levels to unlock/burn less, burn levels, etc
-</t>
-  </si>
-  <si>
-    <t>* Make game run in javascript/whatever online so you can play game online. 
-* Also has QT scoreboard so more compeditive</t>
-  </si>
-  <si>
-    <t>* Make other players be able to interact, fight, talk to eachother</t>
+          Interactable can go, just add a moveable flag to items with new entity structute that allows give/take
+* See TODO list for rest of rebuild notes</t>
   </si>
   <si>
     <t>* See 13 Hollywood Productions March 7th large section of ideas.
@@ -1093,326 +1425,30 @@
 *  At least for now someone comes back for round two.
 * Every Person has their own weakness/strengths.
 * Use Darksouls style damage system
-* Bullet time</t>
-  </si>
-  <si>
-    <t>* Adding time to game. 
-* Either BOTW 2 min for 1 hr with longest day, or minecraft. I don't think ever step 5 minutes. 
-* Maybe watch system
-* time based events, 
-* time based characters/moving, etc. 
-* Starting day is 12pm, day after Kipling (for 2017-2018 version).
-* For 2019 version make so have at least a week before kipling</t>
-  </si>
-  <si>
-    <t>BD, 15+10+8+15+20?</t>
-  </si>
-  <si>
-    <t>* Making so save/load and all personal game data is kept safe and unhackable 
-* Also probably encrypted is better for online pins, etc</t>
-  </si>
-  <si>
-    <t>* Making so surroundings of obveous areas print out. 
-* Have lore print first and then title+search around you.</t>
-  </si>
-  <si>
-    <t>* Can add content to game and make their own quests/stories. 
-* Maybe unlocks when you beat the game.
-* Save files need to be able to recompile after adding items
-* Able to add items, quests, people, change descriptions, etc
-* Almost like scripting tools within the game
-* Maybe make a set of mod tools with the game? Maybe those are Excel Sheets?</t>
-  </si>
-  <si>
-    <t>* Move map to right side GUI.
-* Map display better
-* quest tracker, can give hints on where to go/where things are
-* Ingame journal or notes function.</t>
-  </si>
-  <si>
-    <t>* Mini-gamers around area. Not made by me but implemented.
-* pong 
-* chess (Mitch is always there) 
-* tetris (Zac introduces you)
-* Zork
-* watching Ascii new hope
-* Classic riddles/storries (goat, chicken, fox)
-* Liars Dice (SP or MP) Tyler and Angus in full pirate gear, Hani is part of the wall (part of the ship part of the crew (the Die is cast and Davy Jones is there as well )</t>
-  </si>
-  <si>
-    <t>* Use google maps data to design exteriors/interriors for things</t>
-  </si>
-  <si>
-    <t>* Make so it takes files automatically
-* gives icon automatically 
-* does code checks out 
-* installer gives desktop icon
-* Overwriting old instal to update would be nice.</t>
-  </si>
-  <si>
-    <t>* In GUI window have options to save/load game, pause, volume settings, window size, text size, colour settings maybe?
-* These settings are saved locally to the game file</t>
-  </si>
-  <si>
-    <t>* Start player in secluded area/small island to get a sense but still have tutorial
-* First 5 minutes set tone of the game, set expectations and colour whole experience. 
-* 3ways to draw in (best have at least 2 of these and multiple intros)
-* 1. Sell you with the narrative 2. Wow you with the mechanics 3. Draw you in with the spectacle
-* Mystery is a great tool for hooking someone. Can also sell the world  (put what is compelling in there and don't hold back)
-* Deliver why player would want to play the game and deliver in 1st 5 minute (don't even have to take away powers). 
-* Shouldn't front load tutorial either. They simplified it
-* Start with spectacular or novel. Can throw into a story already in progress (in medius res)</t>
-  </si>
-  <si>
-    <t>* People drop money/you can make money
-* Petter is a seller and you can buy Marvin the Martian thing
-* Can drop a little bit from cops but not too much to farm
-* Investing in stocks that are real and pulled from an API
-* Grand exchange for items</t>
-  </si>
-  <si>
-    <t>*Adding different weather changes
-* debufs
-* envoirnment to keep up emersion
-* Pulling realworld weather and weather predictions from an API</t>
-  </si>
-  <si>
-    <t>* Attack and defense, speed doesn't do anything. 
-* Would need to be be after combat update. 
-* Possibly have star/some sort of indicator for bosses OR have the indicator just be how hard they can hit you/how big they are
-* More direct reward for exploration with something that ties back into game (like BOTW)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Do more with name including character address you by name and work with names including name infulence. </t>
-  </si>
-  <si>
-    <t>* Easy, Medium, Hard, Ironman verson where can't heal/carry more than you can
-* Maybe all with different endings
-* Easy-medium-Hardcore modes where you have 
-1. map w. quest outline (maybe a box?) - exploitable map/looking - no map  
-2. Enemy difficulty 
-3. Item outlines? 
-4. No eating 
-5. Full inventory vs expandable vs just you?
-* Try not to do just simple health/attack scaling. Maybe add new mechanics</t>
-  </si>
-  <si>
-    <t>* Items can give Flying, Electricity, crafting, survival, weight, volume stored
-* Water, food, and stanima for player
-* Being able to carry more things or have Backbacks
-* Including Iron man suit with Energy, craftables and consumables with energy. 
-* Secret weird flying place/base. Secret places you can only get to by flying into upper buildings
-* You can fly up too far and fly out of the game</t>
-  </si>
-  <si>
-    <t>* Keep track of all items/things collected
-* Steam/platinum trophies</t>
-  </si>
-  <si>
-    <t>* Make facebook, twitter, website, instagram outreach and update to keep players/community involved and invite new players
-* Put game on steam</t>
-  </si>
-  <si>
-    <t>* Ritual gone wrong that spawns dumb undead things at night. Ritual involves turning Casion calculator into the other.
-* If you go to edge and press side 1000(50) times you go around to the other edge
-* Pressing down 420 times in a certain place sents you to hell and you fight satan, and Bezabad plays.
-* You can also sumon Satan to get the joint of destiny
-* Teachers come back to life and you can kill zombie versions of them
-* Maybe involve kathulu</t>
-  </si>
-  <si>
-    <t>* They move around
-* Have  a companion
-* Can equip items to yourself to store for later games so they act as a companion.</t>
-  </si>
-  <si>
-    <t>* Sling ring, teliport anywhere you know
-* Portal gun
-* Teliport anywhere you can see
-* Instant transmission (anything)
-* Zombies teliporter (where another one is but also in time)
-* Star Trek teliport (anywhere but only to/from consol).</t>
-  </si>
-  <si>
-    <t>* Building and all things are breakable/fightable/destroyable.
-* When things break the items/characters get put on main floor but dead, interrior destroyed
-* Blowing up building calls to police</t>
-  </si>
-  <si>
-    <t>* Star level where police come after you, eventually SWAT
-* eventually have to escape on rocket in smoke stack to go meet Elon musk on the moon</t>
-  </si>
-  <si>
-    <t>* GUI text printer, change colour, font, style of words to highlight.</t>
-  </si>
-  <si>
-    <t>* Involves lore from the skate video
-. You see a campus police guard pull up to talk to someone on the skateboard.
-"Erik the Sk8r: Hey Bill"
-"Bill the Mac Cop: Hey Erik, you know you can't be here right?"
-"Bill: Comomon man we do this every day"
-"Erik: Okay then, see you tomorrow!"
-He scates off quickly up 
-"Bill the Mac Cop: You can't skate on campus prop... aww whatever."</t>
-  </si>
-  <si>
-    <t>* Hollywood Murder Mystery. All aspects and functions of hollywood
-* Have to fight the racoons</t>
-  </si>
-  <si>
-    <t>* Phil clones himself to make it more efficient but gets out of control
-* Have to fight off all ranges of Phils
-* Only way to kill them is to poisen cafine supply into the school
-* So only drunk Phil remains</t>
-  </si>
-  <si>
-    <t>* Fight combatants against eachother (including different Phils).
-* Can also fight in it yourself to go up ranks</t>
-  </si>
-  <si>
-    <t>* You teliport to green lake, explore all the mysteries of Brendan Fallon's past and life
-* See update notes</t>
-  </si>
-  <si>
-    <t>* Expand Map to whole school
-* make a storyline containing first year eng experience and classes</t>
-  </si>
-  <si>
-    <t>* Just bassically Nazi Zombies mode
-* Wunderwaffe DG-2  1000, 100, -10
-*  Chain lightning! 115 not included</t>
-  </si>
-  <si>
-    <t>* Real life farming times for best weapons
-* Every 1/20 pumpkin gives mutated Wunder pumpkin which is best headgear
-* Because it's better reactor it's mutated
-* If creating long term things need to have good, stable, encrypted save files that can be updated with version
-* Create element 420 in the reactor to make wonder weapons</t>
-  </si>
-  <si>
-    <t>* Matlab 
-* HFF 2020
-* any other game I make</t>
-  </si>
-  <si>
-    <t>* Having a ascii art converter and font typing creator
-* making a cover picture
-* having all the pictures of stuff in game</t>
-  </si>
-  <si>
-    <t>Text/Grammar/Naming</t>
-  </si>
-  <si>
-    <t>Short word for verbs,  for inv, s for stats</t>
-  </si>
-  <si>
-    <t>* Make keywords shorter, have list of items to choose from quickly [1-2], maybe accept short names? 
-* Maybe take cardinal coords. 
-* More things rather than equip. 
-* Also possibly controller support?
-* Short word for verbs,  for inv, s for stats</t>
-  </si>
-  <si>
-    <t>Angus, Beef, Barber ("Call me a liar")</t>
-  </si>
-  <si>
-    <t>Map/Items/People</t>
-  </si>
-  <si>
-    <t>I kinda disagree with this one for now. Don't think it should autosave</t>
-  </si>
-  <si>
-    <t>* A way to make game update automatically is with an update launcher
-* Only if not going online
-* Auto save every once and a while</t>
-  </si>
-  <si>
-    <t>* Making sure all bosses are beatable without secrets so at least not frustrating for new players
-* See balance metrics from balance sheet
-* Maybe only have saving and autosaving as a developer.</t>
-  </si>
-  <si>
-    <t>* Adding map and all suplementary info to the GUI (maybe whole game?) so we can customize content. 
-* IDK. I like idea of two window system with map, player icon, pictures, etc on side. 
-* Size of window (ascii art print)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Spelling and grammar check before release (maybe needs a text output function)
-* Don't except empty name
-* "B is back" (Zac)
-* "Dell, Intel Inside"
-* search keyword for search
+* Bullet time
+* Maybe have speed play more of a factor, maybe balance in other ways
+* Name everything and attack dialougs (use x to do y)</t>
+  </si>
+  <si>
+    <t>Integrate TODO list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Making so save/load and all personal game data is kept safe and unhackable 
+* Also probably encrypted is better for online pins, etc
+Write to a file and encrypt it after finishing
+* https://www.guru99.com/reading-and-writing-files-in-python.html
+* https://www.youtube.com/watch?v=xSGnLPTjaXo
+* https://docs.python.org/2/tutorial/inputoutput.html - save structured data
+* Update save files so you write or so you understand pickling
 </t>
   </si>
   <si>
-    <t>*Year selector
-* tutorial
-* intro
-* Map/characters ( Measure Alice or Bob &amp; they collapse, also DOD)
-* BSB Dungeon
-* storyline/quests. This is a substantial piece of work
-* See Google Keep notes on the story</t>
-  </si>
-  <si>
-    <t>Balance</t>
-  </si>
-  <si>
-    <t>Queues</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>* When you inspect the car it says 'Ya thought these were the keys"
-* When you searching when nothings there "You double take and there's still nothing there" (If you search 20 times you die)</t>
-  </si>
-  <si>
-    <t>SharpExchange</t>
-  </si>
-  <si>
-    <t>* Right now defense is v important but with healing items added this should fix it
-* Better head items plz
-* Need story arc for body armour</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Need to know that Jana has the textbook, maybe the story should say that somewhere
-* Not obveous that equip means to pick up
-* Phil says that need to be pushed more toward the Phenoix (more people you talk to, or items, tell story about the Phoneix)
-</t>
-  </si>
-  <si>
-    <t>More use of storyline, music, definition to people to give realism to the world</t>
-  </si>
-  <si>
-    <t>Put into feature lock</t>
-  </si>
-  <si>
-    <t>Music</t>
-  </si>
-  <si>
-    <t>Have Brendan Fallon character with eclipse mug, rocketry t-shirt, Strainer on head?SafetyGlasses?, and iron ring (more characters)</t>
-  </si>
-  <si>
-    <t>Easier way to access game, not just goo.gl/iK8dL9 (Website maybe)</t>
-  </si>
-  <si>
-    <t>* Allow Sounds to play
-* transitions and have 
-* different music for different settings
-* Belzabad plays when you fight kleiman
-* Channel Orange by Frank Ocean</t>
-  </si>
-  <si>
-    <t>* Error checking to see if place exists before moving
-* Wear earphones on head
-* 3W text in QT
-* Add Nicole to EP office
-* Wacky items are good
-* 3BB PID with MSP430
-* Have Brendan Fallon character with eclipse mug, rocketry t-shirt, Strainer on head?SafetyGlasses?, and iron ring (more characters)</t>
-  </si>
-  <si>
-    <t>18 - 90 Cleaned up features list, started going through and combining with feedback</t>
+    <t>* Make a basic interrior of bsb and fully test. 
+* Then make all multilevel buildings an interrior
+* Shouldn't be in here but also from load screen Allow you to save as/copy, and delete files</t>
+  </si>
+  <si>
+    <t>19 - ✔ Finished integrating feedback and integrating TODO list</t>
   </si>
 </sst>
 </file>
@@ -1535,23 +1571,6 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -1597,6 +1616,23 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1611,14 +1647,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H51" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H51" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A1:H51"/>
   <sortState ref="A2:H51">
     <sortCondition ref="B1:B51"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="Feedback" dataDxfId="6"/>
-    <tableColumn id="2" name="Priority" dataDxfId="5"/>
+    <tableColumn id="1" name="Feedback" dataDxfId="5"/>
+    <tableColumn id="2" name="Priority" dataDxfId="4"/>
     <tableColumn id="3" name="Links"/>
     <tableColumn id="4" name="When Reported (update)"/>
     <tableColumn id="5" name="Est Implement Time (hrs)"/>
@@ -1631,16 +1667,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:I56" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A4:I56"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:I58" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A4:I58"/>
+  <sortState ref="A5:I58">
+    <sortCondition ref="A4:A58"/>
+  </sortState>
   <tableColumns count="9">
     <tableColumn id="1" name="Feature"/>
-    <tableColumn id="2" name="0.30 Priority" dataDxfId="3"/>
+    <tableColumn id="2" name="0.30 Priority" dataDxfId="2"/>
     <tableColumn id="3" name="Links"/>
     <tableColumn id="4" name="Est Implement Time (hrs)"/>
     <tableColumn id="5" name="Description (64 char max)"/>
-    <tableColumn id="6" name="Details" dataDxfId="2"/>
-    <tableColumn id="7" name="When to implement(update)" dataDxfId="1"/>
+    <tableColumn id="6" name="Details" dataDxfId="1"/>
+    <tableColumn id="7" name="When to implement(update)" dataDxfId="0"/>
     <tableColumn id="8" name="What kind of game it makes "/>
     <tableColumn id="9" name="Who would play this game"/>
   </tableColumns>
@@ -1913,8 +1952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1986,13 +2025,13 @@
         <v>94</v>
       </c>
       <c r="H9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I9" s="9">
         <v>45</v>
       </c>
       <c r="J9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2000,22 +2039,22 @@
         <v>97</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
+        <v>197</v>
+      </c>
+      <c r="D10" t="s">
         <v>198</v>
       </c>
-      <c r="D10" t="s">
-        <v>199</v>
-      </c>
       <c r="E10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H10">
         <v>330</v>
@@ -2023,80 +2062,80 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>323</v>
+      </c>
+      <c r="B11" t="s">
         <v>324</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>387</v>
+      </c>
+      <c r="D11" t="s">
+        <v>405</v>
+      </c>
+      <c r="E11" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" t="s">
+        <v>100</v>
+      </c>
+      <c r="I11" t="s">
         <v>325</v>
-      </c>
-      <c r="C11" t="s">
-        <v>401</v>
-      </c>
-      <c r="D11" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" t="s">
-        <v>99</v>
-      </c>
-      <c r="F11" t="s">
-        <v>100</v>
-      </c>
-      <c r="G11" t="s">
-        <v>101</v>
-      </c>
-      <c r="I11" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" t="s">
         <v>102</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>103</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>104</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>105</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>106</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>107</v>
       </c>
-      <c r="G12" t="s">
-        <v>108</v>
-      </c>
       <c r="I12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" t="s">
         <v>109</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>110</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>111</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>112</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>113</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>114</v>
       </c>
-      <c r="G13" t="s">
-        <v>115</v>
-      </c>
       <c r="I13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -2108,8 +2147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2364,7 +2403,7 @@
         <v>0.75</v>
       </c>
       <c r="F10" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>14</v>
@@ -2438,7 +2477,7 @@
         <v>0.25</v>
       </c>
       <c r="F14" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2449,7 +2488,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="D15">
         <v>0.28000000000000003</v>
@@ -2458,7 +2497,7 @@
         <v>0.5</v>
       </c>
       <c r="F15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2475,7 +2514,7 @@
         <v>1.5</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2492,7 +2531,7 @@
         <v>0.5</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2546,7 +2585,7 @@
         <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2658,14 +2697,14 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="19">
+      <c r="A27" s="11">
         <v>36</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="D27">
         <v>0.28999999999999998</v>
@@ -2674,14 +2713,14 @@
         <v>6</v>
       </c>
       <c r="F27" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="19">
+      <c r="A28" s="11">
         <v>38</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2694,14 +2733,14 @@
         <v>1.5</v>
       </c>
       <c r="F28" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="19">
+      <c r="A29" s="11">
         <v>40</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2714,11 +2753,11 @@
         <v>5</v>
       </c>
       <c r="F29" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="19">
+      <c r="A30" s="11">
         <v>42</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2731,11 +2770,14 @@
         <v>0.5</v>
       </c>
       <c r="F30" t="s">
-        <v>391</v>
+        <v>378</v>
+      </c>
+      <c r="G30" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="19">
+      <c r="A31" s="11">
         <v>44</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2748,11 +2790,11 @@
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="19">
+      <c r="A32" s="11">
         <v>45</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -2765,103 +2807,106 @@
         <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="19">
-        <v>50</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>17</v>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
+        <v>4</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="D33">
-        <v>0.28999999999999998</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E33">
-        <v>4</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>398</v>
+        <v>1.5</v>
+      </c>
+      <c r="F33" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>4</v>
+      <c r="A34" s="11">
+        <v>16</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="C34" t="s">
+        <v>58</v>
+      </c>
       <c r="D34">
         <v>0.28000000000000003</v>
       </c>
       <c r="E34">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="F34" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>16</v>
+      <c r="A35" s="11">
+        <v>17</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C35" t="s">
-        <v>58</v>
-      </c>
       <c r="D35">
         <v>0.28000000000000003</v>
       </c>
       <c r="E35">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>17</v>
+      <c r="A36" s="11">
+        <v>28</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="C36" t="s">
+        <v>61</v>
+      </c>
       <c r="D36">
         <v>0.28000000000000003</v>
       </c>
       <c r="E36">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="F36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
         <v>37</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>28</v>
-      </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C37" t="s">
-        <v>61</v>
       </c>
       <c r="D37">
         <v>0.28000000000000003</v>
       </c>
       <c r="E37">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>48</v>
+        <v>376</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="19">
-        <v>37</v>
+      <c r="A38" s="11">
+        <v>47</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>14</v>
@@ -2869,31 +2914,28 @@
       <c r="D38">
         <v>0.28000000000000003</v>
       </c>
-      <c r="E38">
-        <v>2</v>
-      </c>
-      <c r="F38" t="s">
-        <v>388</v>
-      </c>
-      <c r="G38" s="14" t="s">
-        <v>393</v>
+      <c r="E38" t="s">
+        <v>294</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="19">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D39">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="E39" t="s">
-        <v>295</v>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>225</v>
+        <v>385</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2957,9 +2999,6 @@
       <c r="F43" t="s">
         <v>42</v>
       </c>
-      <c r="G43" t="s">
-        <v>205</v>
-      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
@@ -3063,7 +3102,7 @@
         <v>3</v>
       </c>
       <c r="F49" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -3080,7 +3119,7 @@
         <v>5</v>
       </c>
       <c r="F50" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -3094,10 +3133,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E51" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -3105,7 +3144,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="F54" t="s">
         <v>64</v>
@@ -3119,10 +3158,10 @@
     <sortCondition ref="J1"/>
   </sortState>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B37">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B32 B34:B37">
       <formula1>$J$2:$J$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B38:B51">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B38:B51 B33">
       <formula1>$J$2:$J$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -3136,10 +3175,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P72"/>
+  <dimension ref="A1:P75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:I56"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3170,7 +3209,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>22</v>
@@ -3223,7 +3262,7 @@
         <v>79</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>332</v>
+        <v>400</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>84</v>
@@ -3264,10 +3303,10 @@
         <v>81</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H6" t="s">
         <v>86</v>
@@ -3299,25 +3338,25 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>404</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>334</v>
-      </c>
-      <c r="G7" s="10" t="s">
+      <c r="H7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" t="s">
         <v>118</v>
-      </c>
-      <c r="H7" t="s">
-        <v>120</v>
-      </c>
-      <c r="I7" t="s">
-        <v>119</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>13</v>
@@ -3346,19 +3385,19 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>335</v>
-      </c>
-      <c r="G8" s="10" t="s">
+      <c r="H8" t="s">
         <v>123</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>124</v>
-      </c>
-      <c r="I8" t="s">
-        <v>125</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>14</v>
@@ -3387,19 +3426,19 @@
         <v>15</v>
       </c>
       <c r="E9" t="s">
+        <v>125</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="H9" t="s">
+        <v>127</v>
+      </c>
+      <c r="I9" t="s">
         <v>126</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>336</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="H9" t="s">
-        <v>128</v>
-      </c>
-      <c r="I9" t="s">
-        <v>127</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>17</v>
@@ -3425,22 +3464,22 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E10" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H10" t="s">
         <v>129</v>
       </c>
-      <c r="F10" s="14" t="s">
-        <v>337</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>130</v>
-      </c>
-      <c r="I10" t="s">
-        <v>131</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>15</v>
@@ -3466,25 +3505,25 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E11" t="s">
         <v>58</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H11" t="s">
+        <v>134</v>
+      </c>
+      <c r="I11" t="s">
         <v>135</v>
-      </c>
-      <c r="I11" t="s">
-        <v>136</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>11</v>
@@ -3498,25 +3537,25 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G12" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="H12" t="s">
         <v>143</v>
       </c>
-      <c r="H12" t="s">
-        <v>144</v>
-      </c>
       <c r="I12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>76</v>
@@ -3533,25 +3572,25 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" t="s">
+        <v>145</v>
+      </c>
+      <c r="F13" t="s">
+        <v>336</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="H13" t="s">
         <v>147</v>
       </c>
-      <c r="D13" t="s">
-        <v>140</v>
-      </c>
-      <c r="E13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F13" t="s">
-        <v>339</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>148</v>
-      </c>
-      <c r="I13" t="s">
-        <v>149</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>17</v>
@@ -3568,17 +3607,17 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>378</v>
+        <v>393</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" t="s">
+        <v>150</v>
+      </c>
+      <c r="I14" t="s">
         <v>151</v>
-      </c>
-      <c r="I14" t="s">
-        <v>152</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>14</v>
@@ -3592,22 +3631,22 @@
         <v>15</v>
       </c>
       <c r="D15" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" t="s">
+        <v>153</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>401</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="E15" t="s">
-        <v>154</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>340</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>156</v>
-      </c>
       <c r="H15" t="s">
+        <v>160</v>
+      </c>
+      <c r="I15" t="s">
         <v>161</v>
-      </c>
-      <c r="I15" t="s">
-        <v>162</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>15</v>
@@ -3621,22 +3660,22 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -3647,25 +3686,25 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -3676,25 +3715,25 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D18">
         <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -3705,25 +3744,25 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D19">
         <v>6</v>
       </c>
       <c r="E19" t="s">
+        <v>167</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="H19" t="s">
         <v>168</v>
       </c>
-      <c r="F19" s="14" t="s">
-        <v>343</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="H19" t="s">
-        <v>169</v>
-      </c>
       <c r="I19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -3737,19 +3776,19 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
+        <v>170</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H20" t="s">
         <v>171</v>
       </c>
-      <c r="F20" s="14" t="s">
-        <v>344</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>172</v>
-      </c>
-      <c r="I20" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -3760,22 +3799,22 @@
         <v>15</v>
       </c>
       <c r="D21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E21" t="s">
+        <v>177</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="F21" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="G21" s="10" t="s">
+      <c r="H21" t="s">
         <v>179</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>180</v>
-      </c>
-      <c r="I21" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -3786,25 +3825,25 @@
         <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D22">
         <v>15</v>
       </c>
       <c r="E22" t="s">
+        <v>181</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>395</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H22" t="s">
         <v>182</v>
       </c>
-      <c r="F22" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>183</v>
-      </c>
-      <c r="I22" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -3818,19 +3857,19 @@
         <v>8</v>
       </c>
       <c r="E23" t="s">
+        <v>184</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H23" t="s">
         <v>185</v>
       </c>
-      <c r="F23" s="14" t="s">
-        <v>347</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>186</v>
-      </c>
-      <c r="I23" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3841,22 +3880,22 @@
         <v>15</v>
       </c>
       <c r="D24" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E24" t="s">
+        <v>187</v>
+      </c>
+      <c r="F24" t="s">
+        <v>342</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H24" t="s">
+        <v>189</v>
+      </c>
+      <c r="I24" t="s">
         <v>188</v>
-      </c>
-      <c r="F24" t="s">
-        <v>348</v>
-      </c>
-      <c r="G24" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="H24" t="s">
-        <v>190</v>
-      </c>
-      <c r="I24" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -3871,19 +3910,19 @@
         <v>4</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F25" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H25" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="G25" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>195</v>
-      </c>
       <c r="I25" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -3897,19 +3936,19 @@
         <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H26" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -3920,25 +3959,25 @@
         <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D27" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E27" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H27" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I27" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -3949,25 +3988,25 @@
         <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D28">
         <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="G28" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="H28" t="s">
         <v>241</v>
       </c>
-      <c r="H28" t="s">
+      <c r="I28" t="s">
         <v>242</v>
-      </c>
-      <c r="I28" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -3978,25 +4017,25 @@
         <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D29" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E29" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H29" t="s">
+        <v>243</v>
+      </c>
+      <c r="I29" t="s">
         <v>244</v>
-      </c>
-      <c r="I29" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -4007,25 +4046,25 @@
         <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D30" t="s">
+        <v>245</v>
+      </c>
+      <c r="E30" t="s">
+        <v>229</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H30" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="E30" t="s">
-        <v>230</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>351</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="H30" s="14" t="s">
+      <c r="I30" s="14" t="s">
         <v>247</v>
-      </c>
-      <c r="I30" s="14" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -4039,19 +4078,19 @@
         <v>8</v>
       </c>
       <c r="E31" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H31" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="I31" s="14" t="s">
         <v>249</v>
-      </c>
-      <c r="I31" s="14" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -4062,25 +4101,25 @@
         <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D32">
         <v>12</v>
       </c>
       <c r="E32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>354</v>
+        <v>390</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H32" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -4094,19 +4133,19 @@
         <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F33" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H33" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -4117,25 +4156,25 @@
         <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D34">
         <v>16</v>
       </c>
       <c r="E34" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H34" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="I34" s="14" t="s">
         <v>258</v>
-      </c>
-      <c r="I34" s="14" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -4149,19 +4188,19 @@
         <v>20</v>
       </c>
       <c r="E35" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="G35" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="H35" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="H35" s="14" t="s">
+      <c r="I35" s="14" t="s">
         <v>261</v>
-      </c>
-      <c r="I35" s="14" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -4175,19 +4214,19 @@
         <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="G36" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="H36" s="14" t="s">
         <v>264</v>
       </c>
-      <c r="H36" s="14" t="s">
-        <v>265</v>
-      </c>
       <c r="I36" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -4201,19 +4240,19 @@
         <v>20</v>
       </c>
       <c r="E37" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>360</v>
+        <v>392</v>
       </c>
       <c r="G37" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="H37" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="H37" s="14" t="s">
-        <v>267</v>
-      </c>
       <c r="I37" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -4224,25 +4263,25 @@
         <v>17</v>
       </c>
       <c r="C38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D38">
         <v>6</v>
       </c>
       <c r="E38" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -4253,25 +4292,25 @@
         <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D39">
         <v>12</v>
       </c>
       <c r="E39" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H39" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -4282,25 +4321,25 @@
         <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D40">
         <v>20</v>
       </c>
       <c r="E40" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>363</v>
+        <v>394</v>
       </c>
       <c r="G40" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="H40" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="H40" s="14" t="s">
+      <c r="I40" s="14" t="s">
         <v>279</v>
-      </c>
-      <c r="I40" s="14" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -4314,19 +4353,19 @@
         <v>10</v>
       </c>
       <c r="E41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="G41" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="H41" s="14" t="s">
         <v>281</v>
       </c>
-      <c r="H41" s="14" t="s">
+      <c r="I41" s="14" t="s">
         <v>282</v>
-      </c>
-      <c r="I41" s="14" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -4340,19 +4379,19 @@
         <v>7</v>
       </c>
       <c r="E42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F42" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H42" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="I42" s="14" t="s">
         <v>285</v>
-      </c>
-      <c r="I42" s="14" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -4366,19 +4405,19 @@
         <v>10</v>
       </c>
       <c r="E43" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -4389,25 +4428,25 @@
         <v>15</v>
       </c>
       <c r="C44" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D44" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E44" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -4418,25 +4457,25 @@
         <v>15</v>
       </c>
       <c r="C45" t="s">
+        <v>300</v>
+      </c>
+      <c r="D45" t="s">
+        <v>299</v>
+      </c>
+      <c r="E45" t="s">
+        <v>221</v>
+      </c>
+      <c r="F45" s="14" t="s">
+        <v>359</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="H45" s="14" t="s">
         <v>301</v>
       </c>
-      <c r="D45" t="s">
-        <v>300</v>
-      </c>
-      <c r="E45" t="s">
-        <v>222</v>
-      </c>
-      <c r="F45" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="G45" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="H45" s="14" t="s">
-        <v>302</v>
-      </c>
       <c r="I45" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -4447,22 +4486,22 @@
         <v>15</v>
       </c>
       <c r="D46" t="s">
+        <v>302</v>
+      </c>
+      <c r="E46" t="s">
+        <v>222</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="H46" s="14" t="s">
         <v>303</v>
       </c>
-      <c r="E46" t="s">
-        <v>223</v>
-      </c>
-      <c r="F46" s="14" t="s">
-        <v>369</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="H46" s="14" t="s">
+      <c r="I46" s="14" t="s">
         <v>304</v>
-      </c>
-      <c r="I46" s="14" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -4473,22 +4512,22 @@
         <v>15</v>
       </c>
       <c r="D47" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H47" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -4499,22 +4538,22 @@
         <v>15</v>
       </c>
       <c r="D48" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H48" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="I48" s="14" t="s">
         <v>308</v>
-      </c>
-      <c r="I48" s="14" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -4525,25 +4564,25 @@
         <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D49" t="s">
+        <v>310</v>
+      </c>
+      <c r="E49" t="s">
+        <v>226</v>
+      </c>
+      <c r="F49" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="H49" s="14" t="s">
         <v>311</v>
       </c>
-      <c r="E49" t="s">
-        <v>227</v>
-      </c>
-      <c r="F49" s="14" t="s">
-        <v>371</v>
-      </c>
-      <c r="G49" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="H49" s="14" t="s">
+      <c r="I49" s="14" t="s">
         <v>312</v>
-      </c>
-      <c r="I49" s="14" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -4554,22 +4593,22 @@
         <v>15</v>
       </c>
       <c r="D50" t="s">
+        <v>314</v>
+      </c>
+      <c r="E50" t="s">
+        <v>234</v>
+      </c>
+      <c r="F50" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="H50" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="I50" s="14" t="s">
         <v>315</v>
-      </c>
-      <c r="E50" t="s">
-        <v>235</v>
-      </c>
-      <c r="F50" s="14" t="s">
-        <v>372</v>
-      </c>
-      <c r="G50" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="H50" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="I50" s="14" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -4580,22 +4619,22 @@
         <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E51" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -4609,19 +4648,19 @@
         <v>8</v>
       </c>
       <c r="E52" t="s">
+        <v>250</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H52" t="s">
         <v>251</v>
       </c>
-      <c r="F52" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="G52" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="H52" t="s">
+      <c r="I52" t="s">
         <v>252</v>
-      </c>
-      <c r="I52" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -4632,22 +4671,22 @@
         <v>15</v>
       </c>
       <c r="D53" t="s">
+        <v>294</v>
+      </c>
+      <c r="E53" t="s">
+        <v>293</v>
+      </c>
+      <c r="F53" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="H53" t="s">
+        <v>296</v>
+      </c>
+      <c r="I53" t="s">
         <v>295</v>
-      </c>
-      <c r="E53" t="s">
-        <v>294</v>
-      </c>
-      <c r="F53" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="G53" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="H53" t="s">
-        <v>297</v>
-      </c>
-      <c r="I53" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -4655,92 +4694,128 @@
         <v>50</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C54" t="s">
-        <v>158</v>
-      </c>
-      <c r="D54" t="s">
-        <v>132</v>
+        <v>16</v>
       </c>
       <c r="E54" t="s">
-        <v>310</v>
+        <v>396</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>375</v>
-      </c>
-      <c r="G54" s="10"/>
+        <v>399</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>50</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" t="s">
+        <v>157</v>
+      </c>
+      <c r="D55" t="s">
+        <v>131</v>
+      </c>
+      <c r="E55" t="s">
+        <v>309</v>
+      </c>
+      <c r="F55" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="G55" s="10"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>51</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E55" t="s">
-        <v>380</v>
-      </c>
-      <c r="F55" s="14" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E63" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E64" t="s">
+        <v>398</v>
+      </c>
+      <c r="G56" s="10"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>52</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" t="s">
+        <v>388</v>
+      </c>
+      <c r="F57" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="G57" s="10"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>53</v>
+      </c>
+      <c r="F58" s="14"/>
+    </row>
+    <row r="65" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="66" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D65" s="11" t="s">
+    <row r="67" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D67" s="11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="68" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D68" s="11" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="69" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D69" s="11" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="66" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D66" s="11" t="s">
+    <row r="70" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D70" s="19" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="71" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="67" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D67" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="68" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D68" t="s">
+    <row r="72" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="69" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D69" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="70" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D70" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="71" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E71" t="s">
+      <c r="F72" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="73" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="72" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D72" t="s">
-        <v>330</v>
+    <row r="74" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="75" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -4748,7 +4823,7 @@
     <sortCondition descending="1" ref="O5"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B55">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B57">
       <formula1>$K$5:$K$10</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Integrated TODO list and EBTA Written work, ready for breakdown
</commit_message>
<xml_diff>
--- a/Dev/EBTA Developent Roadmap.xlsx
+++ b/Dev/EBTA Developent Roadmap.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="412">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -327,9 +327,6 @@
     <t>9 -</t>
   </si>
   <si>
-    <t>20 -</t>
-  </si>
-  <si>
     <t>21 -</t>
   </si>
   <si>
@@ -396,9 +393,6 @@
     <t>Future expansions, dungeons, kipling, tutorial room, etc</t>
   </si>
   <si>
-    <t>Nonsense Update</t>
-  </si>
-  <si>
     <t>0.30 ?</t>
   </si>
   <si>
@@ -1024,22 +1018,6 @@
   </si>
   <si>
     <t>Item/Player Attributes</t>
-  </si>
-  <si>
-    <t>* Make PAP unlock when you get to end of game
-* Unlocked by finishing all of the game
-* Sound of lightening
- * followed by the sounds of cowboys
-* Looks like you need to give something to get something in return
-* PAP EXP level</t>
-  </si>
-  <si>
-    <t>* Adding your dad, Alex Jones, Arnold, Jesse Ventura, auto turrets etc, harry potter ring that can talk to the dead
-* Even more secret place under okons storage place. Leads to underground base.
-* Mike the liar random event. Running across campus saying stuff. Comments on 4th wall things about the game ex) "They need an autocomplete"
-* Stackable Visor Glasses
-* Brendan's jacket holds things in the game
-scuba Steve (and it's Haugen)</t>
   </si>
   <si>
     <t xml:space="preserve">* Adding explinations to all jokes and inside things to keep game relavent. Not sure if this would take away from game OR if you would only play the year you have it. Idk.
@@ -1048,15 +1026,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">* Adding an experience level to the game and mobs that respawn so you feel like you're progressing. Probably buffs stats and helps you beat higher level people/things. Also the respawn with golden gauntlet thanos for Paul the buss driver.
-* In general, have more crazy/dangerous things happen as you progress in quests/storyline (sand worms pop up, idk, crazyness)
-* Could have random drop loot
-* Having fire with cooking be able to cook multiple types of foods (Eggs, meat, bread, ) with BOTW sound
-* Having more combinations of cooking food
-* Having more Runescape cooking, experience levels to unlock/burn less, burn levels, etc
-</t>
-  </si>
-  <si>
     <t>* Make game run in javascript/whatever online so you can play game online. 
 * Also has QT scoreboard so more compeditive</t>
   </si>
@@ -1064,28 +1033,11 @@
     <t>* Make other players be able to interact, fight, talk to eachother</t>
   </si>
   <si>
-    <t>* Adding time to game. 
-* Either BOTW 2 min for 1 hr with longest day, or minecraft. I don't think ever step 5 minutes. 
-* Maybe watch system
-* time based events, 
-* time based characters/moving, etc. 
-* Starting day is 12pm, day after Kipling (for 2017-2018 version).
-* For 2019 version make so have at least a week before kipling</t>
-  </si>
-  <si>
     <t>BD, 15+10+8+15+20?</t>
   </si>
   <si>
     <t>* Making so surroundings of obveous areas print out. 
 * Have lore print first and then title+search around you.</t>
-  </si>
-  <si>
-    <t>* Can add content to game and make their own quests/stories. 
-* Maybe unlocks when you beat the game.
-* Save files need to be able to recompile after adding items
-* Able to add items, quests, people, change descriptions, etc
-* Almost like scripting tools within the game
-* Maybe make a set of mod tools with the game? Maybe those are Excel Sheets?</t>
   </si>
   <si>
     <t>* Mini-gamers around area. Not made by me but implemented.
@@ -1099,13 +1051,6 @@
   </si>
   <si>
     <t>* Use google maps data to design exteriors/interriors for things</t>
-  </si>
-  <si>
-    <t>* Make so it takes files automatically
-* gives icon automatically 
-* does code checks out 
-* installer gives desktop icon
-* Overwriting old instal to update would be nice.</t>
   </si>
   <si>
     <t>* In GUI window have options to save/load game, pause, volume settings, window size, text size, colour settings maybe?
@@ -1157,10 +1102,6 @@
 * You can fly up too far and fly out of the game</t>
   </si>
   <si>
-    <t>* Keep track of all items/things collected
-* Steam/platinum trophies</t>
-  </si>
-  <si>
     <t>* Make facebook, twitter, website, instagram outreach and update to keep players/community involved and invite new players
 * Put game on steam</t>
   </si>
@@ -1229,11 +1170,6 @@
 * Create element 420 in the reactor to make wonder weapons</t>
   </si>
   <si>
-    <t>* Matlab 
-* HFF 2020
-* any other game I make</t>
-  </si>
-  <si>
     <t>* Having a ascii art converter and font typing creator
 * making a cover picture
 * having all the pictures of stuff in game</t>
@@ -1259,20 +1195,6 @@
     <t>* Making sure all bosses are beatable without secrets so at least not frustrating for new players
 * See balance metrics from balance sheet
 * Maybe only have saving and autosaving as a developer.</t>
-  </si>
-  <si>
-    <t>* Adding map and all suplementary info to the GUI (maybe whole game?) so we can customize content. 
-* IDK. I like idea of two window system with map, player icon, pictures, etc on side. 
-* Size of window (ascii art print)</t>
-  </si>
-  <si>
-    <t>*Year selector
-* tutorial
-* intro
-* Map/characters ( Measure Alice or Bob &amp; they collapse, also DOD)
-* BSB Dungeon
-* storyline/quests. This is a substantial piece of work
-* See Google Keep notes on the story</t>
   </si>
   <si>
     <t>Balance</t>
@@ -1311,13 +1233,6 @@
   </si>
   <si>
     <t>Easier way to access game, not just goo.gl/iK8dL9 (Website maybe)</t>
-  </si>
-  <si>
-    <t>* Allow Sounds to play
-* transitions and have 
-* different music for different settings
-* Belzabad plays when you fight kleiman
-* Channel Orange by Frank Ocean</t>
   </si>
   <si>
     <t>18 - 90 Cleaned up features list, started going through and combining with feedback</t>
@@ -1349,14 +1264,6 @@
 * Maybe involve kathulu</t>
   </si>
   <si>
-    <t>* Make keywords shorter, have list of items to choose from quickly [1-2], maybe accept short names? 
-* Maybe take cardinal coords. 
-* More things rather than equip. 
-* Also possibly controller support?
-* Short word for verbs,  for inv, s for stats
-* Try having WASD and other key accepts (maybe arrow keys) on the GUI acceptable</t>
-  </si>
-  <si>
     <t>* Building and all things are breakable/fightable/destroyable.
 * When things break the items/characters get put on main floor but dead, interrior destroyed
 * Blowing up building calls to police
@@ -1373,16 +1280,6 @@
   </si>
   <si>
     <t>Finished Feature lock so all future features go marked as not in this update</t>
-  </si>
-  <si>
-    <t>* Spelling and grammar check before release (maybe needs a text output function)
-* Don't except empty name
-* "B is back" (Zac)
-* "Dell, Intel Inside"
-* search keyword for search
-* When you inspect the car it says 'Ya thought these were the keys'
-* When you searching when nothings there "You double take and there's still nothing there" (If you search 20 times you die)
-* See TODO list for all remaining bugs</t>
   </si>
   <si>
     <t>* Error checking to see if place exists before moving
@@ -1402,11 +1299,120 @@
 * See TODO list for all remaining bugs</t>
   </si>
   <si>
+    <t>Integrate TODO list</t>
+  </si>
+  <si>
+    <t>19 - ✔ Finished integrating feedback and integrating TODO list</t>
+  </si>
+  <si>
+    <t>Fully Integrate (and delete) EBTA Written Work</t>
+  </si>
+  <si>
+    <t>* Keep track of all items/things collected
+* will need to Keep lots of stats on character including dumb ones like people killed, items picked up, spaces/distance moved, etc
+* Steam/platinum trophies</t>
+  </si>
+  <si>
+    <t>Mod Tools</t>
+  </si>
+  <si>
+    <t>Creators/Creative Person</t>
+  </si>
+  <si>
+    <t>Involved with players that can make their own stuff and post it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Can add content to game and make their own quests/stories. 
+* Maybe unlocks when you beat the game.
+* Save files need to be able to recompile after adding items
+* Able to add items, quests, people, change descriptions, etc
+* Almost like scripting tools within the game
+</t>
+  </si>
+  <si>
+    <t>* Bassically graphical version of Creative Mode scripting
+* Maybe make a set of mod tools with the game? Maybe those are Excel Sheets?
+* CSV entity importer and code writer (helps as part of Mod Tools where you can draw map in Excel and it imports it)</t>
+  </si>
+  <si>
+    <t>Nonsense/Insanity Update</t>
+  </si>
+  <si>
+    <t>* Make PAP unlock when you get to end of game
+* Unlocked by finishing all of the game
+* Sound of lightening
+ * followed by the sounds of cowboys
+* Looks like you need to give something to get something in return
+* PAP EXP level
+* - [x] Pack-a-punch 
+    - [ ] With sounds when it starts and ends
+    - [ ] Bell dongs every hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Allow Sounds to play
+* transitions and have 
+* different music for different settings
+* Belzabad plays when you fight kleiman
+* Channel Orange by Frank Ocean
+* More/changing voice dialoges for people
+* ability for characters to play audio when you talk to them
+* Make high pitch willhelm screen when women die
+</t>
+  </si>
+  <si>
+    <t>*Year selector
+* tutorial
+* intro
+* Map/characters ( Measure Alice or Bob &amp; they collapse, also DOD)
+* BSB Dungeon
+* storyline/quests. This is a substantial piece of work
+* See Google Keep notes on the story
+* BSB IS A DUNGEON WITH KEYS (EITHER UNIQUE OR NOT )</t>
+  </si>
+  <si>
+    <t>* Convert the game to Matlab to play!
+* HFF 2020
+* any other game I make</t>
+  </si>
+  <si>
+    <t>* Make a basic interrior of bsb and fully test. 
+* Then make all multilevel buildings an interrior
+* Shouldn't be in here but also from load screen Allow you to save as/copy, and delete files
+* Dictionary with dimension number so you only need to reference that</t>
+  </si>
+  <si>
+    <t>* Making so save/load and all personal game data is kept safe and unhackable 
+* Also probably encrypted is better for online pins, etc
+Write to a file and encrypt it after finishing
+* https://www.guru99.com/reading-and-writing-files-in-python.html
+* https://www.youtube.com/watch?v=xSGnLPTjaXo
+* https://docs.python.org/2/tutorial/inputoutput.html - save structured data
+* Update save files so you write or so you understand pickling
+* change the file extensions and names of folders in EBTA to .EBTA or something random (or blank) to hide or obscure files  (make sure it works)</t>
+  </si>
+  <si>
+    <t>* Make so it takes files automatically
+* gives icon automatically 
+* does code checks out 
+* installer gives desktop icon
+* Overwriting old instal to update would be nice.
+* Try changing the file extensions and names of folders in EBTA to .EBTA or something random (or blank) to hide or obscure files (make sure it works first)</t>
+  </si>
+  <si>
     <t>* Classes, object methods, how map works (numbered adjacency lists), commenting code. Updating to python 3. Interactables class. Buildings as an entity.
 * PP8 style using PyCharm
 * Get rid of global variables and restructure code
 * Using and understanding effecient python code chunks (See Liam F. and his book)
 * Make an entity class (name, description, location, stats, health, item need, item give, inventory, deathtext, etc) and then all subclasses  using inheritance
+* Map
+So we are making a MUD and I didn't know it LOL
+Better than trying to retrofit everything and then you have unique addressing
+Have a linked exit on the spots beside, no need to go inside or anything, just update position and move around
+Map will just constrain itself by where edges are and where you can move
+* Nevada Game engine
+Graph with adjacency list (stored effeciently) that gives the possible options. 
+Using paths with path constructor to translate between points (instead of on-command search). Then maps just become entities addresses by the name.
+For destruction just do pointer to point all old places to the new place (but does damage/kill people when you do destroy a spot)
 * Entity
      Person(each has same attributes and stuff, even schedule would be the same)
           Boss?
@@ -1415,6 +1421,8 @@
      Item
           Interactable
           Interactable can go, just add a moveable flag to items with new entity structute that allows give/take
+* Have a generalized interface class/objects so you don't have to make new ones every time
+* Calling it Mac Quest? McMaster MUD? MMUD
 * See TODO list for rest of rebuild notes</t>
   </si>
   <si>
@@ -1424,31 +1432,104 @@
 * Mashing a key to beat someone.
 *  At least for now someone comes back for round two.
 * Every Person has their own weakness/strengths.
-* Use Darksouls style damage system
+* Use Darksouls style damage system (non-subtractive)
 * Bullet time
 * Maybe have speed play more of a factor, maybe balance in other ways
-* Name everything and attack dialougs (use x to do y)</t>
-  </si>
-  <si>
-    <t>Integrate TODO list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">* Making so save/load and all personal game data is kept safe and unhackable 
-* Also probably encrypted is better for online pins, etc
-Write to a file and encrypt it after finishing
-* https://www.guru99.com/reading-and-writing-files-in-python.html
-* https://www.youtube.com/watch?v=xSGnLPTjaXo
-* https://docs.python.org/2/tutorial/inputoutput.html - save structured data
-* Update save files so you write or so you understand pickling
+* Name everything and attack dialougs (use x to do y)
+* High skill cap mobs you need to farm
+* -more health near end of health bar
+-first bit of damage doesn't actually hurt you a lot
+-hud elements, no health bar just visual indicators
+-all GUI things in dead space are immersed in the game</t>
+  </si>
+  <si>
+    <t>* Adding map and all suplementary info to the GUI (maybe whole game?) so we can customize content. 
+* IDK. I like idea of two window system with map, player icon, pictures, etc on side. 
+* Size of window (ascii art print)
+** All ellements possible are text based
+* Health/other indicators like blood on screen instead of just health bar
+* Every time you launch different load screen background, text colour, font (as long as it looks good) as well as being able to choose</t>
+  </si>
+  <si>
+    <t>* Adding time to game. 
+* Either BOTW 2 min for 1 hr with longest day, or minecraft. I don't think ever step 5 minutes. 
+* In BOTW 2m = 1 hr and very long days. How much in Minecraft?
+* Maybe watch system
+* time based events, 
+* time based characters/moving, etc. 
+* Starting day is 12pm, day after Kipling (for 2017-2018 version).
+* For 2019 version make so have at least a week before kipling</t>
+  </si>
+  <si>
+    <t>* Spelling and grammar check before release (maybe needs a text output function)
+* Don't except empty name
+* "B is back" (Zac)
+* "Dell, Intel Inside"
+* search keyword for search
+* When you inspect the car it says 'Ya thought these were the keys'
+* When you searching when nothings there "You double take and there's still nothing there" (If you search 20 times you die)
+* Make father frobenius and Mario Ponce tovar spelled right with accent
+* See TODO list for all remaining bugs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*-fast addressing like underlining the shortcut, having one letter verrbs, and having be able to pick up things using the number position it was displayed it (maybe display number?). Then can type like "p 1" to pick up first item. Also maybe can do multiple notations like "p 3-6" or "p 3,5,6" or "exa 1,3".  Also make sure the items display in order they were in
+* Make keywords shorter, have list of items to choose from quickly [1-2], maybe accept short names? 
+* Maybe take cardinal coords. 
+* More things rather than equip. 
+* Also possibly controller support?
+* Short word for verbs,  for inv, s for stats
+* Try having WASD and other key accepts (maybe arrow keys) on the GUI acceptable
+* add verb accepts for 2 words and 1 word for
+* add accept for remove, speak, look
+* move, go, run, jog, bike, scate, drive, head
+* add cardinal directions to those directions
+* See if accept accents and other characters in output/input. </t>
+  </si>
+  <si>
+    <t>* Adding an experience level to the game and mobs that respawn so you feel like you're progressing. Probably buffs stats and helps you beat higher level people/things. Also the respawn with golden gauntlet thanos for Paul the buss driver.
+* have SOME sort of leveling/experience system (weapons or yourself)
+Overall level based on exponential EXP and experience gained on Enemy health or quests
+Cows in OSRS respawn based on player count, I'll do random from 0.5-2 mins based on stats/level?
+* In general, have more crazy/dangerous things happen as you progress in quests/storyline (sand worms pop up, idk, crazyness)
+* Could have random drop loot
+* Having fire with cooking be able to cook multiple types of foods (Eggs, meat, bread, ) with BOTW sound
+* Having more combinations of cooking food
+* Having more Runescape cooking, experience levels to unlock/burn less, burn levels, etc
+* Make a really hard boss that is almost impossible to beat (Single High combat class mob or boss for challenge)
+* Talking experience to level up by talking to NPCs (just talk faster? Unlocks the quest? Will say "OKAY OKAY I"LL GIVE YOU WHATEVER YOU WANT")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Adding your dad, Alex Jones, Arnold, Jesse Ventura, auto turrets etc, harry potter ring that can talk to the dead
+* Even more secret place under okons storage place. Leads to underground base.
+* Mike the liar random event. Running across campus saying stuff. Comments on 4th wall things about the game ex) "They need an autocomplete"
+* Stackable Visor Glasses
+* Brendan's jacket holds things in the game
+* scuba Steve (and it's Haugen)
+* Make EpiPen able to save you
+* Big Lez show intercut 00:38:40, 00:49:00
+* Revive life by having a fairy
+* Insanity Update
+ADDED Your dad and Super crocs that show secrets
+Alex Jones 
+Rhomes around
+Brings you down to 1 health unless you have a tin foil hat
+Super Male Vitality
+-5, -5, -5, -5
+has been used by Alex Jones in order to maximize vitality when working up to 12 hours a day or more in the fight for freedom.
+Patriot Blend Medium Roast
+-5,-5,15, 5
+Start your day off right with our gourmet, 100% organic coffee and help us Wake Up America!
+Jesse Ventura
+I'm a peaceful warrior
+I HUNTED PREDITORS IN QUATAMALA.
+I DON"T HAVE TO DO ANYTHING. WHAT ARE YOU MY COMMANDING OFFICER
 </t>
   </si>
   <si>
-    <t>* Make a basic interrior of bsb and fully test. 
-* Then make all multilevel buildings an interrior
-* Shouldn't be in here but also from load screen Allow you to save as/copy, and delete files</t>
-  </si>
-  <si>
-    <t>19 - ✔ Finished integrating feedback and integrating TODO list</t>
+    <t>20 - ✔ Integrated TODO list and EBTA Written work, ready for breakdown</t>
+  </si>
+  <si>
+    <t>BD, 20?</t>
   </si>
 </sst>
 </file>
@@ -1670,7 +1751,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:I58" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A4:I58"/>
   <sortState ref="A5:I58">
-    <sortCondition ref="A4:A58"/>
+    <sortCondition ref="B4:B58"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" name="Feature"/>
@@ -1953,7 +2034,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2025,13 +2106,13 @@
         <v>94</v>
       </c>
       <c r="H9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="I9" s="9">
         <v>45</v>
       </c>
       <c r="J9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2039,22 +2120,22 @@
         <v>97</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G10" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H10">
         <v>330</v>
@@ -2062,80 +2143,80 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>321</v>
+      </c>
+      <c r="B11" t="s">
+        <v>322</v>
+      </c>
+      <c r="C11" t="s">
+        <v>374</v>
+      </c>
+      <c r="D11" t="s">
+        <v>386</v>
+      </c>
+      <c r="E11" t="s">
+        <v>410</v>
+      </c>
+      <c r="F11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" t="s">
+        <v>99</v>
+      </c>
+      <c r="I11" t="s">
         <v>323</v>
-      </c>
-      <c r="B11" t="s">
-        <v>324</v>
-      </c>
-      <c r="C11" t="s">
-        <v>387</v>
-      </c>
-      <c r="D11" t="s">
-        <v>405</v>
-      </c>
-      <c r="E11" t="s">
-        <v>98</v>
-      </c>
-      <c r="F11" t="s">
-        <v>99</v>
-      </c>
-      <c r="G11" t="s">
-        <v>100</v>
-      </c>
-      <c r="I11" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" t="s">
         <v>101</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>102</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>103</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>104</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>105</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>106</v>
       </c>
-      <c r="G12" t="s">
-        <v>107</v>
-      </c>
       <c r="I12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" t="s">
         <v>108</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>109</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>110</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>111</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>112</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>113</v>
       </c>
-      <c r="G13" t="s">
-        <v>114</v>
-      </c>
       <c r="I13" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -2147,7 +2228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
@@ -2403,7 +2484,7 @@
         <v>0.75</v>
       </c>
       <c r="F10" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>14</v>
@@ -2477,7 +2558,7 @@
         <v>0.25</v>
       </c>
       <c r="F14" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2488,7 +2569,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="D15">
         <v>0.28000000000000003</v>
@@ -2497,7 +2578,7 @@
         <v>0.5</v>
       </c>
       <c r="F15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2514,7 +2595,7 @@
         <v>1.5</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2531,7 +2612,7 @@
         <v>0.5</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2585,7 +2666,7 @@
         <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2704,7 +2785,7 @@
         <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="D27">
         <v>0.28999999999999998</v>
@@ -2713,10 +2794,10 @@
         <v>6</v>
       </c>
       <c r="F27" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2733,10 +2814,10 @@
         <v>1.5</v>
       </c>
       <c r="F28" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2753,7 +2834,7 @@
         <v>5</v>
       </c>
       <c r="F29" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2770,10 +2851,10 @@
         <v>0.5</v>
       </c>
       <c r="F30" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="G30" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2790,7 +2871,7 @@
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2807,7 +2888,7 @@
         <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2898,10 +2979,10 @@
         <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="G37" s="14" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2915,10 +2996,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E38" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2935,7 +3016,7 @@
         <v>4</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3102,7 +3183,7 @@
         <v>3</v>
       </c>
       <c r="F49" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -3119,7 +3200,7 @@
         <v>5</v>
       </c>
       <c r="F50" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -3133,10 +3214,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E51" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -3144,7 +3225,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="F54" t="s">
         <v>64</v>
@@ -3175,10 +3256,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P75"/>
+  <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="F72" sqref="F72"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3209,7 +3290,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>22</v>
@@ -3247,31 +3328,16 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>382</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>400</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="H5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I5" t="s">
-        <v>82</v>
+        <v>384</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>7</v>
@@ -3291,29 +3357,18 @@
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6">
-        <v>1.5</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>81</v>
+        <v>357</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>331</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="H6" t="s">
-        <v>86</v>
-      </c>
-      <c r="I6" t="s">
-        <v>87</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="G6" s="10"/>
       <c r="K6" s="1" t="s">
         <v>16</v>
       </c>
@@ -3332,31 +3387,28 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
-        <v>120</v>
-      </c>
       <c r="D7">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>395</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>404</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>117</v>
-      </c>
       <c r="H7" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="I7" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>13</v>
@@ -3376,28 +3428,31 @@
     </row>
     <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>119</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>332</v>
+        <v>399</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H8" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I8" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>14</v>
@@ -3417,28 +3472,28 @@
     </row>
     <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D9">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>125</v>
+        <v>168</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>333</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>156</v>
+        <v>116</v>
       </c>
       <c r="H9" t="s">
-        <v>127</v>
+        <v>169</v>
       </c>
       <c r="I9" t="s">
-        <v>126</v>
+        <v>170</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>17</v>
@@ -3457,29 +3512,30 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E10" t="s">
-        <v>128</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>334</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="H10" t="s">
-        <v>129</v>
-      </c>
-      <c r="I10" t="s">
-        <v>130</v>
+      <c r="A10" s="11">
+        <v>21</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11">
+        <v>4</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>186</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>15</v>
@@ -3499,31 +3555,28 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>133</v>
-      </c>
-      <c r="D11" t="s">
-        <v>132</v>
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>58</v>
+        <v>190</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>373</v>
+        <v>401</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H11" t="s">
-        <v>134</v>
+        <v>194</v>
       </c>
       <c r="I11" t="s">
-        <v>135</v>
+        <v>193</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>11</v>
@@ -3531,31 +3584,28 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>140</v>
-      </c>
-      <c r="D12" t="s">
-        <v>139</v>
-      </c>
       <c r="E12" t="s">
-        <v>138</v>
+        <v>248</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>335</v>
+        <v>362</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="H12" t="s">
-        <v>143</v>
+        <v>249</v>
       </c>
       <c r="I12" t="s">
-        <v>149</v>
+        <v>250</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>76</v>
@@ -3566,31 +3616,28 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>146</v>
-      </c>
-      <c r="D13" t="s">
-        <v>139</v>
+        <v>17</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>145</v>
-      </c>
-      <c r="F13" t="s">
-        <v>336</v>
+        <v>394</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>409</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="H13" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="I13" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>17</v>
@@ -3598,26 +3645,28 @@
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D14">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>206</v>
+        <v>123</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>393</v>
-      </c>
-      <c r="G14" s="10"/>
+        <v>329</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>154</v>
+      </c>
       <c r="H14" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="I14" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>14</v>
@@ -3625,28 +3674,31 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" t="s">
-        <v>154</v>
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>281</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>153</v>
+        <v>179</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="H15" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="I15" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>15</v>
@@ -3654,1090 +3706,1122 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" t="s">
-        <v>338</v>
+        <v>17</v>
+      </c>
+      <c r="D16">
+        <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>374</v>
+        <v>334</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="H16" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="I16" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>159</v>
-      </c>
-      <c r="D17">
-        <v>10</v>
+        <v>281</v>
+      </c>
+      <c r="D17" t="s">
+        <v>237</v>
       </c>
       <c r="E17" t="s">
-        <v>158</v>
+        <v>231</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>386</v>
+        <v>336</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H17" t="s">
-        <v>162</v>
+        <v>241</v>
       </c>
       <c r="I17" t="s">
-        <v>175</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D18">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="H18" t="s">
-        <v>166</v>
-      </c>
-      <c r="I18" t="s">
-        <v>174</v>
+        <v>116</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>169</v>
+        <v>17</v>
       </c>
       <c r="D19">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>167</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>403</v>
+        <v>210</v>
+      </c>
+      <c r="F19" t="s">
+        <v>347</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="H19" t="s">
-        <v>168</v>
-      </c>
-      <c r="I19" t="s">
-        <v>173</v>
+        <v>116</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20">
-        <v>6</v>
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>155</v>
+      </c>
+      <c r="D20" t="s">
+        <v>129</v>
       </c>
       <c r="E20" t="s">
-        <v>170</v>
+        <v>307</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>339</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="H20" t="s">
-        <v>171</v>
-      </c>
-      <c r="I20" t="s">
-        <v>172</v>
-      </c>
+        <v>356</v>
+      </c>
+      <c r="G20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>132</v>
+        <v>411</v>
       </c>
       <c r="E21" t="s">
-        <v>177</v>
+        <v>126</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>340</v>
+        <v>408</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>178</v>
+        <v>116</v>
       </c>
       <c r="H21" t="s">
-        <v>179</v>
+        <v>127</v>
       </c>
       <c r="I21" t="s">
-        <v>180</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>283</v>
-      </c>
-      <c r="D22">
-        <v>15</v>
+        <v>131</v>
+      </c>
+      <c r="D22" t="s">
+        <v>130</v>
       </c>
       <c r="E22" t="s">
-        <v>181</v>
+        <v>58</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="H22" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="I22" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D23">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>341</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>122</v>
-      </c>
+        <v>407</v>
+      </c>
+      <c r="G23" s="10"/>
       <c r="H23" t="s">
-        <v>185</v>
+        <v>148</v>
       </c>
       <c r="I23" t="s">
-        <v>186</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>190</v>
+        <v>332</v>
       </c>
       <c r="E24" t="s">
-        <v>187</v>
-      </c>
-      <c r="F24" t="s">
-        <v>342</v>
+        <v>155</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>397</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="H24" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
       <c r="I24" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
-        <v>21</v>
-      </c>
-      <c r="B25" s="12" t="s">
+      <c r="A25">
         <v>13</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11">
-        <v>4</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="I25" s="11" t="s">
-        <v>188</v>
+      <c r="B25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" t="s">
+        <v>157</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>156</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>396</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="H25" t="s">
+        <v>160</v>
+      </c>
+      <c r="I25" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="C26" t="s">
+        <v>163</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>343</v>
+        <v>405</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H26" t="s">
-        <v>196</v>
+        <v>164</v>
       </c>
       <c r="I26" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>268</v>
+        <v>155</v>
       </c>
       <c r="D27" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E27" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>371</v>
+        <v>337</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="H27" t="s">
-        <v>238</v>
-      </c>
-      <c r="I27" t="s">
-        <v>237</v>
+        <v>116</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>164</v>
-      </c>
-      <c r="D28">
-        <v>10</v>
+        <v>85</v>
+      </c>
+      <c r="D28" t="s">
+        <v>80</v>
       </c>
       <c r="E28" t="s">
-        <v>232</v>
+        <v>79</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>347</v>
+        <v>402</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>240</v>
+        <v>84</v>
       </c>
       <c r="H28" t="s">
-        <v>241</v>
+        <v>83</v>
       </c>
       <c r="I28" t="s">
-        <v>242</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>283</v>
+        <v>138</v>
       </c>
       <c r="D29" t="s">
-        <v>239</v>
+        <v>137</v>
       </c>
       <c r="E29" t="s">
-        <v>233</v>
+        <v>136</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="H29" t="s">
-        <v>243</v>
+        <v>141</v>
       </c>
       <c r="I29" t="s">
-        <v>244</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="D30" t="s">
-        <v>245</v>
+        <v>137</v>
       </c>
       <c r="E30" t="s">
-        <v>229</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>345</v>
+        <v>143</v>
+      </c>
+      <c r="F30" t="s">
+        <v>331</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="I30" s="14" t="s">
-        <v>247</v>
+        <v>142</v>
+      </c>
+      <c r="H30" t="s">
+        <v>145</v>
+      </c>
+      <c r="I30" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D31">
-        <v>8</v>
+      <c r="D31" t="s">
+        <v>152</v>
       </c>
       <c r="E31" t="s">
-        <v>227</v>
+        <v>151</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>346</v>
+        <v>403</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="I31" s="14" t="s">
-        <v>249</v>
+        <v>153</v>
+      </c>
+      <c r="H31" t="s">
+        <v>158</v>
+      </c>
+      <c r="I31" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>200</v>
+        <v>167</v>
       </c>
       <c r="D32">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>199</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>390</v>
+        <v>165</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>400</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="H32" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="I32" s="14" t="s">
-        <v>186</v>
+        <v>153</v>
+      </c>
+      <c r="H32" t="s">
+        <v>166</v>
+      </c>
+      <c r="I32" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D33">
-        <v>6</v>
+      <c r="C33" t="s">
+        <v>389</v>
+      </c>
+      <c r="D33" t="s">
+        <v>130</v>
       </c>
       <c r="E33" t="s">
-        <v>201</v>
-      </c>
-      <c r="F33" t="s">
-        <v>348</v>
+        <v>175</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>392</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="H33" s="14" t="s">
-        <v>254</v>
-      </c>
-      <c r="I33" s="14" t="s">
-        <v>135</v>
+        <v>176</v>
+      </c>
+      <c r="H33" t="s">
+        <v>177</v>
+      </c>
+      <c r="I33" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C34" t="s">
-        <v>256</v>
-      </c>
-      <c r="D34">
-        <v>16</v>
+      <c r="D34" t="s">
+        <v>188</v>
       </c>
       <c r="E34" t="s">
-        <v>202</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>349</v>
+        <v>185</v>
+      </c>
+      <c r="F34" t="s">
+        <v>335</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="H34" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="I34" s="14" t="s">
-        <v>258</v>
+        <v>139</v>
+      </c>
+      <c r="H34" t="s">
+        <v>187</v>
+      </c>
+      <c r="I34" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D35">
-        <v>20</v>
+      <c r="C35" t="s">
+        <v>266</v>
+      </c>
+      <c r="D35" t="s">
+        <v>237</v>
       </c>
       <c r="E35" t="s">
-        <v>330</v>
+        <v>229</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>259</v>
-      </c>
-      <c r="H35" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="I35" s="14" t="s">
-        <v>261</v>
+        <v>140</v>
+      </c>
+      <c r="H35" t="s">
+        <v>236</v>
+      </c>
+      <c r="I35" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="C36" t="s">
+        <v>162</v>
       </c>
       <c r="D36">
         <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>207</v>
+        <v>230</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="H36" s="14" t="s">
-        <v>264</v>
-      </c>
-      <c r="I36" s="14" t="s">
-        <v>262</v>
+        <v>238</v>
+      </c>
+      <c r="H36" t="s">
+        <v>239</v>
+      </c>
+      <c r="I36" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D37">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E37" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>392</v>
+        <v>338</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>265</v>
+        <v>238</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>266</v>
+        <v>246</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>318</v>
+        <v>247</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C38" t="s">
-        <v>164</v>
+        <v>198</v>
       </c>
       <c r="D38">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E38" t="s">
-        <v>208</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>353</v>
+        <v>197</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>377</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C39" t="s">
-        <v>268</v>
-      </c>
       <c r="D39">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E39" t="s">
-        <v>209</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>354</v>
+        <v>199</v>
+      </c>
+      <c r="F39" t="s">
+        <v>340</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>269</v>
+        <v>153</v>
       </c>
       <c r="H39" s="14" t="s">
-        <v>276</v>
+        <v>252</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>275</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C40" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="D40">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E40" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>394</v>
+        <v>341</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>277</v>
+        <v>253</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>278</v>
+        <v>255</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>279</v>
+        <v>256</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D41">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E41" t="s">
-        <v>211</v>
+        <v>328</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>355</v>
+        <v>342</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>280</v>
+        <v>257</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>282</v>
+        <v>259</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D42">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E42" t="s">
-        <v>212</v>
-      </c>
-      <c r="F42" t="s">
-        <v>356</v>
+        <v>205</v>
+      </c>
+      <c r="F42" s="14" t="s">
+        <v>388</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>117</v>
+        <v>261</v>
       </c>
       <c r="H42" s="14" t="s">
-        <v>284</v>
+        <v>262</v>
       </c>
       <c r="I42" s="14" t="s">
-        <v>285</v>
+        <v>260</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D43">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E43" t="s">
         <v>214</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>357</v>
+        <v>379</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>290</v>
+        <v>264</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>289</v>
+        <v>316</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C44" t="s">
-        <v>292</v>
-      </c>
-      <c r="D44" t="s">
-        <v>291</v>
+        <v>266</v>
+      </c>
+      <c r="D44">
+        <v>12</v>
       </c>
       <c r="E44" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>358</v>
+        <v>345</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>297</v>
+        <v>274</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>176</v>
+        <v>273</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C45" t="s">
-        <v>300</v>
-      </c>
-      <c r="D45" t="s">
-        <v>299</v>
+        <v>266</v>
+      </c>
+      <c r="D45">
+        <v>20</v>
       </c>
       <c r="E45" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>359</v>
+        <v>380</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="H45" s="14" t="s">
-        <v>301</v>
+        <v>276</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>298</v>
+        <v>277</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D46" t="s">
-        <v>302</v>
+      <c r="D46">
+        <v>10</v>
       </c>
       <c r="E46" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>360</v>
+        <v>346</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>303</v>
+        <v>279</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>304</v>
+        <v>280</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D47" t="s">
-        <v>299</v>
+      <c r="D47">
+        <v>10</v>
       </c>
       <c r="E47" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="G47" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="I47" s="14" t="s">
         <v>287</v>
-      </c>
-      <c r="H47" s="14" t="s">
-        <v>306</v>
-      </c>
-      <c r="I47" s="14" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C48" t="s">
+        <v>290</v>
+      </c>
       <c r="D48" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="E48" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>144</v>
+        <v>275</v>
       </c>
       <c r="H48" s="14" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>308</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="D49" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="E49" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>259</v>
+        <v>284</v>
       </c>
       <c r="H49" s="14" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="E50" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>322</v>
+        <v>297</v>
       </c>
       <c r="E51" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="D52" t="s">
+        <v>300</v>
       </c>
       <c r="E52" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>372</v>
+        <v>343</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="H52" t="s">
-        <v>251</v>
-      </c>
-      <c r="I52" t="s">
-        <v>252</v>
+        <v>142</v>
+      </c>
+      <c r="H52" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="I52" s="14" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C53" t="s">
+        <v>311</v>
+      </c>
       <c r="D53" t="s">
-        <v>294</v>
+        <v>308</v>
       </c>
       <c r="E53" t="s">
-        <v>293</v>
+        <v>224</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="H53" t="s">
-        <v>296</v>
-      </c>
-      <c r="I53" t="s">
-        <v>295</v>
+        <v>257</v>
+      </c>
+      <c r="H53" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="I53" s="14" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="D54" t="s">
+        <v>312</v>
       </c>
       <c r="E54" t="s">
-        <v>396</v>
+        <v>232</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>399</v>
+        <v>354</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="H54" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="I54" s="14" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C55" t="s">
-        <v>157</v>
+        <v>15</v>
       </c>
       <c r="D55" t="s">
-        <v>131</v>
+        <v>320</v>
       </c>
       <c r="E55" t="s">
-        <v>309</v>
+        <v>233</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>366</v>
-      </c>
-      <c r="G55" s="10"/>
+        <v>355</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="H55" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="I55" s="14" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="D56" t="s">
+        <v>292</v>
       </c>
       <c r="E56" t="s">
-        <v>367</v>
+        <v>291</v>
       </c>
       <c r="F56" s="14" t="s">
         <v>398</v>
       </c>
-      <c r="G56" s="10"/>
+      <c r="G56" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="H56" t="s">
+        <v>294</v>
+      </c>
+      <c r="I56" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
@@ -4747,10 +4831,10 @@
         <v>15</v>
       </c>
       <c r="E57" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>389</v>
+        <v>376</v>
       </c>
       <c r="G57" s="10"/>
     </row>
@@ -4758,11 +4842,31 @@
       <c r="A58">
         <v>53</v>
       </c>
-      <c r="F58" s="14"/>
+      <c r="B58" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" t="s">
+        <v>266</v>
+      </c>
+      <c r="E58" t="s">
+        <v>389</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="G58" t="s">
+        <v>176</v>
+      </c>
+      <c r="H58" t="s">
+        <v>391</v>
+      </c>
+      <c r="I58" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="65" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E65" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" spans="4:6" x14ac:dyDescent="0.25">
@@ -4772,50 +4876,55 @@
     </row>
     <row r="67" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D67" s="11" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="68" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D68" s="11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="69" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D69" s="11" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="70" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D70" s="19" t="s">
-        <v>402</v>
+      <c r="D70" s="11" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="71" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D71" t="s">
-        <v>271</v>
+      <c r="D71" s="11" t="s">
+        <v>387</v>
       </c>
     </row>
     <row r="72" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>272</v>
-      </c>
-      <c r="F72" t="s">
-        <v>397</v>
+        <v>269</v>
       </c>
     </row>
     <row r="73" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
-        <v>317</v>
+        <v>270</v>
+      </c>
+      <c r="F73" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="74" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E74" t="s">
-        <v>316</v>
+      <c r="D74" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="75" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D75" t="s">
-        <v>329</v>
+      <c r="E75" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="76" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>327</v>
       </c>
     </row>
   </sheetData>
@@ -4823,7 +4932,7 @@
     <sortCondition descending="1" ref="O5"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B57">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B58">
       <formula1>$K$5:$K$10</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Started whiteboarding list. Next will be writing up list and actually breaking things down into tasks.
</commit_message>
<xml_diff>
--- a/Dev/EBTA Developent Roadmap.xlsx
+++ b/Dev/EBTA Developent Roadmap.xlsx
@@ -327,12 +327,6 @@
     <t>9 -</t>
   </si>
   <si>
-    <t>21 -</t>
-  </si>
-  <si>
-    <t>22 -</t>
-  </si>
-  <si>
     <t>23 -</t>
   </si>
   <si>
@@ -661,9 +655,6 @@
   </si>
   <si>
     <t>GTA Police</t>
-  </si>
-  <si>
-    <t>Text Display</t>
   </si>
   <si>
     <t>Some sort of skill component to fighting</t>
@@ -1123,9 +1114,6 @@
 * eventually have to escape on rocket in smoke stack to go meet Elon musk on the moon</t>
   </si>
   <si>
-    <t>* GUI text printer, change colour, font, style of words to highlight.</t>
-  </si>
-  <si>
     <t>* Involves lore from the skate video
 . You see a campus police guard pull up to talk to someone on the skateboard.
 "Erik the Sk8r: Hey Bill"
@@ -1280,23 +1268,6 @@
   </si>
   <si>
     <t>Finished Feature lock so all future features go marked as not in this update</t>
-  </si>
-  <si>
-    <t>* Error checking to see if place exists before moving
-* Wear earphones on head
-* 3W text in QT
-* Add Nicole to EP office
-* Wacky items are good
-* 3BB PID with MSP430
-* Have Brendan Fallon character with eclipse mug, rocketry t-shirt, Strainer on head?SafetyGlasses?, and iron ring (more characters)
-* Giving context about 3W text and also have more things tell you about phoneix and also items (More use of storyline, music, definition to people to give realism to the world)
-* After giving dirty needle to sharp exchange a random encounter with a person that says "You're the greatest semaritan in the world" and gives you and Uzi
-* Need to know that Jana has the textbook, maybe the story should say that somewhere
-* Not obveous that equip means to pick up
-* Phil says that need to be pushed more toward the Phenoix (more people you talk to, or items, tell story about the Phoneix)
-** Tyler wants it to be Sandbox mode, no linear stuff, events unfold from there
-* Expand on the Story and the high council so they can piece everything together
-* See TODO list for all remaining bugs</t>
   </si>
   <si>
     <t>Integrate TODO list</t>
@@ -1358,16 +1329,6 @@
 * ability for characters to play audio when you talk to them
 * Make high pitch willhelm screen when women die
 </t>
-  </si>
-  <si>
-    <t>*Year selector
-* tutorial
-* intro
-* Map/characters ( Measure Alice or Bob &amp; they collapse, also DOD)
-* BSB Dungeon
-* storyline/quests. This is a substantial piece of work
-* See Google Keep notes on the story
-* BSB IS A DUNGEON WITH KEYS (EITHER UNIQUE OR NOT )</t>
   </si>
   <si>
     <t>* Convert the game to Matlab to play!
@@ -1530,6 +1491,45 @@
   </si>
   <si>
     <t>BD, 20?</t>
+  </si>
+  <si>
+    <t>*Year selector
+* tutorial
+* intro
+* Map/characters ( Measure Alice or Bob &amp; they collapse, also DOD)
+* BSB Dungeon
+* storyline/quests. This is a substantial piece of work
+* See Google Keep notes on the story
+* BSB IS A DUNGEON WITH KEYS (EITHER UNIQUE OR NOT )
+* Have Brendan Fallon character with eclipse mug, rocketry t-shirt, Strainer on head?SafetyGlasses?, and iron ring (more characters)</t>
+  </si>
+  <si>
+    <t>* Error checking to see if place exists before moving
+* Wear earphones on head
+* 3W text in QT
+* Add Nicole to EP office
+* Wacky items are good
+* 3BB PID with MSP430
+* Giving context about 3W text and also have more things tell you about phoneix and also items (More use of storyline, music, definition to people to give realism to the world)
+* After giving dirty needle to sharp exchange a random encounter with a person that says "You're the greatest semaritan in the world" and gives you and Uzi
+* Need to know that Jana has the textbook, maybe the story should say that somewhere
+* Not obveous that equip means to pick up
+* Phil says that need to be pushed more toward the Phenoix (more people you talk to, or items, tell story about the Phoneix)
+** Tyler wants it to be Sandbox mode, no linear stuff, events unfold from there
+* Expand on the Story and the high council so they can piece everything together
+* See TODO list for all remaining bugs</t>
+  </si>
+  <si>
+    <t>Text Display on GUI</t>
+  </si>
+  <si>
+    <t>* GUI text printer/input, change colour, font, style of words to highlight.</t>
+  </si>
+  <si>
+    <t>21 - ✔ Started whiteboarding list. Next will be writing up list and actually breaking things down into tasks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22 - </t>
   </si>
 </sst>
 </file>
@@ -2034,7 +2034,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,13 +2106,13 @@
         <v>94</v>
       </c>
       <c r="H9" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="I9" s="9">
         <v>45</v>
       </c>
       <c r="J9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2120,22 +2120,22 @@
         <v>97</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E10" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F10" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G10" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="H10">
         <v>330</v>
@@ -2143,80 +2143,83 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B11" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C11" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D11" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="E11" t="s">
+        <v>404</v>
+      </c>
+      <c r="F11" t="s">
         <v>410</v>
       </c>
-      <c r="F11" t="s">
-        <v>98</v>
-      </c>
       <c r="G11" t="s">
-        <v>99</v>
+        <v>411</v>
+      </c>
+      <c r="H11">
+        <v>195</v>
       </c>
       <c r="I11" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" t="s">
         <v>100</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>101</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>102</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>103</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>104</v>
       </c>
-      <c r="F12" t="s">
-        <v>105</v>
-      </c>
-      <c r="G12" t="s">
-        <v>106</v>
-      </c>
       <c r="I12" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C13" t="s">
         <v>107</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>108</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>109</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
         <v>110</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>111</v>
       </c>
-      <c r="F13" t="s">
-        <v>112</v>
-      </c>
-      <c r="G13" t="s">
-        <v>113</v>
-      </c>
       <c r="I13" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
   </sheetData>
@@ -2484,7 +2487,7 @@
         <v>0.75</v>
       </c>
       <c r="F10" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>14</v>
@@ -2558,7 +2561,7 @@
         <v>0.25</v>
       </c>
       <c r="F14" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2569,7 +2572,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D15">
         <v>0.28000000000000003</v>
@@ -2578,7 +2581,7 @@
         <v>0.5</v>
       </c>
       <c r="F15" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2595,7 +2598,7 @@
         <v>1.5</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2612,7 +2615,7 @@
         <v>0.5</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2666,7 +2669,7 @@
         <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2785,7 +2788,7 @@
         <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D27">
         <v>0.28999999999999998</v>
@@ -2794,10 +2797,10 @@
         <v>6</v>
       </c>
       <c r="F27" t="s">
+        <v>359</v>
+      </c>
+      <c r="G27" s="14" t="s">
         <v>363</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2814,10 +2817,10 @@
         <v>1.5</v>
       </c>
       <c r="F28" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2834,7 +2837,7 @@
         <v>5</v>
       </c>
       <c r="F29" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2851,10 +2854,10 @@
         <v>0.5</v>
       </c>
       <c r="F30" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="G30" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2871,7 +2874,7 @@
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2888,7 +2891,7 @@
         <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2979,10 +2982,10 @@
         <v>2</v>
       </c>
       <c r="F37" t="s">
+        <v>360</v>
+      </c>
+      <c r="G37" s="14" t="s">
         <v>364</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2996,10 +2999,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E38" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3016,7 +3019,7 @@
         <v>4</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3183,7 +3186,7 @@
         <v>3</v>
       </c>
       <c r="F49" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -3200,7 +3203,7 @@
         <v>5</v>
       </c>
       <c r="F50" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -3214,10 +3217,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E51" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -3225,7 +3228,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="F54" t="s">
         <v>64</v>
@@ -3258,8 +3261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3290,7 +3293,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>22</v>
@@ -3334,10 +3337,10 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>384</v>
+        <v>407</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>7</v>
@@ -3363,10 +3366,10 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="G6" s="10"/>
       <c r="K6" s="1" t="s">
@@ -3399,10 +3402,10 @@
         <v>81</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H7" t="s">
         <v>86</v>
@@ -3434,25 +3437,25 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H8" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" t="s">
         <v>115</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>399</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="H8" t="s">
-        <v>118</v>
-      </c>
-      <c r="I8" t="s">
-        <v>117</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>14</v>
@@ -3481,19 +3484,19 @@
         <v>6</v>
       </c>
       <c r="E9" t="s">
+        <v>166</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H9" t="s">
+        <v>167</v>
+      </c>
+      <c r="I9" t="s">
         <v>168</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>333</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="H9" t="s">
-        <v>169</v>
-      </c>
-      <c r="I9" t="s">
-        <v>170</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>17</v>
@@ -3523,19 +3526,19 @@
         <v>4</v>
       </c>
       <c r="E10" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="F10" s="11" t="s">
-        <v>191</v>
-      </c>
       <c r="G10" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>15</v>
@@ -3564,19 +3567,19 @@
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H11" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I11" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>11</v>
@@ -3593,19 +3596,19 @@
         <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H12" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="I12" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>76</v>
@@ -3625,19 +3628,19 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="G13" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="H13" t="s">
+        <v>119</v>
+      </c>
+      <c r="I13" t="s">
         <v>120</v>
-      </c>
-      <c r="H13" t="s">
-        <v>121</v>
-      </c>
-      <c r="I13" t="s">
-        <v>122</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>17</v>
@@ -3654,19 +3657,19 @@
         <v>15</v>
       </c>
       <c r="E14" t="s">
+        <v>121</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="H14" t="s">
         <v>123</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>329</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="H14" t="s">
-        <v>125</v>
-      </c>
       <c r="I14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>14</v>
@@ -3674,31 +3677,28 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C15" t="s">
-        <v>281</v>
-      </c>
       <c r="D15">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>381</v>
+        <v>331</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H15" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>15</v>
@@ -3706,325 +3706,331 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C16" t="s">
+        <v>196</v>
+      </c>
       <c r="D16">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
+        <v>195</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="I16" s="14" t="s">
         <v>182</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>334</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="H16" t="s">
-        <v>183</v>
-      </c>
-      <c r="I16" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>281</v>
-      </c>
-      <c r="D17" t="s">
-        <v>237</v>
+        <v>160</v>
+      </c>
+      <c r="D17">
+        <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>231</v>
+        <v>204</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="H17" t="s">
-        <v>241</v>
-      </c>
-      <c r="I17" t="s">
-        <v>242</v>
+        <v>114</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>162</v>
-      </c>
-      <c r="D18">
-        <v>6</v>
+        <v>153</v>
+      </c>
+      <c r="D18" t="s">
+        <v>127</v>
       </c>
       <c r="E18" t="s">
-        <v>206</v>
+        <v>304</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>344</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>265</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>133</v>
-      </c>
+        <v>352</v>
+      </c>
+      <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>405</v>
       </c>
       <c r="E19" t="s">
-        <v>210</v>
-      </c>
-      <c r="F19" t="s">
-        <v>347</v>
+        <v>124</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>402</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>282</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>283</v>
+        <v>114</v>
+      </c>
+      <c r="H19" t="s">
+        <v>125</v>
+      </c>
+      <c r="I19" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="D20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E20" t="s">
-        <v>307</v>
+        <v>58</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>356</v>
-      </c>
-      <c r="G20" s="10"/>
+        <v>398</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H20" t="s">
+        <v>130</v>
+      </c>
+      <c r="I20" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D21" t="s">
-        <v>411</v>
+      <c r="D21">
+        <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>126</v>
+        <v>202</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>408</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>116</v>
-      </c>
+        <v>401</v>
+      </c>
+      <c r="G21" s="10"/>
       <c r="H21" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="I21" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C22" t="s">
-        <v>131</v>
-      </c>
       <c r="D22" t="s">
-        <v>130</v>
+        <v>329</v>
       </c>
       <c r="E22" t="s">
-        <v>58</v>
+        <v>153</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H22" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
       <c r="I22" t="s">
-        <v>133</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C23" t="s">
+        <v>155</v>
+      </c>
       <c r="D23">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E23" t="s">
-        <v>204</v>
+        <v>154</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>407</v>
-      </c>
-      <c r="G23" s="10"/>
+        <v>391</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>114</v>
+      </c>
       <c r="H23" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="I23" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D24" t="s">
-        <v>332</v>
+      <c r="C24" t="s">
+        <v>161</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H24" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I24" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>157</v>
-      </c>
-      <c r="D25">
-        <v>10</v>
+        <v>278</v>
+      </c>
+      <c r="D25" t="s">
+        <v>234</v>
       </c>
       <c r="E25" t="s">
-        <v>156</v>
+        <v>228</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>396</v>
+        <v>333</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H25" t="s">
-        <v>160</v>
+        <v>238</v>
       </c>
       <c r="I25" t="s">
-        <v>173</v>
+        <v>239</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>163</v>
-      </c>
-      <c r="D26">
-        <v>10</v>
+        <v>153</v>
+      </c>
+      <c r="D26" t="s">
+        <v>240</v>
       </c>
       <c r="E26" t="s">
-        <v>162</v>
+        <v>224</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>405</v>
+        <v>334</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="H26" t="s">
-        <v>164</v>
-      </c>
-      <c r="I26" t="s">
-        <v>172</v>
+        <v>114</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>155</v>
-      </c>
-      <c r="D27" t="s">
-        <v>243</v>
+        <v>278</v>
+      </c>
+      <c r="D27">
+        <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>227</v>
+        <v>177</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>337</v>
+        <v>377</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="I27" s="14" t="s">
-        <v>245</v>
+        <v>118</v>
+      </c>
+      <c r="H27" t="s">
+        <v>178</v>
+      </c>
+      <c r="I27" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -4044,7 +4050,7 @@
         <v>79</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>84</v>
@@ -4064,25 +4070,25 @@
         <v>15</v>
       </c>
       <c r="C29" t="s">
+        <v>136</v>
+      </c>
+      <c r="D29" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" t="s">
+        <v>134</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="G29" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="D29" t="s">
-        <v>137</v>
-      </c>
-      <c r="E29" t="s">
-        <v>136</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>330</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>140</v>
-      </c>
       <c r="H29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="I29" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -4093,25 +4099,25 @@
         <v>15</v>
       </c>
       <c r="C30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" t="s">
+        <v>135</v>
+      </c>
+      <c r="E30" t="s">
+        <v>141</v>
+      </c>
+      <c r="F30" t="s">
+        <v>328</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="H30" t="s">
+        <v>143</v>
+      </c>
+      <c r="I30" t="s">
         <v>144</v>
-      </c>
-      <c r="D30" t="s">
-        <v>137</v>
-      </c>
-      <c r="E30" t="s">
-        <v>143</v>
-      </c>
-      <c r="F30" t="s">
-        <v>331</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="H30" t="s">
-        <v>145</v>
-      </c>
-      <c r="I30" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -4122,22 +4128,22 @@
         <v>15</v>
       </c>
       <c r="D31" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E31" t="s">
+        <v>149</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="G31" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="F31" s="14" t="s">
-        <v>403</v>
-      </c>
-      <c r="G31" s="10" t="s">
-        <v>153</v>
-      </c>
       <c r="H31" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I31" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -4148,25 +4154,25 @@
         <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D32">
         <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I32" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -4177,25 +4183,25 @@
         <v>15</v>
       </c>
       <c r="C33" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="D33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E33" t="s">
+        <v>173</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="H33" t="s">
         <v>175</v>
       </c>
-      <c r="F33" s="14" t="s">
-        <v>392</v>
-      </c>
-      <c r="G33" s="10" t="s">
+      <c r="I33" t="s">
         <v>176</v>
-      </c>
-      <c r="H33" t="s">
-        <v>177</v>
-      </c>
-      <c r="I33" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -4206,22 +4212,22 @@
         <v>15</v>
       </c>
       <c r="D34" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E34" t="s">
+        <v>183</v>
+      </c>
+      <c r="F34" t="s">
+        <v>332</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="H34" t="s">
         <v>185</v>
       </c>
-      <c r="F34" t="s">
-        <v>335</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="H34" t="s">
-        <v>187</v>
-      </c>
       <c r="I34" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -4232,25 +4238,25 @@
         <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D35" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E35" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H35" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="I35" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -4261,25 +4267,25 @@
         <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D36">
         <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H36" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="I36" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -4293,97 +4299,94 @@
         <v>8</v>
       </c>
       <c r="E37" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C38" t="s">
-        <v>198</v>
-      </c>
       <c r="D38">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E38" t="s">
         <v>197</v>
       </c>
-      <c r="F38" s="18" t="s">
-        <v>377</v>
+      <c r="F38" t="s">
+        <v>337</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>184</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C39" t="s">
+        <v>251</v>
+      </c>
       <c r="D39">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E39" t="s">
-        <v>199</v>
-      </c>
-      <c r="F39" t="s">
-        <v>340</v>
+        <v>198</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>338</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>153</v>
+        <v>250</v>
       </c>
       <c r="H39" s="14" t="s">
         <v>252</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>133</v>
+        <v>253</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40">
+        <v>20</v>
+      </c>
+      <c r="E40" t="s">
+        <v>325</v>
+      </c>
+      <c r="F40" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="G40" s="10" t="s">
         <v>254</v>
-      </c>
-      <c r="D40">
-        <v>16</v>
-      </c>
-      <c r="E40" t="s">
-        <v>200</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>341</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>253</v>
       </c>
       <c r="H40" s="14" t="s">
         <v>255</v>
@@ -4394,129 +4397,129 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D41">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E41" t="s">
-        <v>328</v>
+        <v>203</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>342</v>
+        <v>383</v>
       </c>
       <c r="G41" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="H41" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="I41" s="14" t="s">
         <v>257</v>
-      </c>
-      <c r="H41" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="I41" s="14" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D42">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E42" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
       <c r="G42" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="H42" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="H42" s="14" t="s">
-        <v>262</v>
-      </c>
       <c r="I42" s="14" t="s">
-        <v>260</v>
+        <v>313</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C43" t="s">
+        <v>263</v>
+      </c>
       <c r="D43">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E43" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>379</v>
+        <v>342</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>316</v>
+        <v>270</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C44" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D44">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E44" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>345</v>
+        <v>376</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="H44" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="I44" s="14" t="s">
         <v>274</v>
-      </c>
-      <c r="I44" s="14" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C45" t="s">
-        <v>266</v>
-      </c>
       <c r="D45">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>380</v>
+        <v>343</v>
       </c>
       <c r="G45" s="10" t="s">
         <v>275</v>
@@ -4530,22 +4533,22 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D46">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E46" t="s">
-        <v>209</v>
-      </c>
-      <c r="F46" s="14" t="s">
-        <v>346</v>
+        <v>408</v>
+      </c>
+      <c r="F46" t="s">
+        <v>409</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>278</v>
+        <v>114</v>
       </c>
       <c r="H46" s="14" t="s">
         <v>279</v>
@@ -4565,19 +4568,19 @@
         <v>10</v>
       </c>
       <c r="E47" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="H47" s="14" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -4588,25 +4591,25 @@
         <v>15</v>
       </c>
       <c r="C48" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D48" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E48" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="H48" s="14" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -4617,25 +4620,25 @@
         <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D49" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E49" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="H49" s="14" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -4646,22 +4649,22 @@
         <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E50" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -4672,22 +4675,22 @@
         <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E51" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -4698,22 +4701,22 @@
         <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E52" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H52" s="14" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -4724,25 +4727,25 @@
         <v>15</v>
       </c>
       <c r="C53" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D53" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E53" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H53" s="14" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -4753,22 +4756,22 @@
         <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="E54" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="H54" s="14" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="I54" s="14" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -4779,22 +4782,22 @@
         <v>15</v>
       </c>
       <c r="D55" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E55" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="H55" s="14" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="I55" s="14" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -4805,22 +4808,22 @@
         <v>15</v>
       </c>
       <c r="D56" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="E56" t="s">
+        <v>288</v>
+      </c>
+      <c r="F56" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="H56" t="s">
         <v>291</v>
       </c>
-      <c r="F56" s="14" t="s">
-        <v>398</v>
-      </c>
-      <c r="G56" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="H56" t="s">
-        <v>294</v>
-      </c>
       <c r="I56" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -4831,10 +4834,10 @@
         <v>15</v>
       </c>
       <c r="E57" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="G57" s="10"/>
     </row>
@@ -4846,27 +4849,27 @@
         <v>15</v>
       </c>
       <c r="C58" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E58" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="G58" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H58" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="I58" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="65" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E65" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="66" spans="4:6" x14ac:dyDescent="0.25">
@@ -4876,55 +4879,55 @@
     </row>
     <row r="67" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D67" s="11" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="68" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D68" s="11" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="69" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D69" s="11" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="70" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D70" s="11" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="71" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D71" s="11" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="72" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="73" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="F73" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="74" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="75" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E75" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="76" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Transferred List and did macro schedule. S*** is bad
</commit_message>
<xml_diff>
--- a/Dev/EBTA Developent Roadmap.xlsx
+++ b/Dev/EBTA Developent Roadmap.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\bflaw\Documents\GitHub\EngPhysAdventure\Dev\"/>
@@ -15,7 +15,9 @@
     <sheet name="Outline" sheetId="2" r:id="rId1"/>
     <sheet name="Feedback" sheetId="1" r:id="rId2"/>
     <sheet name="Alpha 0.30 Feature Lock" sheetId="4" r:id="rId3"/>
-    <sheet name="Habit Diagram" sheetId="3" r:id="rId4"/>
+    <sheet name="Alpha 0.30 Feature List" sheetId="5" r:id="rId4"/>
+    <sheet name="Alpha 0.30 Scheduling" sheetId="6" r:id="rId5"/>
+    <sheet name="Habit Diagram" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Alpha 0.30 Feature Lock'!$A$4:$I$54</definedName>
@@ -26,12 +28,18 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="482">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -325,21 +333,6 @@
   </si>
   <si>
     <t>9 -</t>
-  </si>
-  <si>
-    <t>23 -</t>
-  </si>
-  <si>
-    <t>24 -</t>
-  </si>
-  <si>
-    <t>25 -</t>
-  </si>
-  <si>
-    <t>26 -</t>
-  </si>
-  <si>
-    <t>27 -</t>
   </si>
   <si>
     <t>28 -</t>
@@ -1022,9 +1015,6 @@
   </si>
   <si>
     <t>* Make other players be able to interact, fight, talk to eachother</t>
-  </si>
-  <si>
-    <t>BD, 15+10+8+15+20?</t>
   </si>
   <si>
     <t>* Making so surroundings of obveous areas print out. 
@@ -1262,9 +1252,6 @@
 * Map display better
 * quest progress tracker, can give hints on where to go/where things are
 * Ingame journal or notes function.</t>
-  </si>
-  <si>
-    <t>Map/Items/People/Quests</t>
   </si>
   <si>
     <t>Finished Feature lock so all future features go marked as not in this update</t>
@@ -1422,17 +1409,6 @@
 * For 2019 version make so have at least a week before kipling</t>
   </si>
   <si>
-    <t>* Spelling and grammar check before release (maybe needs a text output function)
-* Don't except empty name
-* "B is back" (Zac)
-* "Dell, Intel Inside"
-* search keyword for search
-* When you inspect the car it says 'Ya thought these were the keys'
-* When you searching when nothings there "You double take and there's still nothing there" (If you search 20 times you die)
-* Make father frobenius and Mario Ponce tovar spelled right with accent
-* See TODO list for all remaining bugs</t>
-  </si>
-  <si>
     <t xml:space="preserve">*-fast addressing like underlining the shortcut, having one letter verrbs, and having be able to pick up things using the number position it was displayed it (maybe display number?). Then can type like "p 1" to pick up first item. Also maybe can do multiple notations like "p 3-6" or "p 3,5,6" or "exa 1,3".  Also make sure the items display in order they were in
 * Make keywords shorter, have list of items to choose from quickly [1-2], maybe accept short names? 
 * Maybe take cardinal coords. 
@@ -1493,17 +1469,6 @@
     <t>BD, 20?</t>
   </si>
   <si>
-    <t>*Year selector
-* tutorial
-* intro
-* Map/characters ( Measure Alice or Bob &amp; they collapse, also DOD)
-* BSB Dungeon
-* storyline/quests. This is a substantial piece of work
-* See Google Keep notes on the story
-* BSB IS A DUNGEON WITH KEYS (EITHER UNIQUE OR NOT )
-* Have Brendan Fallon character with eclipse mug, rocketry t-shirt, Strainer on head?SafetyGlasses?, and iron ring (more characters)</t>
-  </si>
-  <si>
     <t>* Error checking to see if place exists before moving
 * Wear earphones on head
 * 3W text in QT
@@ -1529,7 +1494,259 @@
     <t>21 - ✔ Started whiteboarding list. Next will be writing up list and actually breaking things down into tasks.</t>
   </si>
   <si>
-    <t xml:space="preserve">22 - </t>
+    <t>2019 Kipling Update, GUI</t>
+  </si>
+  <si>
+    <t>22 - ✔ breaking down auto descriptions on whiteboard</t>
+  </si>
+  <si>
+    <t>23 - ✔ breaking doen GUI on whiteboard and still needs work</t>
+  </si>
+  <si>
+    <t>24 - 1 hr GUI on whiteboard coming up with schemes</t>
+  </si>
+  <si>
+    <t>25 - ✔ rethinking GUI layout on whiteboard, rethinking entire GUI and input architecture of the game (eg. if text based adventure would focus on terminal/text parser but because MUD want to focus on integrated and fully easy to use GUI. Game will start default Consol mode but support WASD w. hotkeys and possibly controller support)</t>
+  </si>
+  <si>
+    <t>Idea is to get stabely working game with 0.30.0 then build onto it with 2019 version</t>
+  </si>
+  <si>
+    <t>Need to finish breaking down before finaliziaing list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.30.0 </t>
+  </si>
+  <si>
+    <t>Half Release</t>
+  </si>
+  <si>
+    <t>Features + Updated 2017-2018</t>
+  </si>
+  <si>
+    <t>0.30.9</t>
+  </si>
+  <si>
+    <t>2019 Kipling</t>
+  </si>
+  <si>
+    <t>2018-2019 story</t>
+  </si>
+  <si>
+    <t>No Particular Order</t>
+  </si>
+  <si>
+    <t>Map/Item/People/Quests</t>
+  </si>
+  <si>
+    <t>Interriors</t>
+  </si>
+  <si>
+    <t>Proper Compile</t>
+  </si>
+  <si>
+    <t>Must have</t>
+  </si>
+  <si>
+    <t>Try, see how goes</t>
+  </si>
+  <si>
+    <t>EXP/LVLs/Mobs</t>
+  </si>
+  <si>
+    <t>Fast Addrewssing</t>
+  </si>
+  <si>
+    <t>Music/Sounds</t>
+  </si>
+  <si>
+    <t>Nice to have</t>
+  </si>
+  <si>
+    <t>Nonsense/Insanity</t>
+  </si>
+  <si>
+    <t>BioCards</t>
+  </si>
+  <si>
+    <t>Item Balance</t>
+  </si>
+  <si>
+    <t>Artwork/ascii converter</t>
+  </si>
+  <si>
+    <t>hard and priority features first so get idea of timeline</t>
+  </si>
+  <si>
+    <t>build from ground up for foundation/bug sake</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (i.e. don't want big feature at end that breaks game and causes big rebuild)</t>
+  </si>
+  <si>
+    <t>Class Level</t>
+  </si>
+  <si>
+    <t>Features/mechanics</t>
+  </si>
+  <si>
+    <t>Compiler</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Standardize before optimize (get it working before pretty)</t>
+  </si>
+  <si>
+    <t>-&gt;</t>
+  </si>
+  <si>
+    <t>Year Selector</t>
+  </si>
+  <si>
+    <t>Intro</t>
+  </si>
+  <si>
+    <t>MAP/Characters</t>
+  </si>
+  <si>
+    <t>BSB Dungeon</t>
+  </si>
+  <si>
+    <t>Storyline/quests</t>
+  </si>
+  <si>
+    <t>Alpha 0.30 - 2 Updates</t>
+  </si>
+  <si>
+    <t>Let's say finish scheduling by October 7th</t>
+  </si>
+  <si>
+    <t>Days between October 7th and December 31st when it's due</t>
+  </si>
+  <si>
+    <t>High end let's say</t>
+  </si>
+  <si>
+    <t>3 day work weekends</t>
+  </si>
+  <si>
+    <t>4 day 'free' weekdays</t>
+  </si>
+  <si>
+    <t>If 5 hours per 'free' weekdays</t>
+  </si>
+  <si>
+    <t>Days In total</t>
+  </si>
+  <si>
+    <t>If 1 hour per weekend</t>
+  </si>
+  <si>
+    <t>Maybe going crazy get 300 hours SOMEHOW</t>
+  </si>
+  <si>
+    <t>So anywhere between 40-275 hours left</t>
+  </si>
+  <si>
+    <t>Let's go somewhere and say we have about 100 hours</t>
+  </si>
+  <si>
+    <t>Jesus crist that's not a lot of time</t>
+  </si>
+  <si>
+    <t>* Spelling and grammar check before release (maybe needs a text output function)
+* Don't except empty name
+* "B is back" (Zac)
+* "Dell, Intel Inside"
+* search keyword for search
+* When you inspect the car it says 'Ya thought these were the keys'
+* When you searching when nothings there "You double take and there's still nothing there" (If you search 20 times you die)
+* Make father frobenius and Mario Ponce tovar spelled right with accent</t>
+  </si>
+  <si>
+    <t>Map/Items/People/Quests/ known Bugs</t>
+  </si>
+  <si>
+    <t>*Year selector
+* intro
+* Map/characters ( Measure Alice or Bob &amp; they collapse, also DOD)
+* BSB Dungeon
+* storyline/quests. This is a substantial piece of work
+* See Google Keep notes on the story
+* tutorial
+* BSB IS A DUNGEON WITH KEYS (EITHER UNIQUE OR NOT )
+* Have Brendan Fallon character with eclipse mug, rocketry t-shirt, Strainer on head?SafetyGlasses?, and iron ring (more characters)</t>
+  </si>
+  <si>
+    <t>BD, 15+8+15+20+30?</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Est. Hours</t>
+  </si>
+  <si>
+    <t>Let's say the estimates are right, they're not, they'll take WAY longer</t>
+  </si>
+  <si>
+    <t>Bugs</t>
+  </si>
+  <si>
+    <t>EVEN without nice to have:</t>
+  </si>
+  <si>
+    <t>Hours Learn Pygame</t>
+  </si>
+  <si>
+    <t>Hours Debugging, polishing, and getting into release state</t>
+  </si>
+  <si>
+    <t>SHIT THAT’S BASSICALLY THE UPPER LIMIT</t>
+  </si>
+  <si>
+    <t>with x1.5 factor:</t>
+  </si>
+  <si>
+    <t>330 min/5.5 hr</t>
+  </si>
+  <si>
+    <t>195 min/3.25 hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27 - </t>
+  </si>
+  <si>
+    <t>26 - ✔ Transferred List and did macro schedule. Shits bad</t>
+  </si>
+  <si>
+    <t>Hours upper limit IF I'M PUSHING IT at 43 hours a week</t>
+  </si>
+  <si>
+    <t>HOURS at 30 mins a day/3.5 hr/week</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the low end/garunteed hours commited to the assignment (not a lot at all)</t>
+  </si>
+  <si>
+    <t>Total Needed</t>
+  </si>
+  <si>
+    <t>hours a week</t>
+  </si>
+  <si>
+    <t>Looking like somewhere around 30 hours a week</t>
+  </si>
+  <si>
+    <t>That's INSANE FIRST OF ALL</t>
+  </si>
+  <si>
+    <t>But that looks like 2 hr Fri-Sat, 2 hr Sun, AND 6.5 HOURS EVER DAY</t>
+  </si>
+  <si>
+    <t>I can do something, I don't know if it's that but I can do something</t>
   </si>
 </sst>
 </file>
@@ -1589,12 +1806,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1609,7 +1832,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1646,6 +1869,14 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2034,7 +2265,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2106,13 +2337,13 @@
         <v>94</v>
       </c>
       <c r="H9" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="I9" s="9">
         <v>45</v>
       </c>
       <c r="J9" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2120,106 +2351,106 @@
         <v>97</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D10" t="s">
+        <v>189</v>
+      </c>
+      <c r="E10" t="s">
         <v>194</v>
       </c>
-      <c r="E10" t="s">
-        <v>199</v>
-      </c>
       <c r="F10" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G10" t="s">
-        <v>231</v>
-      </c>
-      <c r="H10">
-        <v>330</v>
+        <v>226</v>
+      </c>
+      <c r="H10" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B11" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C11" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="D11" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="E11" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="F11" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="G11" t="s">
-        <v>411</v>
-      </c>
-      <c r="H11">
-        <v>195</v>
+        <v>403</v>
+      </c>
+      <c r="H11" t="s">
+        <v>470</v>
       </c>
       <c r="I11" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>404</v>
+      </c>
+      <c r="B12" t="s">
+        <v>405</v>
+      </c>
+      <c r="C12" t="s">
+        <v>406</v>
+      </c>
+      <c r="D12" t="s">
+        <v>472</v>
+      </c>
+      <c r="E12" t="s">
+        <v>471</v>
+      </c>
+      <c r="F12" t="s">
         <v>98</v>
       </c>
-      <c r="B12" t="s">
+      <c r="G12" t="s">
         <v>99</v>
       </c>
-      <c r="C12" t="s">
-        <v>100</v>
-      </c>
-      <c r="D12" t="s">
-        <v>101</v>
-      </c>
-      <c r="E12" t="s">
-        <v>102</v>
-      </c>
-      <c r="F12" t="s">
-        <v>103</v>
-      </c>
-      <c r="G12" t="s">
-        <v>104</v>
-      </c>
       <c r="I12" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" t="s">
         <v>105</v>
       </c>
-      <c r="B13" t="s">
+      <c r="G13" t="s">
         <v>106</v>
       </c>
-      <c r="C13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D13" t="s">
-        <v>108</v>
-      </c>
-      <c r="E13" t="s">
-        <v>109</v>
-      </c>
-      <c r="F13" t="s">
-        <v>110</v>
-      </c>
-      <c r="G13" t="s">
-        <v>111</v>
-      </c>
       <c r="I13" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -2231,8 +2462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2487,7 +2718,7 @@
         <v>0.75</v>
       </c>
       <c r="F10" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>14</v>
@@ -2561,7 +2792,7 @@
         <v>0.25</v>
       </c>
       <c r="F14" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2572,7 +2803,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D15">
         <v>0.28000000000000003</v>
@@ -2581,7 +2812,7 @@
         <v>0.5</v>
       </c>
       <c r="F15" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2598,7 +2829,7 @@
         <v>1.5</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2615,7 +2846,7 @@
         <v>0.5</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2669,7 +2900,7 @@
         <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2788,7 +3019,7 @@
         <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="D27">
         <v>0.28999999999999998</v>
@@ -2797,10 +3028,10 @@
         <v>6</v>
       </c>
       <c r="F27" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2817,10 +3048,10 @@
         <v>1.5</v>
       </c>
       <c r="F28" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2837,7 +3068,7 @@
         <v>5</v>
       </c>
       <c r="F29" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2854,10 +3085,10 @@
         <v>0.5</v>
       </c>
       <c r="F30" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="G30" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2874,7 +3105,7 @@
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2891,7 +3122,7 @@
         <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -2982,10 +3213,10 @@
         <v>2</v>
       </c>
       <c r="F37" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="G37" s="14" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2999,10 +3230,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E38" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3019,7 +3250,7 @@
         <v>4</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3186,7 +3417,7 @@
         <v>3</v>
       </c>
       <c r="F49" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -3203,7 +3434,7 @@
         <v>5</v>
       </c>
       <c r="F50" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -3217,10 +3448,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="E51" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -3228,7 +3459,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="F54" t="s">
         <v>64</v>
@@ -3261,8 +3492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P76"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3293,7 +3524,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>22</v>
@@ -3336,11 +3567,14 @@
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="D5">
+        <v>5</v>
+      </c>
       <c r="E5" t="s">
-        <v>378</v>
+        <v>457</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>7</v>
@@ -3365,11 +3599,14 @@
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
       <c r="E6" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>400</v>
+        <v>456</v>
       </c>
       <c r="G6" s="10"/>
       <c r="K6" s="1" t="s">
@@ -3402,10 +3639,10 @@
         <v>81</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H7" t="s">
         <v>86</v>
@@ -3437,25 +3674,25 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="I8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>14</v>
@@ -3484,19 +3721,19 @@
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H9" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="I9" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>17</v>
@@ -3526,19 +3763,19 @@
         <v>4</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>15</v>
@@ -3567,19 +3804,19 @@
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H11" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I11" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="P11" s="1" t="s">
         <v>11</v>
@@ -3596,19 +3833,19 @@
         <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H12" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="I12" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>76</v>
@@ -3628,19 +3865,19 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H13" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I13" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>17</v>
@@ -3657,19 +3894,19 @@
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="H14" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I14" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>14</v>
@@ -3686,19 +3923,19 @@
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H15" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I15" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>15</v>
@@ -3712,25 +3949,25 @@
         <v>17</v>
       </c>
       <c r="C16" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D16">
         <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -3741,25 +3978,25 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D17">
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -3770,238 +4007,238 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>153</v>
+        <v>402</v>
       </c>
       <c r="D18" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E18" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="G18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C19" t="s">
+        <v>148</v>
+      </c>
       <c r="D19" t="s">
-        <v>405</v>
+        <v>235</v>
       </c>
       <c r="E19" t="s">
-        <v>124</v>
+        <v>219</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>402</v>
+        <v>328</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="H19" t="s">
-        <v>125</v>
-      </c>
-      <c r="I19" t="s">
-        <v>126</v>
+        <v>109</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C20" t="s">
-        <v>129</v>
-      </c>
       <c r="D20" t="s">
-        <v>128</v>
+        <v>397</v>
       </c>
       <c r="E20" t="s">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H20" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="I20" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D21">
-        <v>9</v>
+      <c r="C21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D21" t="s">
+        <v>123</v>
       </c>
       <c r="E21" t="s">
-        <v>202</v>
+        <v>58</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>401</v>
-      </c>
-      <c r="G21" s="10"/>
+        <v>391</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>109</v>
+      </c>
       <c r="H21" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="I21" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D22" t="s">
-        <v>329</v>
+      <c r="D22">
+        <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>153</v>
+        <v>197</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>406</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>114</v>
-      </c>
+        <v>393</v>
+      </c>
+      <c r="G22" s="10"/>
       <c r="H22" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="I22" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C23" t="s">
-        <v>155</v>
-      </c>
-      <c r="D23">
-        <v>10</v>
+      <c r="D23" t="s">
+        <v>459</v>
       </c>
       <c r="E23" t="s">
+        <v>148</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>458</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H23" t="s">
         <v>154</v>
       </c>
-      <c r="F23" s="14" t="s">
-        <v>391</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="H23" t="s">
-        <v>158</v>
-      </c>
       <c r="I23" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D24">
         <v>10</v>
       </c>
       <c r="E24" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H24" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="I24" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>278</v>
-      </c>
-      <c r="D25" t="s">
-        <v>234</v>
+        <v>156</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
       </c>
       <c r="E25" t="s">
-        <v>228</v>
+        <v>155</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>333</v>
+        <v>392</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H25" t="s">
-        <v>238</v>
+        <v>157</v>
       </c>
       <c r="I25" t="s">
-        <v>239</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>153</v>
+        <v>273</v>
       </c>
       <c r="D26" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="E26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="H26" s="14" t="s">
-        <v>241</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>242</v>
+        <v>109</v>
+      </c>
+      <c r="H26" t="s">
+        <v>233</v>
+      </c>
+      <c r="I26" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -4012,25 +4249,25 @@
         <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D27">
         <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H27" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="I27" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -4050,7 +4287,7 @@
         <v>79</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>84</v>
@@ -4070,25 +4307,25 @@
         <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D29" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E29" t="s">
+        <v>129</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="H29" t="s">
         <v>134</v>
       </c>
-      <c r="F29" s="14" t="s">
-        <v>327</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="H29" t="s">
-        <v>139</v>
-      </c>
       <c r="I29" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -4099,25 +4336,25 @@
         <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D30" t="s">
+        <v>130</v>
+      </c>
+      <c r="E30" t="s">
+        <v>136</v>
+      </c>
+      <c r="F30" t="s">
+        <v>323</v>
+      </c>
+      <c r="G30" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="E30" t="s">
-        <v>141</v>
-      </c>
-      <c r="F30" t="s">
-        <v>328</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>140</v>
-      </c>
       <c r="H30" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="I30" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -4128,22 +4365,22 @@
         <v>15</v>
       </c>
       <c r="D31" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E31" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="G31" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="H31" t="s">
         <v>151</v>
       </c>
-      <c r="H31" t="s">
-        <v>156</v>
-      </c>
       <c r="I31" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -4154,25 +4391,25 @@
         <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D32">
         <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H32" t="s">
+        <v>159</v>
+      </c>
+      <c r="I32" t="s">
         <v>164</v>
-      </c>
-      <c r="I32" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -4183,25 +4420,25 @@
         <v>15</v>
       </c>
       <c r="C33" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="D33" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E33" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H33" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="I33" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -4212,22 +4449,22 @@
         <v>15</v>
       </c>
       <c r="D34" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E34" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F34" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H34" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="I34" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -4238,25 +4475,25 @@
         <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D35" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E35" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H35" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="I35" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -4267,25 +4504,25 @@
         <v>15</v>
       </c>
       <c r="C36" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D36">
         <v>10</v>
       </c>
       <c r="E36" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="H36" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="I36" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -4299,19 +4536,19 @@
         <v>8</v>
       </c>
       <c r="E37" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="H37" s="14" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -4325,19 +4562,19 @@
         <v>6</v>
       </c>
       <c r="E38" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F38" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -4348,25 +4585,25 @@
         <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D39">
         <v>16</v>
       </c>
       <c r="E39" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="H39" s="14" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -4380,19 +4617,19 @@
         <v>20</v>
       </c>
       <c r="E40" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -4406,19 +4643,19 @@
         <v>10</v>
       </c>
       <c r="E41" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -4432,19 +4669,19 @@
         <v>20</v>
       </c>
       <c r="E42" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="H42" s="14" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="I42" s="14" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -4455,25 +4692,25 @@
         <v>15</v>
       </c>
       <c r="C43" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D43">
         <v>12</v>
       </c>
       <c r="E43" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -4484,25 +4721,25 @@
         <v>15</v>
       </c>
       <c r="C44" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D44">
         <v>20</v>
       </c>
       <c r="E44" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -4516,19 +4753,19 @@
         <v>10</v>
       </c>
       <c r="E45" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="H45" s="14" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -4538,23 +4775,26 @@
       <c r="B46" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C46" t="s">
+        <v>58</v>
+      </c>
       <c r="D46">
         <v>7</v>
       </c>
       <c r="E46" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
       <c r="F46" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -4568,19 +4808,19 @@
         <v>10</v>
       </c>
       <c r="E47" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="H47" s="14" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -4591,25 +4831,25 @@
         <v>15</v>
       </c>
       <c r="C48" t="s">
+        <v>282</v>
+      </c>
+      <c r="D48" t="s">
+        <v>281</v>
+      </c>
+      <c r="E48" t="s">
+        <v>210</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="H48" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="D48" t="s">
-        <v>286</v>
-      </c>
-      <c r="E48" t="s">
-        <v>215</v>
-      </c>
-      <c r="F48" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>272</v>
-      </c>
-      <c r="H48" s="14" t="s">
-        <v>292</v>
-      </c>
       <c r="I48" s="14" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -4620,25 +4860,25 @@
         <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D49" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="E49" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="H49" s="14" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -4649,22 +4889,22 @@
         <v>15</v>
       </c>
       <c r="D50" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E50" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -4675,22 +4915,22 @@
         <v>15</v>
       </c>
       <c r="D51" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="E51" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -4701,22 +4941,22 @@
         <v>15</v>
       </c>
       <c r="D52" t="s">
+        <v>292</v>
+      </c>
+      <c r="E52" t="s">
+        <v>215</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="H52" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="E52" t="s">
-        <v>220</v>
-      </c>
-      <c r="F52" s="14" t="s">
-        <v>340</v>
-      </c>
-      <c r="G52" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="H52" s="14" t="s">
-        <v>302</v>
-      </c>
       <c r="I52" s="14" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -4727,25 +4967,25 @@
         <v>15</v>
       </c>
       <c r="C53" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="D53" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E53" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H53" s="14" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -4756,22 +4996,22 @@
         <v>15</v>
       </c>
       <c r="D54" t="s">
+        <v>304</v>
+      </c>
+      <c r="E54" t="s">
+        <v>224</v>
+      </c>
+      <c r="F54" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="H54" s="14" t="s">
         <v>309</v>
       </c>
-      <c r="E54" t="s">
-        <v>229</v>
-      </c>
-      <c r="F54" s="14" t="s">
-        <v>350</v>
-      </c>
-      <c r="G54" s="10" t="s">
-        <v>282</v>
-      </c>
-      <c r="H54" s="14" t="s">
-        <v>314</v>
-      </c>
       <c r="I54" s="14" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -4782,22 +5022,22 @@
         <v>15</v>
       </c>
       <c r="D55" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="E55" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="H55" s="14" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="I55" s="14" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -4808,22 +5048,22 @@
         <v>15</v>
       </c>
       <c r="D56" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="E56" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="H56" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="I56" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -4834,10 +5074,10 @@
         <v>15</v>
       </c>
       <c r="E57" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="G57" s="10"/>
     </row>
@@ -4849,27 +5089,27 @@
         <v>15</v>
       </c>
       <c r="C58" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="E58" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="F58" s="14" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="G58" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="H58" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="I58" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
     </row>
     <row r="65" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E65" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="4:6" x14ac:dyDescent="0.25">
@@ -4879,55 +5119,55 @@
     </row>
     <row r="67" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D67" s="11" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="68" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D68" s="11" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="69" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D69" s="11" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="70" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D70" s="11" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
     </row>
     <row r="71" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D71" s="11" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
     </row>
     <row r="72" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="73" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="F73" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
     </row>
     <row r="74" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="75" spans="4:6" x14ac:dyDescent="0.25">
       <c r="E75" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="76" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -4949,6 +5189,860 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" activeCellId="2" sqref="A12 A20 A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B2" t="s">
+        <v>410</v>
+      </c>
+      <c r="C2" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>412</v>
+      </c>
+      <c r="B3" t="s">
+        <v>413</v>
+      </c>
+      <c r="C3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="F12" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>416</v>
+      </c>
+      <c r="F13" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" t="s">
+        <v>432</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>437</v>
+      </c>
+      <c r="H15" t="s">
+        <v>433</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>437</v>
+      </c>
+      <c r="J15" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" s="23" t="s">
+        <v>437</v>
+      </c>
+      <c r="L15" t="s">
+        <v>434</v>
+      </c>
+      <c r="M15" s="23" t="s">
+        <v>437</v>
+      </c>
+      <c r="N15" t="s">
+        <v>435</v>
+      </c>
+      <c r="O15" s="23" t="s">
+        <v>437</v>
+      </c>
+      <c r="P15" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>417</v>
+      </c>
+      <c r="F16" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="19" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G62"/>
+  <sheetViews>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>450-365</f>
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2*0.5</f>
+        <v>42.5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>474</v>
+      </c>
+      <c r="C3" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>12*4+12*3</f>
+        <v>84</v>
+      </c>
+      <c r="B8" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>A6*4*5</f>
+        <v>240</v>
+      </c>
+      <c r="B10" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>A7*3*1</f>
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>A11+A10</f>
+        <v>276</v>
+      </c>
+      <c r="B12" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>460</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>461</v>
+      </c>
+      <c r="D19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="20">
+        <v>50</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="20">
+        <v>5</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="19">
+        <v>51</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="19">
+        <v>2</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="20">
+        <v>2</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="19">
+        <v>3</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="19">
+        <v>2</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="20">
+        <v>16</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="20">
+        <v>6</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="20">
+        <v>22</v>
+      </c>
+      <c r="B25" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="20">
+        <v>4</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="19">
+        <v>48</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="19">
+        <v>8</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="19">
+        <v>6</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="19">
+        <v>20</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="20">
+        <v>7</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="20">
+        <v>30</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="19">
+        <v>10</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="19">
+        <v>9</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="20">
+        <v>12</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="20">
+        <f>15+8+15+20+30</f>
+        <v>88</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="19">
+        <v>13</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="19">
+        <v>10</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="20">
+        <v>14</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="20">
+        <v>10</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="19">
+        <v>25</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="19">
+        <v>15</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="20">
+        <v>4</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="20">
+        <v>2</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="19">
+        <v>5</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="19">
+        <v>15</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="20">
+        <v>19</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="20">
+        <v>8</v>
+      </c>
+      <c r="D36" s="20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="19">
+        <v>28</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="19">
+        <v>12</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="20">
+        <v>34</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="20">
+        <v>6</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="19">
+        <v>50</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="19">
+        <v>10</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="20">
+        <v>26</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C40" s="20">
+        <v>12</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>20</v>
+      </c>
+      <c r="B41" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>15</v>
+      </c>
+      <c r="B43" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="B47">
+        <f>SUM(C20:C21)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>419</v>
+      </c>
+      <c r="B48">
+        <f>SUM(C22:C26)</f>
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="B49">
+        <f>SUM(C27:C33)</f>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="B50">
+        <f>SUM(C34:C40)</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="D53">
+        <f>SUM(B47:B49,A43,A41)</f>
+        <v>245.5</v>
+      </c>
+      <c r="F53">
+        <f>D53/12</f>
+        <v>20.458333333333332</v>
+      </c>
+      <c r="G53" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>468</v>
+      </c>
+      <c r="D54">
+        <f>D53*1.5</f>
+        <v>368.25</v>
+      </c>
+      <c r="F54">
+        <f>D54/12</f>
+        <v>30.6875</v>
+      </c>
+      <c r="G54" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="C56">
+        <f>SUM(B47:B50,A43,A41)</f>
+        <v>310.5</v>
+      </c>
+      <c r="E56">
+        <f>C56/12</f>
+        <v>25.875</v>
+      </c>
+      <c r="F56" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>468</v>
+      </c>
+      <c r="C57">
+        <f>C56*1.5</f>
+        <v>465.75</v>
+      </c>
+      <c r="E57">
+        <f>C57/12</f>
+        <v>38.8125</v>
+      </c>
+      <c r="F57" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>481</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20:B40">
+      <formula1>$K$5:$K$10</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
remade list based on plan
</commit_message>
<xml_diff>
--- a/Dev/EBTA Developent Roadmap.xlsx
+++ b/Dev/EBTA Developent Roadmap.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="535">
   <si>
     <t>Develement Roadmap (feedback, features, featurelocks, and roadmap)</t>
   </si>
@@ -987,12 +987,6 @@
   </si>
   <si>
     <t>Would like to finish feature lock at least and get into breakdown</t>
-  </si>
-  <si>
-    <t>Breakdown</t>
-  </si>
-  <si>
-    <t>Feature lock release Oct 1?</t>
   </si>
   <si>
     <t>Total</t>
@@ -1087,11 +1081,6 @@
 * Put game on steam</t>
   </si>
   <si>
-    <t>* They move around
-* Have  a companion
-* Can equip items to yourself to store for later games so they act as a companion.</t>
-  </si>
-  <si>
     <t>* Sling ring, teliport anywhere you know
 * Portal gun
 * Teliport anywhere you can see
@@ -1170,11 +1159,6 @@
 * Auto save every once and a while</t>
   </si>
   <si>
-    <t>* Making sure all bosses are beatable without secrets so at least not frustrating for new players
-* See balance metrics from balance sheet
-* Maybe only have saving and autosaving as a developer.</t>
-  </si>
-  <si>
     <t>Balance</t>
   </si>
   <si>
@@ -1220,13 +1204,6 @@
   </si>
   <si>
     <t>Having Map/dungeons, maybe charaters, proceduraly generated</t>
-  </si>
-  <si>
-    <t>* Attack and defense, speed doesn't do anything. 
-* Would need to be be after combat update. 
-* Possibly have star/some sort of indicator for bosses OR have the indicator just be how hard they can hit you/how big they are
-* More direct reward for exploration with something that ties back into game (like BOTW)
-* Having body armour Quantum relic</t>
   </si>
   <si>
     <t>* When you inspect the car it says 'Ya thought these were the keys'
@@ -1345,33 +1322,6 @@
 * installer gives desktop icon
 * Overwriting old instal to update would be nice.
 * Try changing the file extensions and names of folders in EBTA to .EBTA or something random (or blank) to hide or obscure files (make sure it works first)</t>
-  </si>
-  <si>
-    <t>* Classes, object methods, how map works (numbered adjacency lists), commenting code. Updating to python 3. Interactables class. Buildings as an entity.
-* PP8 style using PyCharm
-* Get rid of global variables and restructure code
-* Using and understanding effecient python code chunks (See Liam F. and his book)
-* Make an entity class (name, description, location, stats, health, item need, item give, inventory, deathtext, etc) and then all subclasses  using inheritance
-* Map
-So we are making a MUD and I didn't know it LOL
-Better than trying to retrofit everything and then you have unique addressing
-Have a linked exit on the spots beside, no need to go inside or anything, just update position and move around
-Map will just constrain itself by where edges are and where you can move
-* Nevada Game engine
-Graph with adjacency list (stored effeciently) that gives the possible options. 
-Using paths with path constructor to translate between points (instead of on-command search). Then maps just become entities addresses by the name.
-For destruction just do pointer to point all old places to the new place (but does damage/kill people when you do destroy a spot)
-* Entity
-     Person(each has same attributes and stuff, even schedule would be the same)
-          Boss?
-     Place
-          Interroor
-     Item
-          Interactable
-          Interactable can go, just add a moveable flag to items with new entity structute that allows give/take
-* Have a generalized interface class/objects so you don't have to make new ones every time
-* Calling it Mac Quest? McMaster MUD? MMUD
-* See TODO list for rest of rebuild notes</t>
   </si>
   <si>
     <t>* See 13 Hollywood Productions March 7th large section of ideas.
@@ -1533,12 +1483,6 @@
     <t>2018-2019 story</t>
   </si>
   <si>
-    <t>No Particular Order</t>
-  </si>
-  <si>
-    <t>Map/Item/People/Quests</t>
-  </si>
-  <si>
     <t>Interriors</t>
   </si>
   <si>
@@ -1563,18 +1507,12 @@
     <t>Nice to have</t>
   </si>
   <si>
-    <t>Nonsense/Insanity</t>
-  </si>
-  <si>
     <t>BioCards</t>
   </si>
   <si>
     <t>Item Balance</t>
   </si>
   <si>
-    <t>Artwork/ascii converter</t>
-  </si>
-  <si>
     <t>hard and priority features first so get idea of timeline</t>
   </si>
   <si>
@@ -1584,22 +1522,7 @@
     <t xml:space="preserve"> (i.e. don't want big feature at end that breaks game and causes big rebuild)</t>
   </si>
   <si>
-    <t>Class Level</t>
-  </si>
-  <si>
-    <t>Features/mechanics</t>
-  </si>
-  <si>
-    <t>Compiler</t>
-  </si>
-  <si>
-    <t>Content</t>
-  </si>
-  <si>
     <t>Standardize before optimize (get it working before pretty)</t>
-  </si>
-  <si>
-    <t>-&gt;</t>
   </si>
   <si>
     <t>Year Selector</t>
@@ -1716,9 +1639,6 @@
     <t>195 min/3.25 hr</t>
   </si>
   <si>
-    <t xml:space="preserve">27 - </t>
-  </si>
-  <si>
     <t>26 - ✔ Transferred List and did macro schedule. Shits bad</t>
   </si>
   <si>
@@ -1747,6 +1667,261 @@
   </si>
   <si>
     <t>I can do something, I don't know if it's that but I can do something</t>
+  </si>
+  <si>
+    <t>Feature lock, breakdown, plan, and shechedule by Oct 7th</t>
+  </si>
+  <si>
+    <t>Get through 0.30.0 Breakdown</t>
+  </si>
+  <si>
+    <t>SO THE PLAN HAS CHANGED</t>
+  </si>
+  <si>
+    <t>MAKE 2017-2018 a Text Based Adventure to its fullest degree to captalize on things that make it great</t>
+  </si>
+  <si>
+    <t>Lean into story</t>
+  </si>
+  <si>
+    <t>Get rid of info that's not immersive</t>
+  </si>
+  <si>
+    <t>Inventory similar but all Text</t>
+  </si>
+  <si>
+    <t>No Ascii art (or at least size of the consol), no sounds/music, stats,</t>
+  </si>
+  <si>
+    <t>DO NOT BREAK IMMERSION</t>
+  </si>
+  <si>
+    <t>So this is good and bad, priorities have changed. I think 2017-2018 will end up the best version of itself and not a launching board for 0.30.9</t>
+  </si>
+  <si>
+    <t>BUT this does mean possibly more work, more focus on playability/balance, and much more design to anticipate the user</t>
+  </si>
+  <si>
+    <t>And a lot of features will be pushed to 2018-2019 version and it becomes a different game</t>
+  </si>
+  <si>
+    <t>This game is a full mud McMaster Eng Phys Multi-User Dungeon (MEPMUD), MEMUD for short</t>
+  </si>
+  <si>
+    <t>These features will cator to an rpg with text-only ellements (for the meme, not necisarily because I don't want to do graphics but I still don't want to make them, oh wait but I will but just convert them to text? Fuck)</t>
+  </si>
+  <si>
+    <t>Tyler likes the idea and how it goes to the whole story</t>
+  </si>
+  <si>
+    <t>Find Jameson who was sick and get solutions to his bot</t>
+  </si>
+  <si>
+    <t>Make something to wake up Liam Dow</t>
+  </si>
+  <si>
+    <t>Go to find Steven but he's not there or in the carabean</t>
+  </si>
+  <si>
+    <t>Need Tyler for writing, Liam for mechanic advise</t>
+  </si>
+  <si>
+    <t>Both seem interested to that capacity</t>
+  </si>
+  <si>
+    <t>Kipling</t>
+  </si>
+  <si>
+    <t>0.31?</t>
+  </si>
+  <si>
+    <t>A reocurring and growing Eng Phys Game</t>
+  </si>
+  <si>
+    <t>Mac Eng students</t>
+  </si>
+  <si>
+    <t>* Have this as kipling game for this year if they want with all people in it
+* April is kickoff for next game
+* Game would still have to be approchable by all people
+* Should definetly bring up as a suggestion</t>
+  </si>
+  <si>
+    <t>0. Class Level</t>
+  </si>
+  <si>
+    <t>1. Features/mechanics</t>
+  </si>
+  <si>
+    <t>2. GUI</t>
+  </si>
+  <si>
+    <t>3. Compiler</t>
+  </si>
+  <si>
+    <t>4. Content (items, quests, people)</t>
+  </si>
+  <si>
+    <t>5. Balance</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Est. Time</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>0. Bug</t>
+  </si>
+  <si>
+    <t>1. Must Have</t>
+  </si>
+  <si>
+    <t>2. Try, see how far</t>
+  </si>
+  <si>
+    <t>3. Nice to Have</t>
+  </si>
+  <si>
+    <t>Map/Item/People/Quests/Text/Grammar/Naming/Bugs</t>
+  </si>
+  <si>
+    <t>BD, 6 est</t>
+  </si>
+  <si>
+    <t>Bd, 10 est</t>
+  </si>
+  <si>
+    <t>* Attack and defense, speed doesn't do anything. 
+* Would need to be be after combat update. 
+* Possibly have star/some sort of indicator for bosses OR have the indicator just be how hard they can hit you/how big they are
+* More direct reward for exploration with something that ties back into game (like BOTW)
+* Having body armour Quantum relic
+* Make sure all items favour equally for game</t>
+  </si>
+  <si>
+    <t>Dev Mode</t>
+  </si>
+  <si>
+    <t>* Making sure all bosses are beatable without secrets so at least not frustrating for new players
+* See balance metrics from balance sheet
+* More exploration as a player</t>
+  </si>
+  <si>
+    <t>* They move around
+* Have  a companion
+* Can equip items to yourself to store for later games so they act as a companion.
+* Playable Characters where you can actually choose one of the players in the game and play as them (but unlock them as you go through story, do their quests, etc) like playable characters in Lego Games</t>
+  </si>
+  <si>
+    <t>Easy to develop but still hidden from players</t>
+  </si>
+  <si>
+    <t>* Enter dev mode by typing 420E69 into the setting screen
+* Only show info that is if you're in dev mode
+* Only have saving as a developer.
+* Only see stats if you're in Dev mode
+* Put you into Tyler Kashak but don't make that your name, name is Doug but is in Tyler Kashak mode which can still be accessed by Typing it in
+* Maybe either hide settings file OR make it identified by something else (Naming of a file?)
+* See if renaming files messes anything up or can keep low level hiding</t>
+  </si>
+  <si>
+    <t>* Classes, object methods, how map works (numbered adjacency lists), commenting code. Updating to python 3. Interactables class. Buildings as an entity.
+* PP8 style using PyCharm
+* Get rid of global variables and restructure code
+* Maybe make each class and big function its own module file
+* Using and understanding effecient python code chunks (See Liam F. and his book)
+* Make an entity class (name, description, location, stats, health, item need, item give, inventory, deathtext, etc) and then all subclasses  using inheritance
+* Map
+So we are making a MUD and I didn't know it LOL
+Better than trying to retrofit everything and then you have unique addressing
+Have a linked exit on the spots beside, no need to go inside or anything, just update position and move around
+Map will just constrain itself by where edges are and where you can move
+* Nevada Game engine
+Graph with adjacency list (stored effeciently) that gives the possible options. 
+Using paths with path constructor to translate between points (instead of on-command search). Then maps just become entities addresses by the name.
+For destruction just do pointer to point all old places to the new place (but does damage/kill people when you do destroy a spot)
+* Entity
+     Person(each has same attributes and stuff, even schedule would be the same)
+          Boss?
+     Place
+          Interroor
+     Item
+          Interactable
+          Interactable can go, just add a moveable flag to items with new entity structute that allows give/take
+* Have a generalized interface class/objects so you don't have to make new ones every time
+* Calling it Mac Quest? McMaster MUD? MMUD
+* See TODO list for rest of rebuild notes</t>
+  </si>
+  <si>
+    <t>Text Interprutation/Lexicon</t>
+  </si>
+  <si>
+    <t>1 hr</t>
+  </si>
+  <si>
+    <t>Hours total worked on</t>
+  </si>
+  <si>
+    <t>Text Based Adventure! Rewarding for players to figure out</t>
+  </si>
+  <si>
+    <t>Adventurers</t>
+  </si>
+  <si>
+    <t>BD, 15?</t>
+  </si>
+  <si>
+    <t>* Lexicon for similar related words
+* There are good lexicons
+* there are machine learning/AI natural language processing - Brian to look into
+*Search for subword in sentence to accept if right things in there as long as doesn't interprut the wrong action
+* Worse thing in a game as a player is to know what to do but not how to do it</t>
+  </si>
+  <si>
+    <t>BD, 15 est</t>
+  </si>
+  <si>
+    <t>BD, 12 est</t>
+  </si>
+  <si>
+    <t>Dev mode/revoke info</t>
+  </si>
+  <si>
+    <t>ascii converter</t>
+  </si>
+  <si>
+    <t>Artwork</t>
+  </si>
+  <si>
+    <t>Balance/bugcheck</t>
+  </si>
+  <si>
+    <t>Learn Pygame</t>
+  </si>
+  <si>
+    <t>BD, 7 est</t>
+  </si>
+  <si>
+    <t>BD, 5 est</t>
+  </si>
+  <si>
+    <t>BD, 8 est</t>
+  </si>
+  <si>
+    <t>Just need thing to drop bio cards</t>
+  </si>
+  <si>
+    <t>4/0</t>
+  </si>
+  <si>
+    <t>27 - 1.25 hr remade list and populating for breakdown tomorrow</t>
   </si>
 </sst>
 </file>
@@ -1979,10 +2154,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:I58" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A4:I58"/>
-  <sortState ref="A5:I58">
-    <sortCondition ref="B4:B58"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:I61" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A4:I61"/>
+  <sortState ref="A5:I61">
+    <sortCondition ref="B4:B61"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" name="Feature"/>
@@ -2264,8 +2439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2337,7 +2512,7 @@
         <v>94</v>
       </c>
       <c r="H9" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I9" s="9">
         <v>45</v>
@@ -2369,7 +2544,13 @@
         <v>226</v>
       </c>
       <c r="H10" t="s">
-        <v>469</v>
+        <v>454</v>
+      </c>
+      <c r="I10" t="s">
+        <v>516</v>
+      </c>
+      <c r="J10" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2380,42 +2561,42 @@
         <v>314</v>
       </c>
       <c r="C11" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="D11" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="E11" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="F11" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="G11" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="H11" t="s">
-        <v>470</v>
-      </c>
-      <c r="I11" t="s">
+        <v>455</v>
+      </c>
+      <c r="I11" s="11" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="B12" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="C12" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="D12" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="E12" t="s">
-        <v>471</v>
+        <v>534</v>
       </c>
       <c r="F12" t="s">
         <v>98</v>
@@ -2424,7 +2605,7 @@
         <v>99</v>
       </c>
       <c r="I12" t="s">
-        <v>316</v>
+        <v>467</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2450,7 +2631,7 @@
         <v>106</v>
       </c>
       <c r="I13" t="s">
-        <v>317</v>
+        <v>466</v>
       </c>
     </row>
   </sheetData>
@@ -2462,8 +2643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2718,7 +2899,7 @@
         <v>0.75</v>
       </c>
       <c r="F10" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>14</v>
@@ -2792,7 +2973,7 @@
         <v>0.25</v>
       </c>
       <c r="F14" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2803,7 +2984,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="D15">
         <v>0.28000000000000003</v>
@@ -2846,7 +3027,7 @@
         <v>0.5</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2900,7 +3081,7 @@
         <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -3019,7 +3200,7 @@
         <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D27">
         <v>0.28999999999999998</v>
@@ -3028,10 +3209,10 @@
         <v>6</v>
       </c>
       <c r="F27" t="s">
+        <v>349</v>
+      </c>
+      <c r="G27" s="14" t="s">
         <v>353</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -3048,10 +3229,10 @@
         <v>1.5</v>
       </c>
       <c r="F28" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -3068,7 +3249,7 @@
         <v>5</v>
       </c>
       <c r="F29" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -3085,7 +3266,7 @@
         <v>0.5</v>
       </c>
       <c r="F30" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="G30" t="s">
         <v>195</v>
@@ -3213,10 +3394,10 @@
         <v>2</v>
       </c>
       <c r="F37" t="s">
+        <v>350</v>
+      </c>
+      <c r="G37" s="14" t="s">
         <v>354</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -3250,7 +3431,7 @@
         <v>4</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3459,7 +3640,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F54" t="s">
         <v>64</v>
@@ -3490,10 +3671,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P76"/>
+  <dimension ref="A1:P79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3571,10 +3752,10 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>7</v>
@@ -3603,10 +3784,10 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>456</v>
+        <v>441</v>
       </c>
       <c r="G6" s="10"/>
       <c r="K6" s="1" t="s">
@@ -3639,7 +3820,7 @@
         <v>81</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>109</v>
@@ -3683,7 +3864,7 @@
         <v>108</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>109</v>
@@ -3718,13 +3899,13 @@
         <v>13</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
         <v>161</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G9" s="10" t="s">
         <v>109</v>
@@ -3807,7 +3988,7 @@
         <v>183</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>109</v>
@@ -3836,7 +4017,7 @@
         <v>240</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>352</v>
+        <v>510</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>109</v>
@@ -3856,28 +4037,25 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>382</v>
+        <v>509</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>395</v>
+        <v>513</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H13" t="s">
-        <v>114</v>
-      </c>
-      <c r="I13" t="s">
-        <v>115</v>
+        <v>512</v>
       </c>
       <c r="P13" s="1" t="s">
         <v>17</v>
@@ -3885,28 +4063,28 @@
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D14">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>116</v>
+        <v>377</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>321</v>
+        <v>389</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="H14" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>14</v>
@@ -3914,28 +4092,28 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D15">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>175</v>
+        <v>116</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
       <c r="H15" t="s">
-        <v>176</v>
+        <v>118</v>
       </c>
       <c r="I15" t="s">
-        <v>177</v>
+        <v>117</v>
       </c>
       <c r="P15" s="1" t="s">
         <v>15</v>
@@ -3943,111 +4121,108 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C16" t="s">
-        <v>191</v>
-      </c>
       <c r="D16">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>190</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>367</v>
+        <v>175</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>323</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>243</v>
-      </c>
-      <c r="I16" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="H16" t="s">
+        <v>176</v>
+      </c>
+      <c r="I16" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>155</v>
+        <v>191</v>
       </c>
       <c r="D17">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>199</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>335</v>
+        <v>190</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>508</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>109</v>
+        <v>146</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>126</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>402</v>
-      </c>
-      <c r="D18" t="s">
-        <v>122</v>
+        <v>155</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>299</v>
+        <v>199</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="G18" s="10"/>
+        <v>511</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>148</v>
+        <v>396</v>
       </c>
       <c r="D19" t="s">
-        <v>235</v>
+        <v>122</v>
       </c>
       <c r="E19" t="s">
-        <v>219</v>
+        <v>299</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>328</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>236</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>237</v>
-      </c>
+        <v>343</v>
+      </c>
+      <c r="G19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -4057,13 +4232,13 @@
         <v>14</v>
       </c>
       <c r="D20" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="E20" t="s">
         <v>119</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>109</v>
@@ -4092,7 +4267,7 @@
         <v>58</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>109</v>
@@ -4118,7 +4293,7 @@
         <v>197</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="G22" s="10"/>
       <c r="H22" t="s">
@@ -4136,13 +4311,13 @@
         <v>14</v>
       </c>
       <c r="D23" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
       <c r="E23" t="s">
         <v>148</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>458</v>
+        <v>443</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>109</v>
@@ -4171,7 +4346,7 @@
         <v>149</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>109</v>
@@ -4200,7 +4375,7 @@
         <v>155</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>109</v>
@@ -4229,7 +4404,7 @@
         <v>223</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>109</v>
@@ -4243,424 +4418,427 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27" t="s">
-        <v>273</v>
-      </c>
-      <c r="D27">
-        <v>15</v>
+        <v>148</v>
+      </c>
+      <c r="D27" t="s">
+        <v>235</v>
       </c>
       <c r="E27" t="s">
-        <v>172</v>
+        <v>219</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>371</v>
+        <v>326</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="H27" t="s">
-        <v>173</v>
-      </c>
-      <c r="I27" t="s">
-        <v>174</v>
+        <v>109</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="I27" s="14" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" t="s">
-        <v>85</v>
+        <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>80</v>
+        <v>520</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>515</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>389</v>
+        <v>521</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="H28" t="s">
-        <v>83</v>
+        <v>518</v>
       </c>
       <c r="I28" t="s">
-        <v>82</v>
+        <v>519</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C29" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="D29" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="E29" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>322</v>
+        <v>514</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>133</v>
+        <v>84</v>
       </c>
       <c r="H29" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
       <c r="I29" t="s">
-        <v>140</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D30" t="s">
         <v>130</v>
       </c>
       <c r="E30" t="s">
-        <v>136</v>
-      </c>
-      <c r="F30" t="s">
-        <v>323</v>
+        <v>129</v>
+      </c>
+      <c r="F30" s="14" t="s">
+        <v>320</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H30" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="I30" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C31" t="s">
+        <v>137</v>
+      </c>
       <c r="D31" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="E31" t="s">
-        <v>144</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>390</v>
+        <v>136</v>
+      </c>
+      <c r="F31" t="s">
+        <v>321</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="H31" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="I31" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C32" t="s">
-        <v>160</v>
-      </c>
-      <c r="D32">
-        <v>6</v>
+      <c r="D32" t="s">
+        <v>145</v>
       </c>
       <c r="E32" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="G32" s="10" t="s">
         <v>146</v>
       </c>
       <c r="H32" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="I32" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C33" t="s">
-        <v>377</v>
-      </c>
-      <c r="D33" t="s">
-        <v>123</v>
+        <v>160</v>
+      </c>
+      <c r="D33">
+        <v>6</v>
       </c>
       <c r="E33" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>169</v>
+        <v>146</v>
       </c>
       <c r="H33" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="I33" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C34" t="s">
+        <v>372</v>
+      </c>
       <c r="D34" t="s">
-        <v>181</v>
+        <v>123</v>
       </c>
       <c r="E34" t="s">
-        <v>178</v>
-      </c>
-      <c r="F34" t="s">
-        <v>326</v>
+        <v>168</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>375</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>132</v>
+        <v>169</v>
       </c>
       <c r="H34" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="I34" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>258</v>
-      </c>
-      <c r="D35" t="s">
-        <v>229</v>
+        <v>273</v>
+      </c>
+      <c r="D35">
+        <v>15</v>
       </c>
       <c r="E35" t="s">
-        <v>221</v>
+        <v>172</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>351</v>
+        <v>366</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="H35" t="s">
-        <v>228</v>
+        <v>173</v>
       </c>
       <c r="I35" t="s">
-        <v>227</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C36" t="s">
-        <v>155</v>
-      </c>
-      <c r="D36">
-        <v>10</v>
+      <c r="D36" t="s">
+        <v>181</v>
       </c>
       <c r="E36" t="s">
-        <v>222</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>330</v>
+        <v>178</v>
+      </c>
+      <c r="F36" t="s">
+        <v>324</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>230</v>
+        <v>132</v>
       </c>
       <c r="H36" t="s">
-        <v>231</v>
+        <v>180</v>
       </c>
       <c r="I36" t="s">
-        <v>232</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D37">
-        <v>8</v>
+      <c r="C37" t="s">
+        <v>258</v>
+      </c>
+      <c r="D37" t="s">
+        <v>229</v>
       </c>
       <c r="E37" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>329</v>
+        <v>348</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="H37" s="14" t="s">
-        <v>238</v>
-      </c>
-      <c r="I37" s="14" t="s">
-        <v>239</v>
+        <v>133</v>
+      </c>
+      <c r="H37" t="s">
+        <v>228</v>
+      </c>
+      <c r="I37" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C38" t="s">
+        <v>155</v>
+      </c>
       <c r="D38">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>192</v>
-      </c>
-      <c r="F38" t="s">
-        <v>331</v>
+        <v>222</v>
+      </c>
+      <c r="F38" s="14" t="s">
+        <v>328</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="H38" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="I38" s="14" t="s">
-        <v>126</v>
+        <v>230</v>
+      </c>
+      <c r="H38" t="s">
+        <v>231</v>
+      </c>
+      <c r="I38" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C39" t="s">
-        <v>246</v>
-      </c>
       <c r="D39">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E39" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="H39" s="14" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D40">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="E40" t="s">
-        <v>320</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>333</v>
+        <v>192</v>
+      </c>
+      <c r="F40" t="s">
+        <v>329</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>249</v>
+        <v>146</v>
       </c>
       <c r="H40" s="14" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>251</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C41" t="s">
+        <v>246</v>
+      </c>
       <c r="D41">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E41" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>376</v>
+        <v>330</v>
       </c>
       <c r="G41" s="10" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>15</v>
@@ -4669,137 +4847,134 @@
         <v>20</v>
       </c>
       <c r="E42" t="s">
-        <v>206</v>
+        <v>318</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>369</v>
+        <v>331</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="H42" s="14" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="I42" s="14" t="s">
-        <v>308</v>
+        <v>251</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C43" t="s">
-        <v>258</v>
-      </c>
       <c r="D43">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E43" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>336</v>
+        <v>371</v>
       </c>
       <c r="G43" s="10" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="H43" s="14" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C44" t="s">
-        <v>258</v>
-      </c>
       <c r="D44">
         <v>20</v>
       </c>
       <c r="E44" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="H44" s="14" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>269</v>
+        <v>308</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C45" t="s">
+        <v>258</v>
+      </c>
       <c r="D45">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E45" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="G45" s="10" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="H45" s="14" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>58</v>
+        <v>258</v>
       </c>
       <c r="D46">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E46" t="s">
-        <v>399</v>
-      </c>
-      <c r="F46" t="s">
-        <v>400</v>
+        <v>201</v>
+      </c>
+      <c r="F46" s="14" t="s">
+        <v>365</v>
       </c>
       <c r="G46" s="10" t="s">
-        <v>109</v>
+        <v>267</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>15</v>
@@ -4808,134 +4983,137 @@
         <v>10</v>
       </c>
       <c r="E47" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="G47" s="10" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="H47" s="14" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C48" t="s">
-        <v>282</v>
-      </c>
-      <c r="D48" t="s">
-        <v>281</v>
+        <v>58</v>
+      </c>
+      <c r="D48">
+        <v>7</v>
       </c>
       <c r="E48" t="s">
-        <v>210</v>
-      </c>
-      <c r="F48" s="14" t="s">
-        <v>339</v>
+        <v>393</v>
+      </c>
+      <c r="F48" t="s">
+        <v>394</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>267</v>
+        <v>109</v>
       </c>
       <c r="H48" s="14" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>167</v>
+        <v>275</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C49" t="s">
-        <v>290</v>
-      </c>
-      <c r="D49" t="s">
-        <v>289</v>
+      <c r="D49">
+        <v>10</v>
       </c>
       <c r="E49" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="H49" s="14" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C50" t="s">
+        <v>282</v>
+      </c>
       <c r="D50" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="E50" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>294</v>
+        <v>167</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C51" t="s">
+        <v>290</v>
+      </c>
       <c r="D51" t="s">
         <v>289</v>
       </c>
       <c r="E51" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F51" s="14" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H51" s="14" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>15</v>
@@ -4944,230 +5122,308 @@
         <v>292</v>
       </c>
       <c r="E52" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F52" s="14" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>135</v>
+        <v>276</v>
       </c>
       <c r="H52" s="14" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C53" t="s">
-        <v>303</v>
-      </c>
       <c r="D53" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="E53" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F53" s="14" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>249</v>
+        <v>277</v>
       </c>
       <c r="H53" s="14" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D54" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="E54" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="F54" s="14" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>277</v>
+        <v>135</v>
       </c>
       <c r="H54" s="14" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="I54" s="14" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C55" t="s">
+        <v>303</v>
+      </c>
       <c r="D55" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="E55" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="F55" s="14" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>278</v>
+        <v>249</v>
       </c>
       <c r="H55" s="14" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="I55" s="14" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D56" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="E56" t="s">
-        <v>283</v>
+        <v>224</v>
       </c>
       <c r="F56" s="14" t="s">
-        <v>385</v>
+        <v>341</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>284</v>
-      </c>
-      <c r="H56" t="s">
-        <v>286</v>
-      </c>
-      <c r="I56" t="s">
-        <v>285</v>
+        <v>277</v>
+      </c>
+      <c r="H56" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="I56" s="14" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="D57" t="s">
+        <v>312</v>
+      </c>
       <c r="E57" t="s">
-        <v>365</v>
+        <v>225</v>
       </c>
       <c r="F57" s="14" t="s">
-        <v>366</v>
-      </c>
-      <c r="G57" s="10"/>
+        <v>342</v>
+      </c>
+      <c r="G57" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="H57" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="I57" s="14" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
+        <v>284</v>
+      </c>
+      <c r="E58" t="s">
+        <v>283</v>
+      </c>
+      <c r="F58" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="H58" t="s">
+        <v>286</v>
+      </c>
+      <c r="I58" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>52</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" t="s">
+        <v>361</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="G59" s="10"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>53</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C60" t="s">
         <v>258</v>
       </c>
-      <c r="E58" t="s">
-        <v>377</v>
-      </c>
-      <c r="F58" s="14" t="s">
-        <v>381</v>
-      </c>
-      <c r="G58" t="s">
+      <c r="E60" t="s">
+        <v>372</v>
+      </c>
+      <c r="F60" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="G60" t="s">
         <v>169</v>
       </c>
-      <c r="H58" t="s">
-        <v>379</v>
-      </c>
-      <c r="I58" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="65" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E65" t="s">
+      <c r="H60" t="s">
+        <v>374</v>
+      </c>
+      <c r="I60" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>54</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" t="s">
+        <v>123</v>
+      </c>
+      <c r="E61" t="s">
+        <v>486</v>
+      </c>
+      <c r="F61" s="14" t="s">
+        <v>490</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>487</v>
+      </c>
+      <c r="H61" t="s">
+        <v>488</v>
+      </c>
+      <c r="I61" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="68" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E66" t="s">
+    <row r="69" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="67" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D67" s="11" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="68" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D68" s="11" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="69" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D69" s="11" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="70" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D70" s="11" t="s">
-        <v>373</v>
+        <v>263</v>
       </c>
     </row>
     <row r="71" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D71" s="11" t="s">
-        <v>375</v>
+        <v>260</v>
       </c>
     </row>
     <row r="72" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D72" t="s">
+      <c r="D72" s="11" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="73" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D73" s="11" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="74" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D74" s="11" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="75" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
         <v>261</v>
-      </c>
-    </row>
-    <row r="73" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D73" t="s">
-        <v>262</v>
-      </c>
-      <c r="F73" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="74" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D74" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="75" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="E75" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="76" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
-        <v>319</v>
+        <v>262</v>
+      </c>
+      <c r="F76" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="77" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D77" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="78" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="79" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D79" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -5175,7 +5431,7 @@
     <sortCondition descending="1" ref="O5"/>
   </sortState>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B58">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B61">
       <formula1>$K$5:$K$10</formula1>
     </dataValidation>
   </dataValidations>
@@ -5189,10 +5445,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P44"/>
+  <dimension ref="A1:W54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" activeCellId="2" sqref="A12 A20 A27"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5200,261 +5456,562 @@
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="B2" t="s">
+        <v>404</v>
+      </c>
+      <c r="C2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B3" t="s">
+        <v>407</v>
+      </c>
+      <c r="C3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" t="s">
+        <v>501</v>
+      </c>
+      <c r="J11" t="s">
+        <v>491</v>
+      </c>
+      <c r="L11" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>505</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="J12" t="s">
+        <v>500</v>
+      </c>
+      <c r="L12" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>161</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>503</v>
+      </c>
+      <c r="J13" t="s">
+        <v>492</v>
+      </c>
+      <c r="L13" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>506</v>
+      </c>
+      <c r="D14" t="s">
         <v>410</v>
       </c>
-      <c r="C2" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>412</v>
-      </c>
-      <c r="B3" t="s">
-        <v>413</v>
-      </c>
-      <c r="C3" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>419</v>
-      </c>
-      <c r="F12" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>416</v>
-      </c>
-      <c r="F13" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>81</v>
-      </c>
-      <c r="F15" t="s">
-        <v>432</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>437</v>
-      </c>
-      <c r="H15" t="s">
-        <v>433</v>
-      </c>
-      <c r="I15" s="23" t="s">
-        <v>437</v>
-      </c>
+      <c r="G14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>504</v>
+      </c>
+      <c r="J14" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>507</v>
+      </c>
+      <c r="D15" t="s">
+        <v>246</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="3"/>
       <c r="J15" t="s">
-        <v>58</v>
-      </c>
-      <c r="K15" s="23" t="s">
-        <v>437</v>
-      </c>
-      <c r="L15" t="s">
-        <v>434</v>
-      </c>
-      <c r="M15" s="23" t="s">
-        <v>437</v>
-      </c>
-      <c r="N15" t="s">
-        <v>435</v>
-      </c>
-      <c r="O15" s="23" t="s">
-        <v>437</v>
-      </c>
-      <c r="P15" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+        <v>493</v>
+      </c>
+      <c r="M15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="S15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="W15" s="23"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>523</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>418</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>522</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>515</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J17" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>529</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>524</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" t="s">
+        <v>500</v>
+      </c>
+      <c r="L18" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>530</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J19" t="s">
+        <v>495</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>531</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>525</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" t="s">
+        <v>500</v>
+      </c>
+      <c r="L20" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>533</v>
+      </c>
+      <c r="C21" t="s">
+        <v>522</v>
+      </c>
+      <c r="D21" s="19" t="s">
         <v>417</v>
       </c>
-      <c r="F16" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="F21" t="s">
+        <v>532</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" t="s">
+        <v>496</v>
+      </c>
+      <c r="L21" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L22" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="19" t="s">
+      <c r="M23" s="14"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G26" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D27" s="5"/>
+      <c r="G27" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D28" s="19"/>
+      <c r="G28" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L29" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L30" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L31" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L32" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L33" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L34" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L35" s="17" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="G36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L36" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>425</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L37" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>427</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L38" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="G39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L39" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+      <c r="G40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L40" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="19" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="19" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L41" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="G42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L42" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="G43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L43" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>175</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>81</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="19" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="19" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="19" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="19" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="19" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="19" t="s">
+        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -5467,7 +6024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
@@ -5475,7 +6032,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5484,7 +6041,7 @@
         <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>445</v>
+        <v>430</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -5493,15 +6050,15 @@
         <v>42.5</v>
       </c>
       <c r="B3" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
       <c r="C3" t="s">
-        <v>475</v>
+        <v>459</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>446</v>
+        <v>431</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5509,7 +6066,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>448</v>
+        <v>433</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -5517,7 +6074,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>447</v>
+        <v>432</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5526,7 +6083,7 @@
         <v>84</v>
       </c>
       <c r="B8" t="s">
-        <v>450</v>
+        <v>435</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -5535,7 +6092,7 @@
         <v>240</v>
       </c>
       <c r="B10" t="s">
-        <v>449</v>
+        <v>434</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -5544,7 +6101,7 @@
         <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -5553,38 +6110,38 @@
         <v>276</v>
       </c>
       <c r="B12" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>460</v>
+        <v>445</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>461</v>
+        <v>446</v>
       </c>
       <c r="D19" t="s">
         <v>71</v>
@@ -5601,7 +6158,7 @@
         <v>5</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>457</v>
+        <v>442</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -5615,7 +6172,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -5798,7 +6355,7 @@
         <v>2</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -5890,7 +6447,7 @@
         <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>465</v>
+        <v>450</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -5898,17 +6455,17 @@
         <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>466</v>
+        <v>451</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>462</v>
+        <v>447</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>463</v>
+        <v>448</v>
       </c>
       <c r="B47">
         <f>SUM(C20:C21)</f>
@@ -5917,7 +6474,7 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="B48">
         <f>SUM(C22:C26)</f>
@@ -5926,7 +6483,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="B49">
         <f>SUM(C27:C33)</f>
@@ -5935,7 +6492,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="B50">
         <f>SUM(C34:C40)</f>
@@ -5944,12 +6501,12 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
-        <v>467</v>
+        <v>452</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>464</v>
+        <v>449</v>
       </c>
       <c r="D53">
         <f>SUM(B47:B49,A43,A41)</f>
@@ -5960,12 +6517,12 @@
         <v>20.458333333333332</v>
       </c>
       <c r="G53" t="s">
-        <v>477</v>
+        <v>461</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>468</v>
+        <v>453</v>
       </c>
       <c r="D54">
         <f>D53*1.5</f>
@@ -5976,12 +6533,12 @@
         <v>30.6875</v>
       </c>
       <c r="G54" t="s">
-        <v>477</v>
+        <v>461</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>476</v>
+        <v>460</v>
       </c>
       <c r="C56">
         <f>SUM(B47:B50,A43,A41)</f>
@@ -5992,12 +6549,12 @@
         <v>25.875</v>
       </c>
       <c r="F56" t="s">
-        <v>477</v>
+        <v>461</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>468</v>
+        <v>453</v>
       </c>
       <c r="C57">
         <f>C56*1.5</f>
@@ -6008,27 +6565,27 @@
         <v>38.8125</v>
       </c>
       <c r="F57" t="s">
-        <v>477</v>
+        <v>461</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>478</v>
+        <v>462</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>479</v>
+        <v>463</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>480</v>
+        <v>464</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>481</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>